<commit_message>
Updating Excel with new policy assignment
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18bd644199e08f73/Documents/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18bd644199e08f73/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F98EF084-0BE2-41E3-899E-AA8B115A5640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09BFE7B1-B927-4B22-9711-47CF30419E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="176">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -234,18 +234,6 @@
     <t>Deny the creation of public IP (azadvertizer.net)</t>
   </si>
   <si>
-    <t>RDP access from the Internet should be blocked</t>
-  </si>
-  <si>
-    <t>This policy denies any network security rule that allows RDP access from Internet.</t>
-  </si>
-  <si>
-    <t>DENY-RDPFromInternetPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>RDP access from the Internet should be blocked (azadvertizer.net)</t>
-  </si>
-  <si>
     <t>Subnets should have a Network Security Group</t>
   </si>
   <si>
@@ -288,9 +276,6 @@
     <t>Deny or Deploy and append TLS requirements and SSL enforcement on resources without Encryption in transit (azadvertizer.net)</t>
   </si>
   <si>
-    <t>This policy denies any network security rule that allows RDP access from Internet</t>
-  </si>
-  <si>
     <t>Network interfaces should disable IP forwarding</t>
   </si>
   <si>
@@ -429,51 +414,6 @@
     <t>Configure Azure PaaS services to use private DNS zones (azadvertizer.net)</t>
   </si>
   <si>
-    <t>Prevent usage of Databricks with public IP</t>
-  </si>
-  <si>
-    <t>Deny public IPs for Databricks cluster</t>
-  </si>
-  <si>
-    <t>Denies the deployment of workspaces that do not use the noPublicIp feature to host Databricks clusters without public IPs.</t>
-  </si>
-  <si>
-    <t>DENY-DatabricksPipPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>Deny public IPs for Databricks cluster (azadvertizer.net)</t>
-  </si>
-  <si>
-    <t>Enforces the use of Premium Databricks workspaces</t>
-  </si>
-  <si>
-    <t>Deny non-premium Databricks sku</t>
-  </si>
-  <si>
-    <t>Enforces the use of Premium Databricks workspaces to make sure appropriate security features are available including Databricks Access Controls, Credential Passthrough and SCIM provisioning for AAD.</t>
-  </si>
-  <si>
-    <t>DENY-DatabricksSkuPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>Deny non-premium Databricks sku (azadvertizer.net)</t>
-  </si>
-  <si>
-    <t>Enforces the use of vnet injection for Databricks</t>
-  </si>
-  <si>
-    <t>Deny Databricks workspaces without Vnet injection</t>
-  </si>
-  <si>
-    <t>Enforces the use of vnet injection for Databricks workspaces.</t>
-  </si>
-  <si>
-    <t>DENY-DatabricksVnetPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>Deny Databricks workspaces without Vnet injection (azadvertizer.net)</t>
-  </si>
-  <si>
     <t>Landing Zones/Online</t>
   </si>
   <si>
@@ -619,13 +559,22 @@
   </si>
   <si>
     <t>AUDIT-UnusedResourcesPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Management port access from the Internet should be blocked</t>
+  </si>
+  <si>
+    <t>DENY-MgmtPortsFromInternetPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>This policy denies any network security rule that allows management port access from the Internet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,23 +594,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -697,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -710,12 +642,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -999,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1198,10 +1124,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1210,16 +1136,16 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="58" x14ac:dyDescent="0.35">
@@ -1227,10 +1153,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1239,16 +1165,16 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1285,10 +1211,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>40</v>
@@ -1297,16 +1223,16 @@
         <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1314,10 +1240,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -1326,16 +1252,16 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1343,10 +1269,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>40</v>
@@ -1355,16 +1281,16 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
@@ -1372,10 +1298,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -1384,16 +1310,16 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1514,10 +1440,10 @@
         <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
@@ -1526,16 +1452,16 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>67</v>
+        <v>174</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1543,10 +1469,10 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -1555,16 +1481,16 @@
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="58" x14ac:dyDescent="0.35">
@@ -1572,10 +1498,10 @@
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>40</v>
@@ -1584,27 +1510,27 @@
         <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
@@ -1613,27 +1539,27 @@
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>40</v>
@@ -1642,27 +1568,27 @@
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>67</v>
+        <v>174</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1671,27 +1597,27 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
@@ -1700,27 +1626,27 @@
         <v>24</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -1729,27 +1655,27 @@
         <v>24</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
@@ -1758,27 +1684,27 @@
         <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>40</v>
@@ -1787,27 +1713,27 @@
         <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>40</v>
@@ -1816,27 +1742,27 @@
         <v>24</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
@@ -1845,21 +1771,21 @@
         <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>47</v>
@@ -1874,7 +1800,7 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>49</v>
@@ -1888,13 +1814,13 @@
     </row>
     <row r="31" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -1903,27 +1829,27 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -1932,27 +1858,27 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -1961,27 +1887,27 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
@@ -1990,27 +1916,27 @@
         <v>12</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2019,27 +1945,27 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
@@ -2048,27 +1974,27 @@
         <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -2077,277 +2003,190 @@
         <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D38" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" s="5" t="s">
+      <c r="F42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="F43" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2362,33 +2201,28 @@
     <hyperlink ref="I15" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
     <hyperlink ref="I16" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
     <hyperlink ref="I17" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I18" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{BAA25D6C-2600-4F8F-BA6A-C0D783184DB7}"/>
-    <hyperlink ref="I19" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I20" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I21" r:id="rId13" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I22" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{528B535E-06D1-4955-81A6-BE451E472AD8}"/>
-    <hyperlink ref="I23" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I24" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I25" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I26" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I27" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I28" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I29" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
-    <hyperlink ref="I30" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I31" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I32" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I33" r:id="rId25" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I36" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I37" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I38" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-NoPublicIp.html" xr:uid="{FFCF2031-D6A6-4381-9237-8632560F40D5}"/>
-    <hyperlink ref="I39" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-Sku.html" xr:uid="{18CEB7C5-C683-47A8-B99C-69984914347F}"/>
-    <hyperlink ref="I40" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-VirtualNetwork.html" xr:uid="{9489E458-C2DA-415E-9F33-CD09149C9B93}"/>
-    <hyperlink ref="I7" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I8" r:id="rId32" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I41" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I19" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I20" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I21" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I23" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I24" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I25" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I26" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I27" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I28" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I29" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
+    <hyperlink ref="I30" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I31" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I32" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I33" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I36" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I37" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I7" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I8" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I38" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Policy Excel Update (#1249)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18bd644199e08f73/Documents/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18bd644199e08f73/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F98EF084-0BE2-41E3-899E-AA8B115A5640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09BFE7B1-B927-4B22-9711-47CF30419E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="176">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -234,18 +234,6 @@
     <t>Deny the creation of public IP (azadvertizer.net)</t>
   </si>
   <si>
-    <t>RDP access from the Internet should be blocked</t>
-  </si>
-  <si>
-    <t>This policy denies any network security rule that allows RDP access from Internet.</t>
-  </si>
-  <si>
-    <t>DENY-RDPFromInternetPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>RDP access from the Internet should be blocked (azadvertizer.net)</t>
-  </si>
-  <si>
     <t>Subnets should have a Network Security Group</t>
   </si>
   <si>
@@ -288,9 +276,6 @@
     <t>Deny or Deploy and append TLS requirements and SSL enforcement on resources without Encryption in transit (azadvertizer.net)</t>
   </si>
   <si>
-    <t>This policy denies any network security rule that allows RDP access from Internet</t>
-  </si>
-  <si>
     <t>Network interfaces should disable IP forwarding</t>
   </si>
   <si>
@@ -429,51 +414,6 @@
     <t>Configure Azure PaaS services to use private DNS zones (azadvertizer.net)</t>
   </si>
   <si>
-    <t>Prevent usage of Databricks with public IP</t>
-  </si>
-  <si>
-    <t>Deny public IPs for Databricks cluster</t>
-  </si>
-  <si>
-    <t>Denies the deployment of workspaces that do not use the noPublicIp feature to host Databricks clusters without public IPs.</t>
-  </si>
-  <si>
-    <t>DENY-DatabricksPipPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>Deny public IPs for Databricks cluster (azadvertizer.net)</t>
-  </si>
-  <si>
-    <t>Enforces the use of Premium Databricks workspaces</t>
-  </si>
-  <si>
-    <t>Deny non-premium Databricks sku</t>
-  </si>
-  <si>
-    <t>Enforces the use of Premium Databricks workspaces to make sure appropriate security features are available including Databricks Access Controls, Credential Passthrough and SCIM provisioning for AAD.</t>
-  </si>
-  <si>
-    <t>DENY-DatabricksSkuPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>Deny non-premium Databricks sku (azadvertizer.net)</t>
-  </si>
-  <si>
-    <t>Enforces the use of vnet injection for Databricks</t>
-  </si>
-  <si>
-    <t>Deny Databricks workspaces without Vnet injection</t>
-  </si>
-  <si>
-    <t>Enforces the use of vnet injection for Databricks workspaces.</t>
-  </si>
-  <si>
-    <t>DENY-DatabricksVnetPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>Deny Databricks workspaces without Vnet injection (azadvertizer.net)</t>
-  </si>
-  <si>
     <t>Landing Zones/Online</t>
   </si>
   <si>
@@ -619,13 +559,22 @@
   </si>
   <si>
     <t>AUDIT-UnusedResourcesPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Management port access from the Internet should be blocked</t>
+  </si>
+  <si>
+    <t>DENY-MgmtPortsFromInternetPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>This policy denies any network security rule that allows management port access from the Internet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,23 +594,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Corbel"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -697,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -710,12 +642,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -999,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1198,10 +1124,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1210,16 +1136,16 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="58" x14ac:dyDescent="0.35">
@@ -1227,10 +1153,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1239,16 +1165,16 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1285,10 +1211,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>40</v>
@@ -1297,16 +1223,16 @@
         <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1314,10 +1240,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -1326,16 +1252,16 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1343,10 +1269,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>40</v>
@@ -1355,16 +1281,16 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
@@ -1372,10 +1298,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
@@ -1384,16 +1310,16 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1514,10 +1440,10 @@
         <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
@@ -1526,16 +1452,16 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>67</v>
+        <v>174</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1543,10 +1469,10 @@
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -1555,16 +1481,16 @@
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="58" x14ac:dyDescent="0.35">
@@ -1572,10 +1498,10 @@
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>40</v>
@@ -1584,27 +1510,27 @@
         <v>24</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
@@ -1613,27 +1539,27 @@
         <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>40</v>
@@ -1642,27 +1568,27 @@
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>67</v>
+        <v>174</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1671,27 +1597,27 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
@@ -1700,27 +1626,27 @@
         <v>24</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -1729,27 +1655,27 @@
         <v>24</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
@@ -1758,27 +1684,27 @@
         <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>40</v>
@@ -1787,27 +1713,27 @@
         <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>40</v>
@@ -1816,27 +1742,27 @@
         <v>24</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
@@ -1845,21 +1771,21 @@
         <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>47</v>
@@ -1874,7 +1800,7 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>49</v>
@@ -1888,13 +1814,13 @@
     </row>
     <row r="31" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -1903,27 +1829,27 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -1932,27 +1858,27 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -1961,27 +1887,27 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>11</v>
@@ -1990,27 +1916,27 @@
         <v>12</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2019,27 +1945,27 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>11</v>
@@ -2048,27 +1974,27 @@
         <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -2077,277 +2003,190 @@
         <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D38" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="5" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" s="5" t="s">
+      <c r="F42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="F43" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2362,33 +2201,28 @@
     <hyperlink ref="I15" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
     <hyperlink ref="I16" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
     <hyperlink ref="I17" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I18" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{BAA25D6C-2600-4F8F-BA6A-C0D783184DB7}"/>
-    <hyperlink ref="I19" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I20" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I21" r:id="rId13" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I22" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{528B535E-06D1-4955-81A6-BE451E472AD8}"/>
-    <hyperlink ref="I23" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I24" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I25" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I26" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I27" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I28" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I29" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
-    <hyperlink ref="I30" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I31" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I32" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I33" r:id="rId25" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I36" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I37" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I38" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-NoPublicIp.html" xr:uid="{FFCF2031-D6A6-4381-9237-8632560F40D5}"/>
-    <hyperlink ref="I39" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-Sku.html" xr:uid="{18CEB7C5-C683-47A8-B99C-69984914347F}"/>
-    <hyperlink ref="I40" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-VirtualNetwork.html" xr:uid="{9489E458-C2DA-415E-9F33-CD09149C9B93}"/>
-    <hyperlink ref="I7" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I8" r:id="rId32" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I41" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I19" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I20" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I21" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I23" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I24" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I25" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I26" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I27" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I28" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I29" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
+    <hyperlink ref="I30" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I31" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I32" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I33" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I36" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I37" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I7" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I8" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I38" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Main content update and new assignment
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26303"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18bd644199e08f73/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09BFE7B1-B927-4B22-9711-47CF30419E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B299002A-7D2D-4FF3-B097-0ABBD96E6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="181">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -568,6 +567,21 @@
   </si>
   <si>
     <t>This policy denies any network security rule that allows management port access from the Internet</t>
+  </si>
+  <si>
+    <t>Deploy-MDEndpoints</t>
+  </si>
+  <si>
+    <t>[Preview]: Deploy Microsoft Defender for Endpoint agent</t>
+  </si>
+  <si>
+    <t>Deploy Microsoft Defender for Endpoint agent on applicable images.</t>
+  </si>
+  <si>
+    <t>DINE-MDEndpointsPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>[Preview]: Deploy Microsoft Defender for Endpoint agent (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -925,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1003,73 +1017,73 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -1078,27 +1092,27 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -1107,27 +1121,27 @@
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1136,27 +1150,27 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>128</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1165,100 +1179,100 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>149</v>
+        <v>41</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>142</v>
@@ -1269,123 +1283,123 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>40</v>
@@ -1394,45 +1408,45 @@
         <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1440,10 +1454,10 @@
         <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
@@ -1452,27 +1466,27 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>175</v>
+        <v>60</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -1481,114 +1495,114 @@
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>175</v>
+        <v>74</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1597,56 +1611,56 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -1655,27 +1669,27 @@
         <v>24</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
@@ -1684,16 +1698,16 @@
         <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1701,10 +1715,10 @@
         <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>40</v>
@@ -1713,27 +1727,27 @@
         <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>40</v>
@@ -1742,27 +1756,27 @@
         <v>24</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
@@ -1771,27 +1785,27 @@
         <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -1800,27 +1814,27 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -1829,16 +1843,16 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
@@ -1846,10 +1860,10 @@
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -1858,27 +1872,27 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -1887,71 +1901,71 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>152</v>
+        <v>61</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>142</v>
@@ -1959,31 +1973,31 @@
     </row>
     <row r="36" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>119</v>
+        <v>162</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1991,10 +2005,10 @@
         <v>115</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -2003,45 +2017,45 @@
         <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>145</v>
+        <v>122</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2049,10 +2063,10 @@
         <v>115</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2061,16 +2075,16 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2078,10 +2092,10 @@
         <v>115</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2090,85 +2104,85 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2177,15 +2191,44 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2193,40 +2236,50 @@
   <autoFilter ref="A1:G1" xr:uid="{49B85179-65FD-4A38-99F4-B2A74C2DA415}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
-    <hyperlink ref="I3" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
-    <hyperlink ref="I4" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
-    <hyperlink ref="I5" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
-    <hyperlink ref="I6" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
-    <hyperlink ref="I9" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I15" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I16" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I17" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I19" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I20" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I21" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I23" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I24" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I25" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I26" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I27" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I28" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I29" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
-    <hyperlink ref="I30" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I31" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I32" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I33" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I36" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I37" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I7" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I8" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I38" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
+    <hyperlink ref="I5" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
+    <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
+    <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
+    <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
+    <hyperlink ref="I16" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I17" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I18" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I20" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I21" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I22" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I24" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I25" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I26" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I27" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I28" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I29" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I30" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
+    <hyperlink ref="I31" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I32" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I33" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I34" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I37" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I38" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I8" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I9" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I39" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I3" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2492,15 +2545,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2515,6 +2559,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2530,14 +2582,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Adding new initiative assignment for Microsoft Defender for Endpoints (#1255)
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26303"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18bd644199e08f73/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09BFE7B1-B927-4B22-9711-47CF30419E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B299002A-7D2D-4FF3-B097-0ABBD96E6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="181">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -568,6 +567,21 @@
   </si>
   <si>
     <t>This policy denies any network security rule that allows management port access from the Internet</t>
+  </si>
+  <si>
+    <t>Deploy-MDEndpoints</t>
+  </si>
+  <si>
+    <t>[Preview]: Deploy Microsoft Defender for Endpoint agent</t>
+  </si>
+  <si>
+    <t>Deploy Microsoft Defender for Endpoint agent on applicable images.</t>
+  </si>
+  <si>
+    <t>DINE-MDEndpointsPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>[Preview]: Deploy Microsoft Defender for Endpoint agent (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -925,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1003,73 +1017,73 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -1078,27 +1092,27 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -1107,27 +1121,27 @@
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1136,27 +1150,27 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>128</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1165,100 +1179,100 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>149</v>
+        <v>41</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>142</v>
@@ -1269,123 +1283,123 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>40</v>
@@ -1394,45 +1408,45 @@
         <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1440,10 +1454,10 @@
         <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
@@ -1452,27 +1466,27 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>175</v>
+        <v>60</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -1481,114 +1495,114 @@
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>175</v>
+        <v>74</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1597,56 +1611,56 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -1655,27 +1669,27 @@
         <v>24</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="116" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
@@ -1684,16 +1698,16 @@
         <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1701,10 +1715,10 @@
         <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>40</v>
@@ -1713,27 +1727,27 @@
         <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>40</v>
@@ -1742,27 +1756,27 @@
         <v>24</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
@@ -1771,27 +1785,27 @@
         <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -1800,27 +1814,27 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -1829,16 +1843,16 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
@@ -1846,10 +1860,10 @@
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -1858,27 +1872,27 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -1887,71 +1901,71 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>152</v>
+        <v>61</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>142</v>
@@ -1959,31 +1973,31 @@
     </row>
     <row r="36" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>116</v>
+        <v>160</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>119</v>
+        <v>162</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -1991,10 +2005,10 @@
         <v>115</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>11</v>
@@ -2003,45 +2017,45 @@
         <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>145</v>
+        <v>122</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2049,10 +2063,10 @@
         <v>115</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2061,16 +2075,16 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2078,10 +2092,10 @@
         <v>115</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2090,85 +2104,85 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>45</v>
+        <v>157</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2177,15 +2191,44 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2193,40 +2236,50 @@
   <autoFilter ref="A1:G1" xr:uid="{49B85179-65FD-4A38-99F4-B2A74C2DA415}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
-    <hyperlink ref="I3" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
-    <hyperlink ref="I4" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
-    <hyperlink ref="I5" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
-    <hyperlink ref="I6" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
-    <hyperlink ref="I9" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I15" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I16" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I17" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I19" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I20" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I21" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I23" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I24" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I25" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I26" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I27" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I28" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I29" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
-    <hyperlink ref="I30" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I31" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I32" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I33" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I36" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I37" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I7" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I8" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I38" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
+    <hyperlink ref="I5" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
+    <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
+    <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
+    <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
+    <hyperlink ref="I16" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I17" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I18" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I20" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I21" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I22" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I24" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I25" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I26" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I27" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I28" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I29" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I30" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
+    <hyperlink ref="I31" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I32" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I33" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I34" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I37" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I38" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I8" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I9" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I39" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I3" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2492,15 +2545,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2515,6 +2559,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2530,14 +2582,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updating spreadsheet to include previous snapshot.
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B299002A-7D2D-4FF3-B097-0ABBD96E6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E9A791-B134-4323-93EB-3F505B94F884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="201">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -582,6 +583,66 @@
   </si>
   <si>
     <t>[Preview]: Deploy Microsoft Defender for Endpoint agent (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>RDP access from the Internet should be blocked</t>
+  </si>
+  <si>
+    <t>This policy denies any network security rule that allows RDP access from Internet.</t>
+  </si>
+  <si>
+    <t>DENY-RDPFromInternetPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>RDP access from the Internet should be blocked (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>This policy denies any network security rule that allows RDP access from Internet</t>
+  </si>
+  <si>
+    <t>Prevent usage of Databricks with public IP</t>
+  </si>
+  <si>
+    <t>Deny public IPs for Databricks cluster</t>
+  </si>
+  <si>
+    <t>Denies the deployment of workspaces that do not use the noPublicIp feature to host Databricks clusters without public IPs.</t>
+  </si>
+  <si>
+    <t>DENY-DatabricksPipPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deny public IPs for Databricks cluster (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforces the use of Premium Databricks workspaces</t>
+  </si>
+  <si>
+    <t>Deny non-premium Databricks sku</t>
+  </si>
+  <si>
+    <t>Enforces the use of Premium Databricks workspaces to make sure appropriate security features are available including Databricks Access Controls, Credential Passthrough and SCIM provisioning for AAD.</t>
+  </si>
+  <si>
+    <t>DENY-DatabricksSkuPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deny non-premium Databricks sku (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforces the use of vnet injection for Databricks</t>
+  </si>
+  <si>
+    <t>Deny Databricks workspaces without Vnet injection</t>
+  </si>
+  <si>
+    <t>Enforces the use of vnet injection for Databricks workspaces.</t>
+  </si>
+  <si>
+    <t>DENY-DatabricksVnetPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deny Databricks workspaces without Vnet injection (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -941,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2270,16 +2331,1070 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
+  <dimension ref="E1:M35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.75" customWidth="1"/>
+    <col min="7" max="7" width="31.25" customWidth="1"/>
+    <col min="10" max="10" width="51.5" customWidth="1"/>
+    <col min="11" max="11" width="16.75" customWidth="1"/>
+    <col min="12" max="12" width="34.5" customWidth="1"/>
+    <col min="13" max="13" width="35.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="E14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="E15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="E23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="E27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="E31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M35" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{6C0005AB-05C9-402B-8F7C-1695E825D2E4}"/>
+    <hyperlink ref="M3" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{E5328607-E4BB-4BB2-B04E-54B1FBB75C53}"/>
+    <hyperlink ref="M4" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{53BA4E2D-923B-44E4-80D1-3856D3E074C9}"/>
+    <hyperlink ref="M5" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{A0E42AD3-1001-4FA5-A454-DCF10DC24CF7}"/>
+    <hyperlink ref="M6" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{5AE47694-C597-40E2-9139-D4741247B209}"/>
+    <hyperlink ref="M7" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{2072CB58-FDAB-4AC2-BC64-5EDF67779D7F}"/>
+    <hyperlink ref="M9" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{12875755-F619-4CDD-B3A3-13FC657D206D}"/>
+    <hyperlink ref="M10" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{4B092CD0-C0EE-418D-95B4-E7C466DCB0C8}"/>
+    <hyperlink ref="M11" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{E9BAB8D5-C7BB-40A8-86D4-AFBBAD22B0E9}"/>
+    <hyperlink ref="M12" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{63558627-2A2E-41D2-A2E6-34C431B58A50}"/>
+    <hyperlink ref="M13" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{F47A46D9-68A3-4280-81E1-EBD9B0AD324E}"/>
+    <hyperlink ref="M14" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{C838334B-24DE-42E8-BF5A-8F31EFAA4B51}"/>
+    <hyperlink ref="M15" r:id="rId13" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{416F0EB5-4575-4032-856B-987081319484}"/>
+    <hyperlink ref="M16" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{810ADB67-120C-4EFE-9AD9-4D78D244C88E}"/>
+    <hyperlink ref="M17" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{BF35414E-01D0-4C78-A293-16E4671AB965}"/>
+    <hyperlink ref="M18" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{8DA99F84-DFBB-470D-A710-22023ABC80A9}"/>
+    <hyperlink ref="M19" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{22EBC4E6-BC9A-46D1-905C-D65F03A5CBAA}"/>
+    <hyperlink ref="M20" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{C269B1C7-1811-4D31-97B6-93DB3082AB99}"/>
+    <hyperlink ref="M21" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{DEAC0A2F-710A-44B9-A365-9E1B0A54BBD8}"/>
+    <hyperlink ref="M22" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{46F04C90-D0BE-4C58-BC95-B3D01D4AE49E}"/>
+    <hyperlink ref="M23" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{B4EE2C2F-345D-41F2-BA49-4D0C22FC16A5}"/>
+    <hyperlink ref="M24" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{02157728-57AD-49BD-BA16-751CB31869D6}"/>
+    <hyperlink ref="M25" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{2EC8C9DF-2F20-46F4-ACE7-875DE89919D4}"/>
+    <hyperlink ref="M26" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{39021DAE-7C21-4E6A-BD70-9C4661A5728C}"/>
+    <hyperlink ref="M27" r:id="rId25" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{42815D8D-00BE-405A-891A-8210A08D1ABE}"/>
+    <hyperlink ref="M28" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{48433B09-EF03-4902-9ABB-400B4E79BD2E}"/>
+    <hyperlink ref="M29" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{C22D4C07-E485-4FEA-9D47-A667A32FDEAF}"/>
+    <hyperlink ref="M30" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-NoPublicIp.html" xr:uid="{D86E3D59-EC83-498B-A206-19508C58A74A}"/>
+    <hyperlink ref="M31" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-Sku.html" xr:uid="{6069D4AB-5A47-49DA-A64D-B87E4D3D9B6F}"/>
+    <hyperlink ref="M32" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-VirtualNetwork.html" xr:uid="{32A80F91-BC9B-47CA-99AA-E04DEBB0FC43}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2545,6 +3660,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2559,14 +3683,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2582,6 +3698,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updating What's New (#1258)
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B299002A-7D2D-4FF3-B097-0ABBD96E6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E9A791-B134-4323-93EB-3F505B94F884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="201">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -582,6 +583,66 @@
   </si>
   <si>
     <t>[Preview]: Deploy Microsoft Defender for Endpoint agent (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>RDP access from the Internet should be blocked</t>
+  </si>
+  <si>
+    <t>This policy denies any network security rule that allows RDP access from Internet.</t>
+  </si>
+  <si>
+    <t>DENY-RDPFromInternetPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>RDP access from the Internet should be blocked (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>This policy denies any network security rule that allows RDP access from Internet</t>
+  </si>
+  <si>
+    <t>Prevent usage of Databricks with public IP</t>
+  </si>
+  <si>
+    <t>Deny public IPs for Databricks cluster</t>
+  </si>
+  <si>
+    <t>Denies the deployment of workspaces that do not use the noPublicIp feature to host Databricks clusters without public IPs.</t>
+  </si>
+  <si>
+    <t>DENY-DatabricksPipPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deny public IPs for Databricks cluster (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforces the use of Premium Databricks workspaces</t>
+  </si>
+  <si>
+    <t>Deny non-premium Databricks sku</t>
+  </si>
+  <si>
+    <t>Enforces the use of Premium Databricks workspaces to make sure appropriate security features are available including Databricks Access Controls, Credential Passthrough and SCIM provisioning for AAD.</t>
+  </si>
+  <si>
+    <t>DENY-DatabricksSkuPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deny non-premium Databricks sku (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforces the use of vnet injection for Databricks</t>
+  </si>
+  <si>
+    <t>Deny Databricks workspaces without Vnet injection</t>
+  </si>
+  <si>
+    <t>Enforces the use of vnet injection for Databricks workspaces.</t>
+  </si>
+  <si>
+    <t>DENY-DatabricksVnetPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deny Databricks workspaces without Vnet injection (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -941,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2270,16 +2331,1070 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
+  <dimension ref="E1:M35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.75" customWidth="1"/>
+    <col min="7" max="7" width="31.25" customWidth="1"/>
+    <col min="10" max="10" width="51.5" customWidth="1"/>
+    <col min="11" max="11" width="16.75" customWidth="1"/>
+    <col min="12" max="12" width="34.5" customWidth="1"/>
+    <col min="13" max="13" width="35.4140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:13" ht="31" x14ac:dyDescent="0.35">
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="E14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="E15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="5:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="E23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="5:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="E26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="E27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="5:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="E31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="E34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M35" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{6C0005AB-05C9-402B-8F7C-1695E825D2E4}"/>
+    <hyperlink ref="M3" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{E5328607-E4BB-4BB2-B04E-54B1FBB75C53}"/>
+    <hyperlink ref="M4" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{53BA4E2D-923B-44E4-80D1-3856D3E074C9}"/>
+    <hyperlink ref="M5" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{A0E42AD3-1001-4FA5-A454-DCF10DC24CF7}"/>
+    <hyperlink ref="M6" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{5AE47694-C597-40E2-9139-D4741247B209}"/>
+    <hyperlink ref="M7" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{2072CB58-FDAB-4AC2-BC64-5EDF67779D7F}"/>
+    <hyperlink ref="M9" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{12875755-F619-4CDD-B3A3-13FC657D206D}"/>
+    <hyperlink ref="M10" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{4B092CD0-C0EE-418D-95B4-E7C466DCB0C8}"/>
+    <hyperlink ref="M11" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{E9BAB8D5-C7BB-40A8-86D4-AFBBAD22B0E9}"/>
+    <hyperlink ref="M12" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{63558627-2A2E-41D2-A2E6-34C431B58A50}"/>
+    <hyperlink ref="M13" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{F47A46D9-68A3-4280-81E1-EBD9B0AD324E}"/>
+    <hyperlink ref="M14" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{C838334B-24DE-42E8-BF5A-8F31EFAA4B51}"/>
+    <hyperlink ref="M15" r:id="rId13" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{416F0EB5-4575-4032-856B-987081319484}"/>
+    <hyperlink ref="M16" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{810ADB67-120C-4EFE-9AD9-4D78D244C88E}"/>
+    <hyperlink ref="M17" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{BF35414E-01D0-4C78-A293-16E4671AB965}"/>
+    <hyperlink ref="M18" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{8DA99F84-DFBB-470D-A710-22023ABC80A9}"/>
+    <hyperlink ref="M19" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{22EBC4E6-BC9A-46D1-905C-D65F03A5CBAA}"/>
+    <hyperlink ref="M20" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{C269B1C7-1811-4D31-97B6-93DB3082AB99}"/>
+    <hyperlink ref="M21" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{DEAC0A2F-710A-44B9-A365-9E1B0A54BBD8}"/>
+    <hyperlink ref="M22" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{46F04C90-D0BE-4C58-BC95-B3D01D4AE49E}"/>
+    <hyperlink ref="M23" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{B4EE2C2F-345D-41F2-BA49-4D0C22FC16A5}"/>
+    <hyperlink ref="M24" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{02157728-57AD-49BD-BA16-751CB31869D6}"/>
+    <hyperlink ref="M25" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{2EC8C9DF-2F20-46F4-ACE7-875DE89919D4}"/>
+    <hyperlink ref="M26" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{39021DAE-7C21-4E6A-BD70-9C4661A5728C}"/>
+    <hyperlink ref="M27" r:id="rId25" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{42815D8D-00BE-405A-891A-8210A08D1ABE}"/>
+    <hyperlink ref="M28" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{48433B09-EF03-4902-9ABB-400B4E79BD2E}"/>
+    <hyperlink ref="M29" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{C22D4C07-E485-4FEA-9D47-A667A32FDEAF}"/>
+    <hyperlink ref="M30" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-NoPublicIp.html" xr:uid="{D86E3D59-EC83-498B-A206-19508C58A74A}"/>
+    <hyperlink ref="M31" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-Sku.html" xr:uid="{6069D4AB-5A47-49DA-A64D-B87E4D3D9B6F}"/>
+    <hyperlink ref="M32" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-VirtualNetwork.html" xr:uid="{32A80F91-BC9B-47CA-99AA-E04DEBB0FC43}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2545,6 +3660,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2559,14 +3683,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2582,6 +3698,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Policy-Refresh - Portal Accelerator UI Update (#1273)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E9A791-B134-4323-93EB-3F505B94F884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F37118-2AFE-4688-955F-8445A5C3F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="57480" yWindow="3795" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -1002,7 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -2333,952 +2333,964 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
-  <dimension ref="E1:M35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
-    <col min="6" max="6" width="29.75" customWidth="1"/>
-    <col min="7" max="7" width="31.25" customWidth="1"/>
-    <col min="10" max="10" width="51.5" customWidth="1"/>
-    <col min="11" max="11" width="16.75" customWidth="1"/>
-    <col min="12" max="12" width="34.5" customWidth="1"/>
-    <col min="13" max="13" width="35.4140625" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.75" customWidth="1"/>
+    <col min="3" max="3" width="31.25" customWidth="1"/>
+    <col min="6" max="6" width="51.5" customWidth="1"/>
+    <col min="7" max="7" width="16.75" customWidth="1"/>
+    <col min="8" max="8" width="34.5" customWidth="1"/>
+    <col min="9" max="9" width="35.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="5:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="H14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="5:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="5:13" x14ac:dyDescent="0.35">
-      <c r="E8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="5:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="E11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="H29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="5:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="E12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="1" t="s">
+      <c r="H30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="F31" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="5:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="E13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="H31" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="F32" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="5:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="E14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="5:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="E15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="5:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="E16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="17" spans="5:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="E17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="5:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="E19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="5:13" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="E23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="5:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="E25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="5:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="E26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="5:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="E27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="5:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="E28" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="5:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="E29" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="5:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="E30" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="31" spans="5:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="E31" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="32" spans="5:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="E32" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="H32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L32" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="M32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E33" s="1" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>45</v>
@@ -3289,23 +3301,23 @@
       <c r="H33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="5:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E34" s="1" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>45</v>
@@ -3316,23 +3328,23 @@
       <c r="H34" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E35" s="1" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>45</v>
@@ -3343,52 +3355,40 @@
       <c r="H35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M35" s="1"/>
+      <c r="I35" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{6C0005AB-05C9-402B-8F7C-1695E825D2E4}"/>
-    <hyperlink ref="M3" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{E5328607-E4BB-4BB2-B04E-54B1FBB75C53}"/>
-    <hyperlink ref="M4" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{53BA4E2D-923B-44E4-80D1-3856D3E074C9}"/>
-    <hyperlink ref="M5" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{A0E42AD3-1001-4FA5-A454-DCF10DC24CF7}"/>
-    <hyperlink ref="M6" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{5AE47694-C597-40E2-9139-D4741247B209}"/>
-    <hyperlink ref="M7" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{2072CB58-FDAB-4AC2-BC64-5EDF67779D7F}"/>
-    <hyperlink ref="M9" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{12875755-F619-4CDD-B3A3-13FC657D206D}"/>
-    <hyperlink ref="M10" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{4B092CD0-C0EE-418D-95B4-E7C466DCB0C8}"/>
-    <hyperlink ref="M11" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{E9BAB8D5-C7BB-40A8-86D4-AFBBAD22B0E9}"/>
-    <hyperlink ref="M12" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{63558627-2A2E-41D2-A2E6-34C431B58A50}"/>
-    <hyperlink ref="M13" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{F47A46D9-68A3-4280-81E1-EBD9B0AD324E}"/>
-    <hyperlink ref="M14" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{C838334B-24DE-42E8-BF5A-8F31EFAA4B51}"/>
-    <hyperlink ref="M15" r:id="rId13" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{416F0EB5-4575-4032-856B-987081319484}"/>
-    <hyperlink ref="M16" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{810ADB67-120C-4EFE-9AD9-4D78D244C88E}"/>
-    <hyperlink ref="M17" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{BF35414E-01D0-4C78-A293-16E4671AB965}"/>
-    <hyperlink ref="M18" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{8DA99F84-DFBB-470D-A710-22023ABC80A9}"/>
-    <hyperlink ref="M19" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{22EBC4E6-BC9A-46D1-905C-D65F03A5CBAA}"/>
-    <hyperlink ref="M20" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{C269B1C7-1811-4D31-97B6-93DB3082AB99}"/>
-    <hyperlink ref="M21" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{DEAC0A2F-710A-44B9-A365-9E1B0A54BBD8}"/>
-    <hyperlink ref="M22" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{46F04C90-D0BE-4C58-BC95-B3D01D4AE49E}"/>
-    <hyperlink ref="M23" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{B4EE2C2F-345D-41F2-BA49-4D0C22FC16A5}"/>
-    <hyperlink ref="M24" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{02157728-57AD-49BD-BA16-751CB31869D6}"/>
-    <hyperlink ref="M25" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{2EC8C9DF-2F20-46F4-ACE7-875DE89919D4}"/>
-    <hyperlink ref="M26" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{39021DAE-7C21-4E6A-BD70-9C4661A5728C}"/>
-    <hyperlink ref="M27" r:id="rId25" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{42815D8D-00BE-405A-891A-8210A08D1ABE}"/>
-    <hyperlink ref="M28" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{48433B09-EF03-4902-9ABB-400B4E79BD2E}"/>
-    <hyperlink ref="M29" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{C22D4C07-E485-4FEA-9D47-A667A32FDEAF}"/>
-    <hyperlink ref="M30" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-NoPublicIp.html" xr:uid="{D86E3D59-EC83-498B-A206-19508C58A74A}"/>
-    <hyperlink ref="M31" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-Sku.html" xr:uid="{6069D4AB-5A47-49DA-A64D-B87E4D3D9B6F}"/>
-    <hyperlink ref="M32" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-VirtualNetwork.html" xr:uid="{32A80F91-BC9B-47CA-99AA-E04DEBB0FC43}"/>
+    <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{6C0005AB-05C9-402B-8F7C-1695E825D2E4}"/>
+    <hyperlink ref="I3" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{E5328607-E4BB-4BB2-B04E-54B1FBB75C53}"/>
+    <hyperlink ref="I4" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{53BA4E2D-923B-44E4-80D1-3856D3E074C9}"/>
+    <hyperlink ref="I5" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{A0E42AD3-1001-4FA5-A454-DCF10DC24CF7}"/>
+    <hyperlink ref="I6" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{5AE47694-C597-40E2-9139-D4741247B209}"/>
+    <hyperlink ref="I7" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{2072CB58-FDAB-4AC2-BC64-5EDF67779D7F}"/>
+    <hyperlink ref="I9" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{12875755-F619-4CDD-B3A3-13FC657D206D}"/>
+    <hyperlink ref="I10" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{4B092CD0-C0EE-418D-95B4-E7C466DCB0C8}"/>
+    <hyperlink ref="I11" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{E9BAB8D5-C7BB-40A8-86D4-AFBBAD22B0E9}"/>
+    <hyperlink ref="I12" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{63558627-2A2E-41D2-A2E6-34C431B58A50}"/>
+    <hyperlink ref="I13" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{F47A46D9-68A3-4280-81E1-EBD9B0AD324E}"/>
+    <hyperlink ref="I14" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{C838334B-24DE-42E8-BF5A-8F31EFAA4B51}"/>
+    <hyperlink ref="I15" r:id="rId13" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{416F0EB5-4575-4032-856B-987081319484}"/>
+    <hyperlink ref="I16" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-RDP-From-Internet.html" xr:uid="{810ADB67-120C-4EFE-9AD9-4D78D244C88E}"/>
+    <hyperlink ref="I17" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{BF35414E-01D0-4C78-A293-16E4671AB965}"/>
+    <hyperlink ref="I18" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{8DA99F84-DFBB-470D-A710-22023ABC80A9}"/>
+    <hyperlink ref="I19" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{22EBC4E6-BC9A-46D1-905C-D65F03A5CBAA}"/>
+    <hyperlink ref="I20" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{C269B1C7-1811-4D31-97B6-93DB3082AB99}"/>
+    <hyperlink ref="I21" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{DEAC0A2F-710A-44B9-A365-9E1B0A54BBD8}"/>
+    <hyperlink ref="I22" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{46F04C90-D0BE-4C58-BC95-B3D01D4AE49E}"/>
+    <hyperlink ref="I23" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{B4EE2C2F-345D-41F2-BA49-4D0C22FC16A5}"/>
+    <hyperlink ref="I24" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{02157728-57AD-49BD-BA16-751CB31869D6}"/>
+    <hyperlink ref="I25" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{2EC8C9DF-2F20-46F4-ACE7-875DE89919D4}"/>
+    <hyperlink ref="I26" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{39021DAE-7C21-4E6A-BD70-9C4661A5728C}"/>
+    <hyperlink ref="I27" r:id="rId25" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{42815D8D-00BE-405A-891A-8210A08D1ABE}"/>
+    <hyperlink ref="I28" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{48433B09-EF03-4902-9ABB-400B4E79BD2E}"/>
+    <hyperlink ref="I29" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{C22D4C07-E485-4FEA-9D47-A667A32FDEAF}"/>
+    <hyperlink ref="I30" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-NoPublicIp.html" xr:uid="{D86E3D59-EC83-498B-A206-19508C58A74A}"/>
+    <hyperlink ref="I31" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-Sku.html" xr:uid="{6069D4AB-5A47-49DA-A64D-B87E4D3D9B6F}"/>
+    <hyperlink ref="I32" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Databricks-VirtualNetwork.html" xr:uid="{32A80F91-BC9B-47CA-99AA-E04DEBB0FC43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3661,15 +3661,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
@@ -3680,6 +3671,15 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3703,14 +3703,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3722,6 +3714,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
ALZ Policies and Excel update
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F37118-2AFE-4688-955F-8445A5C3F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5E88B6-D3D8-4A8E-A93B-6A093ED44E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="3795" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="211">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -468,9 +468,6 @@
     <t>ENFORCE-ALZ-SandboxPolicyAssignment.json</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Deny network interfaces having a public IP associated</t>
   </si>
   <si>
@@ -504,9 +501,6 @@
     <t>ENFORCE-GuardrailsKeyVaultPolicyAssignment.json</t>
   </si>
   <si>
-    <t>Audit Private Link Private DNS Zone resources</t>
-  </si>
-  <si>
     <t>Audits the deployment of Private Link Private DNS Zone resources in the Corp landing zone.</t>
   </si>
   <si>
@@ -643,12 +637,51 @@
   </si>
   <si>
     <t>Deny Databricks workspaces without Vnet injection (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Enforce recommended guardrails for Azure Key Vault (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforce policies in the Decommissioned Landing Zone (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforce policies in the Sandbox Landing Zone (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Web Application Firewall (WAF) should be enabled for Application Gateway (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Audit the creation of Private Link Private DNS Zones</t>
+  </si>
+  <si>
+    <t>Audit the creation of Private Link Private DNS Zones (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Not allowed resource types (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Management port access from the Internet should be blocked (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Unused resources driving cost should be avoided (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Audit VMs that do not use managed disks (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforce Azure Compute Security Benchmark compliance auditing (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -704,7 +737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -717,6 +750,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1000,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1017,10 +1059,11 @@
     <col min="7" max="7" width="17.08203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="44.75" style="1" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.58203125" style="1"/>
+    <col min="10" max="10" width="12.4140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1048,8 +1091,11 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J1" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1077,16 +1123,19 @@
       <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J2" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1095,19 +1144,22 @@
         <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+      <c r="J3" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1135,8 +1187,11 @@
       <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="J4" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1164,8 +1219,11 @@
       <c r="I5" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J5" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1193,8 +1251,11 @@
       <c r="I6" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="J6" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1222,8 +1283,11 @@
       <c r="I7" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="J7" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1248,11 +1312,14 @@
       <c r="H8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J8" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1280,8 +1347,11 @@
       <c r="I9" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J9" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1309,16 +1379,19 @@
       <c r="I10" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J10" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>40</v>
@@ -1327,27 +1400,30 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J11" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -1356,27 +1432,30 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J12" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>40</v>
@@ -1385,27 +1464,30 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J13" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
@@ -1414,19 +1496,22 @@
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J14" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1451,8 +1536,14 @@
       <c r="H15" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="I15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1480,8 +1571,11 @@
       <c r="I16" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J16" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1509,8 +1603,11 @@
       <c r="I17" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J17" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -1538,16 +1635,19 @@
       <c r="I18" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J18" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -1556,19 +1656,22 @@
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J19" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1596,8 +1699,11 @@
       <c r="I20" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J20" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1625,8 +1731,11 @@
       <c r="I21" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J21" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -1654,16 +1763,19 @@
       <c r="I22" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J22" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1672,19 +1784,22 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J23" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -1712,8 +1827,11 @@
       <c r="I24" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J24" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -1741,8 +1859,11 @@
       <c r="I25" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="J25" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -1770,8 +1891,11 @@
       <c r="I26" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J26" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1799,8 +1923,11 @@
       <c r="I27" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J27" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -1828,8 +1955,11 @@
       <c r="I28" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J28" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
@@ -1857,8 +1987,11 @@
       <c r="I29" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="J29" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
@@ -1886,8 +2019,11 @@
       <c r="I30" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J30" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -1915,8 +2051,11 @@
       <c r="I31" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="J31" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -1944,8 +2083,11 @@
       <c r="I32" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="J32" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -1973,8 +2115,11 @@
       <c r="I33" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="J33" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -2002,16 +2147,19 @@
       <c r="I34" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J34" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
@@ -2020,27 +2168,30 @@
         <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I35" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J35" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2049,19 +2200,22 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J36" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>115</v>
       </c>
@@ -2089,8 +2243,11 @@
       <c r="I37" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J37" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
@@ -2118,17 +2275,20 @@
       <c r="I38" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J38" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
       </c>
@@ -2136,27 +2296,30 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+      <c r="J39" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2165,27 +2328,30 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J40" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>40</v>
@@ -2194,19 +2360,22 @@
         <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J41" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -2232,10 +2401,13 @@
         <v>45</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="J42" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>125</v>
       </c>
@@ -2260,11 +2432,14 @@
       <c r="H43" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="I43" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J43" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>126</v>
       </c>
@@ -2289,8 +2464,11 @@
       <c r="H44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>142</v>
+      <c r="I44" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J44" s="5">
+        <v>45018</v>
       </c>
     </row>
   </sheetData>
@@ -2325,9 +2503,21 @@
     <hyperlink ref="I9" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
     <hyperlink ref="I39" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
     <hyperlink ref="I3" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
+    <hyperlink ref="I35" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I43" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I44" r:id="rId32" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I36" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I40" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I41" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I23" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I19" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I14" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
+    <hyperlink ref="I13" r:id="rId39" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
+    <hyperlink ref="I12" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
+    <hyperlink ref="I11" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
 
@@ -2672,10 +2862,10 @@
         <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>40</v>
@@ -2684,16 +2874,16 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2788,10 +2978,10 @@
         <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>40</v>
@@ -2800,16 +2990,16 @@
         <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -3194,10 +3384,10 @@
         <v>115</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -3206,16 +3396,16 @@
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
@@ -3223,10 +3413,10 @@
         <v>115</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -3235,16 +3425,16 @@
         <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -3252,10 +3442,10 @@
         <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -3264,16 +3454,16 @@
         <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -3395,6 +3585,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3660,29 +3872,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3702,26 +3912,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Wiki deployments and Excel content update (#1302)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F37118-2AFE-4688-955F-8445A5C3F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5E88B6-D3D8-4A8E-A93B-6A093ED44E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="3795" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="211">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -468,9 +468,6 @@
     <t>ENFORCE-ALZ-SandboxPolicyAssignment.json</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Deny network interfaces having a public IP associated</t>
   </si>
   <si>
@@ -504,9 +501,6 @@
     <t>ENFORCE-GuardrailsKeyVaultPolicyAssignment.json</t>
   </si>
   <si>
-    <t>Audit Private Link Private DNS Zone resources</t>
-  </si>
-  <si>
     <t>Audits the deployment of Private Link Private DNS Zone resources in the Corp landing zone.</t>
   </si>
   <si>
@@ -643,12 +637,51 @@
   </si>
   <si>
     <t>Deny Databricks workspaces without Vnet injection (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Enforce recommended guardrails for Azure Key Vault (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforce policies in the Decommissioned Landing Zone (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforce policies in the Sandbox Landing Zone (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Web Application Firewall (WAF) should be enabled for Application Gateway (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Audit the creation of Private Link Private DNS Zones</t>
+  </si>
+  <si>
+    <t>Audit the creation of Private Link Private DNS Zones (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Not allowed resource types (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Management port access from the Internet should be blocked (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Unused resources driving cost should be avoided (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Audit VMs that do not use managed disks (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforce Azure Compute Security Benchmark compliance auditing (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -704,7 +737,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -717,6 +750,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1000,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1017,10 +1059,11 @@
     <col min="7" max="7" width="17.08203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="44.75" style="1" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.58203125" style="1"/>
+    <col min="10" max="10" width="12.4140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1048,8 +1091,11 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J1" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1077,16 +1123,19 @@
       <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J2" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -1095,19 +1144,22 @@
         <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+      <c r="J3" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1135,8 +1187,11 @@
       <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="J4" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1164,8 +1219,11 @@
       <c r="I5" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J5" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1193,8 +1251,11 @@
       <c r="I6" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="J6" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1222,8 +1283,11 @@
       <c r="I7" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="J7" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1248,11 +1312,14 @@
       <c r="H8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J8" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1280,8 +1347,11 @@
       <c r="I9" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J9" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1309,16 +1379,19 @@
       <c r="I10" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J10" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>40</v>
@@ -1327,27 +1400,30 @@
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J11" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -1356,27 +1432,30 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>166</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J12" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>40</v>
@@ -1385,27 +1464,30 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J13" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
@@ -1414,19 +1496,22 @@
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J14" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1451,8 +1536,14 @@
       <c r="H15" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="I15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1480,8 +1571,11 @@
       <c r="I16" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J16" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1509,8 +1603,11 @@
       <c r="I17" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J17" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -1538,16 +1635,19 @@
       <c r="I18" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J18" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -1556,19 +1656,22 @@
         <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J19" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1596,8 +1699,11 @@
       <c r="I20" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J20" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1625,8 +1731,11 @@
       <c r="I21" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J21" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -1654,16 +1763,19 @@
       <c r="I22" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J22" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1672,19 +1784,22 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J23" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -1712,8 +1827,11 @@
       <c r="I24" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J24" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -1741,8 +1859,11 @@
       <c r="I25" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="J25" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -1770,8 +1891,11 @@
       <c r="I26" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J26" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1799,8 +1923,11 @@
       <c r="I27" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J27" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -1828,8 +1955,11 @@
       <c r="I28" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="J28" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
@@ -1857,8 +1987,11 @@
       <c r="I29" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="J29" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
@@ -1886,8 +2019,11 @@
       <c r="I30" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J30" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -1915,8 +2051,11 @@
       <c r="I31" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="J31" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -1944,8 +2083,11 @@
       <c r="I32" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="J32" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -1973,8 +2115,11 @@
       <c r="I33" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="J33" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -2002,16 +2147,19 @@
       <c r="I34" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J34" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>11</v>
@@ -2020,27 +2168,30 @@
         <v>12</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I35" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J35" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2049,19 +2200,22 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J36" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>115</v>
       </c>
@@ -2089,8 +2243,11 @@
       <c r="I37" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J37" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
@@ -2118,17 +2275,20 @@
       <c r="I38" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="J38" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
       </c>
@@ -2136,27 +2296,30 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+      <c r="J39" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2165,27 +2328,30 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>154</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J40" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>40</v>
@@ -2194,19 +2360,22 @@
         <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J41" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -2232,10 +2401,13 @@
         <v>45</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+      <c r="J42" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>125</v>
       </c>
@@ -2260,11 +2432,14 @@
       <c r="H43" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="I43" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J43" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>126</v>
       </c>
@@ -2289,8 +2464,11 @@
       <c r="H44" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>142</v>
+      <c r="I44" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J44" s="5">
+        <v>45018</v>
       </c>
     </row>
   </sheetData>
@@ -2325,9 +2503,21 @@
     <hyperlink ref="I9" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
     <hyperlink ref="I39" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
     <hyperlink ref="I3" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
+    <hyperlink ref="I35" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I43" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I44" r:id="rId32" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I36" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I40" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I41" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I23" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I19" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I14" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
+    <hyperlink ref="I13" r:id="rId39" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
+    <hyperlink ref="I12" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
+    <hyperlink ref="I11" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
 
@@ -2672,10 +2862,10 @@
         <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>40</v>
@@ -2684,16 +2874,16 @@
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2788,10 +2978,10 @@
         <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>40</v>
@@ -2800,16 +2990,16 @@
         <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -3194,10 +3384,10 @@
         <v>115</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -3206,16 +3396,16 @@
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
@@ -3223,10 +3413,10 @@
         <v>115</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -3235,16 +3425,16 @@
         <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -3252,10 +3442,10 @@
         <v>115</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -3264,16 +3454,16 @@
         <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -3395,6 +3585,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3660,29 +3872,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3702,26 +3912,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Portal accelerator updates (#1342)
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5E88B6-D3D8-4A8E-A93B-6A093ED44E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037006B-0FD9-49D8-8343-5103B3A55946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="215">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -673,6 +673,18 @@
   </si>
   <si>
     <t>Enforce Azure Compute Security Benchmark compliance auditing (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy TDE on SQL servers</t>
+  </si>
+  <si>
+    <t>This policy ensures that Transparent Data Encryption is enabled on SQL Servers.</t>
+  </si>
+  <si>
+    <t>DINE-SQLThreatPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy SQL DB transparent data encryption (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -680,7 +692,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -751,7 +763,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1044,26 +1056,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.08203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.58203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.08203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.4140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.58203125" style="1"/>
+    <col min="10" max="10" width="12.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1107,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1159,7 +1171,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1191,7 +1203,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1223,7 +1235,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1255,7 +1267,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1299,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1319,7 +1331,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1351,7 +1363,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1383,7 +1395,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1415,7 +1427,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1447,7 +1459,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1491,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1511,7 +1523,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1543,7 +1555,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1575,7 +1587,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1607,7 +1619,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1671,7 +1683,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1703,7 +1715,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1735,7 +1747,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -1767,7 +1779,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
@@ -1799,7 +1811,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -1831,7 +1843,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -1863,7 +1875,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -1895,7 +1907,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1927,7 +1939,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -1959,7 +1971,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
@@ -1982,24 +1994,24 @@
         <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>99</v>
+        <v>213</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>100</v>
       </c>
       <c r="J29" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>68</v>
+        <v>211</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>211</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -2008,22 +2020,22 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>71</v>
+        <v>99</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J30" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2055,7 +2067,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -2087,7 +2099,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -2119,7 +2131,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -2151,7 +2163,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
@@ -2183,7 +2195,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
@@ -2215,7 +2227,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>115</v>
       </c>
@@ -2247,7 +2259,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
@@ -2279,7 +2291,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -2311,7 +2323,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>115</v>
       </c>
@@ -2343,7 +2355,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
@@ -2375,7 +2387,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -2407,7 +2419,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>125</v>
       </c>
@@ -2439,7 +2451,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>126</v>
       </c>
@@ -2492,29 +2504,29 @@
     <hyperlink ref="I27" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
     <hyperlink ref="I28" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
     <hyperlink ref="I29" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I30" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
-    <hyperlink ref="I31" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I32" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I33" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I34" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I37" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I38" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I8" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I9" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I39" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
-    <hyperlink ref="I3" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I35" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I43" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I44" r:id="rId32" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I36" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I40" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I41" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I23" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I19" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
-    <hyperlink ref="I14" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
-    <hyperlink ref="I13" r:id="rId39" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
-    <hyperlink ref="I12" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
-    <hyperlink ref="I11" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
+    <hyperlink ref="I31" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I32" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I33" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I34" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I37" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I38" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I39" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
+    <hyperlink ref="I35" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I43" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I44" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I36" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I40" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I41" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I23" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I19" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
+    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
+    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
+    <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
+    <hyperlink ref="I30" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId42"/>
@@ -2529,18 +2541,18 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.75" customWidth="1"/>
-    <col min="3" max="3" width="31.25" customWidth="1"/>
-    <col min="6" max="6" width="51.5" customWidth="1"/>
-    <col min="7" max="7" width="16.75" customWidth="1"/>
-    <col min="8" max="8" width="34.5" customWidth="1"/>
-    <col min="9" max="9" width="35.4140625" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" customWidth="1"/>
+    <col min="9" max="9" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2569,7 +2581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2598,7 +2610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2627,7 +2639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2656,7 +2668,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2685,7 +2697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2714,7 +2726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2743,7 +2755,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -2770,7 +2782,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2799,7 +2811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -2828,7 +2840,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2857,7 +2869,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2886,7 +2898,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -2915,7 +2927,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -2944,7 +2956,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -2973,7 +2985,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -3002,7 +3014,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -3031,7 +3043,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -3060,7 +3072,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -3089,7 +3101,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -3118,7 +3130,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -3176,7 +3188,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
@@ -3205,7 +3217,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -3234,7 +3246,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -3263,7 +3275,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -3292,7 +3304,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -3321,7 +3333,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -3350,7 +3362,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>115</v>
       </c>
@@ -3379,7 +3391,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -3408,7 +3420,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>115</v>
       </c>
@@ -3437,7 +3449,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -3466,7 +3478,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>124</v>
       </c>
@@ -3493,7 +3505,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>125</v>
       </c>
@@ -3520,7 +3532,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>126</v>
       </c>
@@ -3594,19 +3606,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3872,6 +3871,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
@@ -3881,18 +3893,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3912,6 +3912,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Policy Refresh Q4FY23 (#1354)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Azure\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5E88B6-D3D8-4A8E-A93B-6A093ED44E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037006B-0FD9-49D8-8343-5103B3A55946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5160" windowWidth="29040" windowHeight="16440" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="215">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -673,6 +673,18 @@
   </si>
   <si>
     <t>Enforce Azure Compute Security Benchmark compliance auditing (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy TDE on SQL servers</t>
+  </si>
+  <si>
+    <t>This policy ensures that Transparent Data Encryption is enabled on SQL Servers.</t>
+  </si>
+  <si>
+    <t>DINE-SQLThreatPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy SQL DB transparent data encryption (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -680,7 +692,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -751,7 +763,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -1044,26 +1056,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.08203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.08203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.58203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.08203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.75" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.4140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.58203125" style="1"/>
+    <col min="10" max="10" width="12.44140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1107,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1159,7 +1171,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1191,7 +1203,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1223,7 +1235,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1255,7 +1267,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1299,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1319,7 +1331,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1351,7 +1363,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1383,7 +1395,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1415,7 +1427,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1447,7 +1459,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1491,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1511,7 +1523,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1543,7 +1555,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1575,7 +1587,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1607,7 +1619,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1671,7 +1683,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -1703,7 +1715,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1735,7 +1747,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -1767,7 +1779,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
@@ -1799,7 +1811,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -1831,7 +1843,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -1863,7 +1875,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -1895,7 +1907,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1927,7 +1939,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -1959,7 +1971,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
@@ -1982,24 +1994,24 @@
         <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>99</v>
+        <v>213</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>100</v>
       </c>
       <c r="J29" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>68</v>
+        <v>211</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
+        <v>211</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -2008,22 +2020,22 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>71</v>
+        <v>99</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J30" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2055,7 +2067,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -2087,7 +2099,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -2119,7 +2131,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="87" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -2151,7 +2163,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
@@ -2183,7 +2195,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
@@ -2215,7 +2227,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>115</v>
       </c>
@@ -2247,7 +2259,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
@@ -2279,7 +2291,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -2311,7 +2323,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>115</v>
       </c>
@@ -2343,7 +2355,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
@@ -2375,7 +2387,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>124</v>
       </c>
@@ -2407,7 +2419,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>125</v>
       </c>
@@ -2439,7 +2451,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>126</v>
       </c>
@@ -2492,29 +2504,29 @@
     <hyperlink ref="I27" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
     <hyperlink ref="I28" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
     <hyperlink ref="I29" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I30" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{84A90F56-6249-44D0-88F8-FE46274A01C1}"/>
-    <hyperlink ref="I31" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I32" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I33" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I34" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I37" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I38" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I8" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I9" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I39" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
-    <hyperlink ref="I3" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I35" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I43" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I44" r:id="rId32" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I36" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I40" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I41" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I23" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I19" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
-    <hyperlink ref="I14" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
-    <hyperlink ref="I13" r:id="rId39" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
-    <hyperlink ref="I12" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
-    <hyperlink ref="I11" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
+    <hyperlink ref="I31" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I32" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I33" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I34" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I37" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I38" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I39" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
+    <hyperlink ref="I35" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I43" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I44" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I36" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I40" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I41" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I23" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I19" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
+    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
+    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
+    <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
+    <hyperlink ref="I30" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId42"/>
@@ -2529,18 +2541,18 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.75" customWidth="1"/>
-    <col min="3" max="3" width="31.25" customWidth="1"/>
-    <col min="6" max="6" width="51.5" customWidth="1"/>
-    <col min="7" max="7" width="16.75" customWidth="1"/>
-    <col min="8" max="8" width="34.5" customWidth="1"/>
-    <col min="9" max="9" width="35.4140625" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" customWidth="1"/>
+    <col min="9" max="9" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2569,7 +2581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2598,7 +2610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2627,7 +2639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2656,7 +2668,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2685,7 +2697,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2714,7 +2726,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2743,7 +2755,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -2770,7 +2782,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2799,7 +2811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -2828,7 +2840,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2857,7 +2869,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2886,7 +2898,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -2915,7 +2927,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -2944,7 +2956,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -2973,7 +2985,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -3002,7 +3014,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -3031,7 +3043,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -3060,7 +3072,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -3089,7 +3101,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -3118,7 +3130,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -3176,7 +3188,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
@@ -3205,7 +3217,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -3234,7 +3246,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -3263,7 +3275,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -3292,7 +3304,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -3321,7 +3333,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -3350,7 +3362,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>115</v>
       </c>
@@ -3379,7 +3391,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -3408,7 +3420,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>115</v>
       </c>
@@ -3437,7 +3449,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -3466,7 +3478,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>124</v>
       </c>
@@ -3493,7 +3505,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>125</v>
       </c>
@@ -3520,7 +3532,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>126</v>
       </c>
@@ -3594,19 +3606,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3872,6 +3871,19 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
@@ -3881,18 +3893,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3912,6 +3912,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Additional documentation updates (to the right branch this time)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037006B-0FD9-49D8-8343-5103B3A55946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE42599A-224F-4AEF-93BC-450C08022674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments" sheetId="3" r:id="rId1"/>
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1523,36 +1523,36 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>151</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>45</v>
+        <v>152</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J15" s="5">
-        <v>45018</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2527,9 +2527,10 @@
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
     <hyperlink ref="I30" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I15" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A26D2675-3D66-4156-A1D3-8DBCB7ADFAC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -3597,12 +3598,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3872,22 +3877,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3913,13 +3918,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add KV Guardrails Assignment to Platform Management group (#1383)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037006B-0FD9-49D8-8343-5103B3A55946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE42599A-224F-4AEF-93BC-450C08022674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments" sheetId="3" r:id="rId1"/>
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1523,36 +1523,36 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>151</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>45</v>
+        <v>152</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J15" s="5">
-        <v>45018</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2527,9 +2527,10 @@
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
     <hyperlink ref="I30" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I15" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A26D2675-3D66-4156-A1D3-8DBCB7ADFAC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -3597,12 +3598,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3872,22 +3877,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3913,13 +3918,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
The Policy Testing Framework - DENY (#1390)
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE42599A-224F-4AEF-93BC-450C08022674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9F957E-4BC5-4E5A-8957-1C5851F8F249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2527,7 +2527,7 @@
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
     <hyperlink ref="I30" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I15" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A26D2675-3D66-4156-A1D3-8DBCB7ADFAC7}"/>
+    <hyperlink ref="I15" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId43"/>

</xml_diff>

<commit_message>
Remediating RBAC Roles on Assignments (#1419)
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9F957E-4BC5-4E5A-8957-1C5851F8F249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDF600B-5C3C-4E8C-A483-BB52C1E92A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="217">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -685,6 +685,12 @@
   </si>
   <si>
     <t>Deploy SQL DB transparent data encryption (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Decommissioned</t>
+  </si>
+  <si>
+    <t>Sandbox</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2421,7 +2427,7 @@
     </row>
     <row r="43" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>135</v>
@@ -2453,7 +2459,7 @@
     </row>
     <row r="44" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>126</v>
+        <v>216</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>139</v>
@@ -3598,16 +3604,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3877,22 +3879,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3918,9 +3920,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Policy Excel updates (#1424)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDF600B-5C3C-4E8C-A483-BB52C1E92A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93951156-9953-48CE-B52B-26D498A183E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
@@ -1062,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,7 +1901,7 @@
         <v>83</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>85</v>
@@ -2125,7 +2125,7 @@
         <v>108</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>109</v>
@@ -3604,12 +3604,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3879,22 +3883,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3920,13 +3924,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Policy Refresh Q1 FY24 (#1426)
Co-authored-by: Jack Tracey <jack@jacktracey.co.uk>
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
Co-authored-by: JamJarchitect <53943045+JamJarchitect@users.noreply.github.com>
Co-authored-by: Panagiotis Korologos <60117125+pkorolo@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C037006B-0FD9-49D8-8343-5103B3A55946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93951156-9953-48CE-B52B-26D498A183E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="217">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -685,6 +685,12 @@
   </si>
   <si>
     <t>Deploy SQL DB transparent data encryption (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Decommissioned</t>
+  </si>
+  <si>
+    <t>Sandbox</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1523,36 +1529,36 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>151</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>45</v>
+        <v>152</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J15" s="5">
-        <v>45018</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -1895,7 +1901,7 @@
         <v>83</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>85</v>
@@ -2119,7 +2125,7 @@
         <v>108</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>109</v>
@@ -2421,7 +2427,7 @@
     </row>
     <row r="43" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>135</v>
@@ -2453,7 +2459,7 @@
     </row>
     <row r="44" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>126</v>
+        <v>216</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>139</v>
@@ -2527,9 +2533,10 @@
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
     <hyperlink ref="I30" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I15" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
@@ -3597,12 +3604,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3872,22 +3883,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3913,13 +3924,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add Amba policies to Excel
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rep\int\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93951156-9953-48CE-B52B-26D498A183E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB278D-3FBA-4E87-9755-74F94D38998E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$49</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="237">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -691,6 +691,66 @@
   </si>
   <si>
     <t>Sandbox</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Service Health</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA Service Health alerts to Azure services</t>
+  </si>
+  <si>
+    <t>DINE-ServiceHealthAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Service Health - Alerting-ServiceHealth (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Connectivity</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA alerts relevant to the ALZ Connectivity management group</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Management</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Identity</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA alerts relevant to the ALZ Management management group</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA alerts relevant to the ALZ Identity management group</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Landing Zone</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA alerts relevant to the ALZ LandingZone management group</t>
+  </si>
+  <si>
+    <t>DINE-ConnectivityAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-ManagementAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-IdentityAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-LandingZoneAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Connectivity - Alerting-Connectivity (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Management - Alerting-Management (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Identity - Alerting-Identity (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Landing Zone - Alerting-LandingZone (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -755,7 +815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -777,6 +837,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1060,28 +1124,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.53125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.796875" style="1" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.5546875" style="1"/>
+    <col min="10" max="10" width="12.46484375" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.53125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1109,11 +1173,11 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="9" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1209,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1177,7 +1241,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1209,7 +1273,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1305,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1273,7 +1337,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1369,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1337,7 +1401,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +1433,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1401,7 +1465,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1497,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1465,7 +1529,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1497,7 +1561,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1529,15 +1593,15 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -1546,62 +1610,62 @@
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="J15" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J16" s="5">
         <v>45124</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>40</v>
@@ -1610,190 +1674,190 @@
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J17" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>221</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>221</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>222</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>63</v>
+        <v>229</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="J18" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>171</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>171</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>173</v>
+        <v>55</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>207</v>
+        <v>56</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="J19" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>225</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>67</v>
+        <v>230</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J20" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="J21" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>77</v>
+        <v>172</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J22" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1802,190 +1866,190 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>173</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>207</v>
+        <v>66</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="J23" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="J24" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>224</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>78</v>
+        <v>224</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>79</v>
+        <v>226</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>81</v>
+        <v>231</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J25" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="J26" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>90</v>
+        <v>172</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J27" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="J28" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
@@ -1994,30 +2058,30 @@
         <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="J29" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>211</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>211</v>
+        <v>82</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -2026,30 +2090,30 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>212</v>
+        <v>83</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>214</v>
+        <v>85</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="J30" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -2058,30 +2122,30 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -2090,30 +2154,30 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2122,30 +2186,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>109</v>
+        <v>213</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J33" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2154,62 +2218,62 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J34" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>200</v>
+        <v>50</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="J35" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>103</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>158</v>
+        <v>103</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2218,126 +2282,126 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>203</v>
+        <v>105</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="J36" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J37" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2346,94 +2410,94 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J41" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="J41" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>45</v>
+        <v>118</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J42" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2442,55 +2506,215 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>201</v>
+        <v>122</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J43" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>216</v>
+        <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>202</v>
+        <v>146</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J44" s="5">
         <v>45018</v>
       </c>
     </row>
+    <row r="45" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J45" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J46" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J47" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J48" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J49" s="5">
+        <v>45018</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{49B85179-65FD-4A38-99F4-B2A74C2DA415}"/>
+  <autoFilter ref="A1:J49" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
     <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
@@ -2498,45 +2722,49 @@
     <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
     <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
     <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I16" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I17" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I18" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I20" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I21" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I22" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I24" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I25" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I26" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I27" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I28" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I29" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I31" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I32" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I33" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I34" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I37" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I38" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I17" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I19" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I21" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I23" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I24" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I26" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I28" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I29" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I30" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I31" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I32" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I33" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I35" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I36" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I37" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I38" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I42" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I43" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
     <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
     <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I39" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I44" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
     <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I35" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I43" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I44" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I36" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I40" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I41" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I23" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I19" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I39" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I40" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I45" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I46" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I27" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I22" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
     <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
     <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
-    <hyperlink ref="I30" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I15" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I34" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I16" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
+    <hyperlink ref="I18" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
+    <hyperlink ref="I20" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
+    <hyperlink ref="I25" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -2548,18 +2776,18 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" customWidth="1"/>
-    <col min="3" max="3" width="31.21875" customWidth="1"/>
-    <col min="6" max="6" width="51.44140625" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" customWidth="1"/>
-    <col min="9" max="9" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.796875" customWidth="1"/>
+    <col min="3" max="3" width="31.19921875" customWidth="1"/>
+    <col min="6" max="6" width="51.46484375" customWidth="1"/>
+    <col min="7" max="7" width="16.796875" customWidth="1"/>
+    <col min="8" max="8" width="34.46484375" customWidth="1"/>
+    <col min="9" max="9" width="35.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2617,7 +2845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2646,7 +2874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2675,7 +2903,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2704,7 +2932,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2733,7 +2961,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2762,7 +2990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -2789,7 +3017,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2818,7 +3046,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -2847,7 +3075,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2876,7 +3104,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2905,7 +3133,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -2934,7 +3162,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -2963,7 +3191,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -2992,7 +3220,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -3021,7 +3249,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -3050,7 +3278,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -3079,7 +3307,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -3108,7 +3336,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -3137,7 +3365,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -3166,7 +3394,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -3195,7 +3423,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
@@ -3224,7 +3452,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -3253,7 +3481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -3282,7 +3510,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -3311,7 +3539,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -3340,7 +3568,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -3369,7 +3597,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>115</v>
       </c>
@@ -3398,7 +3626,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -3427,7 +3655,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>115</v>
       </c>
@@ -3456,7 +3684,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -3485,7 +3713,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>124</v>
       </c>
@@ -3512,7 +3740,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>125</v>
       </c>
@@ -3539,7 +3767,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>126</v>
       </c>
@@ -3604,16 +3832,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3883,22 +4107,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3924,9 +4148,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Include AMBA policies in portal accelerator (#1414)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rep\int\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93951156-9953-48CE-B52B-26D498A183E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB278D-3FBA-4E87-9755-74F94D38998E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$49</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="237">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -691,6 +691,66 @@
   </si>
   <si>
     <t>Sandbox</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Service Health</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA Service Health alerts to Azure services</t>
+  </si>
+  <si>
+    <t>DINE-ServiceHealthAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Service Health - Alerting-ServiceHealth (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Connectivity</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA alerts relevant to the ALZ Connectivity management group</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Management</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Identity</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA alerts relevant to the ALZ Management management group</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA alerts relevant to the ALZ Identity management group</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Landing Zone</t>
+  </si>
+  <si>
+    <t>Initiative to deploy AMBA alerts relevant to the ALZ LandingZone management group</t>
+  </si>
+  <si>
+    <t>DINE-ConnectivityAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-ManagementAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-IdentityAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-LandingZoneAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Connectivity - Alerting-Connectivity (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Management - Alerting-Management (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Identity - Alerting-Identity (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deploy Azure Monitor Baseline Alerts for Landing Zone - Alerting-LandingZone (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -755,7 +815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -777,6 +837,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1060,28 +1124,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.53125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.796875" style="1" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.5546875" style="1"/>
+    <col min="10" max="10" width="12.46484375" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.53125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1109,11 +1173,11 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="9" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1209,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1177,7 +1241,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1209,7 +1273,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1305,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1273,7 +1337,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +1369,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1337,7 +1401,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +1433,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1401,7 +1465,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1497,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1465,7 +1529,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1497,7 +1561,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1529,15 +1593,15 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -1546,62 +1610,62 @@
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="J15" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J16" s="5">
         <v>45124</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>40</v>
@@ -1610,190 +1674,190 @@
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J17" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>221</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>221</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>222</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>63</v>
+        <v>229</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="J18" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>171</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>171</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>173</v>
+        <v>55</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>207</v>
+        <v>56</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="J19" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>225</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>67</v>
+        <v>230</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J20" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="J21" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>77</v>
+        <v>172</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J22" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1802,190 +1866,190 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>173</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>207</v>
+        <v>66</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="J23" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="J24" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>224</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>78</v>
+        <v>224</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>79</v>
+        <v>226</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>81</v>
+        <v>231</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J25" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="J26" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>90</v>
+        <v>172</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J27" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="J28" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
@@ -1994,30 +2058,30 @@
         <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>213</v>
+        <v>80</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="J29" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>211</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>211</v>
+        <v>82</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -2026,30 +2090,30 @@
         <v>24</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>212</v>
+        <v>83</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>214</v>
+        <v>85</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="J30" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -2058,30 +2122,30 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -2090,30 +2154,30 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2122,30 +2186,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>109</v>
+        <v>213</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J33" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2154,62 +2218,62 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>112</v>
+        <v>212</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>114</v>
+        <v>99</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J34" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>200</v>
+        <v>50</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="J35" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>103</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>158</v>
+        <v>103</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2218,126 +2282,126 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>159</v>
+        <v>104</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>203</v>
+        <v>105</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="J36" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J37" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2346,94 +2410,94 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J41" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="J41" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>45</v>
+        <v>118</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J42" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2442,55 +2506,215 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>201</v>
+        <v>122</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J43" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>216</v>
+        <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>202</v>
+        <v>146</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J44" s="5">
         <v>45018</v>
       </c>
     </row>
+    <row r="45" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J45" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J46" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J47" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J48" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J49" s="5">
+        <v>45018</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{49B85179-65FD-4A38-99F4-B2A74C2DA415}"/>
+  <autoFilter ref="A1:J49" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
     <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
@@ -2498,45 +2722,49 @@
     <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
     <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
     <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I16" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I17" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I18" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I20" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I21" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I22" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I24" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I25" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I26" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I27" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I28" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I29" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I31" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I32" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I33" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I34" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I37" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I38" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I17" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I19" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I21" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I23" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I24" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I26" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I28" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I29" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I30" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I31" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I32" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I33" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I35" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I36" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I37" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I38" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I42" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I43" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
     <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
     <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I39" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I44" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
     <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I35" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I43" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I44" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I36" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I40" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I41" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I23" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I19" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I39" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I40" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I45" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I46" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I27" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I22" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
     <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
     <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
-    <hyperlink ref="I30" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I15" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I34" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I16" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
+    <hyperlink ref="I18" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
+    <hyperlink ref="I20" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
+    <hyperlink ref="I25" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -2548,18 +2776,18 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.77734375" customWidth="1"/>
-    <col min="3" max="3" width="31.21875" customWidth="1"/>
-    <col min="6" max="6" width="51.44140625" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" customWidth="1"/>
-    <col min="9" max="9" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.796875" customWidth="1"/>
+    <col min="3" max="3" width="31.19921875" customWidth="1"/>
+    <col min="6" max="6" width="51.46484375" customWidth="1"/>
+    <col min="7" max="7" width="16.796875" customWidth="1"/>
+    <col min="8" max="8" width="34.46484375" customWidth="1"/>
+    <col min="9" max="9" width="35.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +2816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2617,7 +2845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2646,7 +2874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2675,7 +2903,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2704,7 +2932,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2733,7 +2961,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2762,7 +2990,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -2789,7 +3017,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -2818,7 +3046,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -2847,7 +3075,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -2876,7 +3104,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2905,7 +3133,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -2934,7 +3162,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -2963,7 +3191,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -2992,7 +3220,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -3021,7 +3249,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -3050,7 +3278,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -3079,7 +3307,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -3108,7 +3336,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -3137,7 +3365,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -3166,7 +3394,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -3195,7 +3423,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
@@ -3224,7 +3452,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -3253,7 +3481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -3282,7 +3510,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -3311,7 +3539,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -3340,7 +3568,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -3369,7 +3597,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>115</v>
       </c>
@@ -3398,7 +3626,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -3427,7 +3655,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>115</v>
       </c>
@@ -3456,7 +3684,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -3485,7 +3713,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>124</v>
       </c>
@@ -3512,7 +3740,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>125</v>
       </c>
@@ -3539,7 +3767,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>126</v>
       </c>
@@ -3604,16 +3832,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3883,22 +4107,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3924,9 +4148,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add document describing Policy Testing concept (#1480)
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rep\int\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB278D-3FBA-4E87-9755-74F94D38998E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E380B3-39F1-447E-B796-D38095CF90CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-38510" yWindow="-30" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
-    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
+    <sheet name="ALZ Policy Assignments 12CY23" sheetId="5" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId2"/>
+    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 12CY23'!$A$1:$J$49</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="237">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -1123,29 +1125,1675 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7B1182-4665-4109-8EF9-9158E84D9F8E}">
+  <dimension ref="A1:J49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J8" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J11" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J12" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J13" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J14" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="J15" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J16" s="5">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="J18" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="J20" s="5">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J22" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J23" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J24" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="J25" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J26" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J27" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J28" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J29" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J30" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J32" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J33" s="5">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="J34" s="5">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J35" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J36" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J37" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J38" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J39" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J40" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J41" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J42" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J43" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J44" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J45" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J46" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J47" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J48" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J49" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J49" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{F68C5E7F-0D92-4692-B9FD-FA4BADBB8FAD}"/>
+    <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{4922A37A-092D-4A2C-81A4-B92C26D8C8E9}"/>
+    <hyperlink ref="I5" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{F8BA97F3-303F-4C38-8898-E256DD9130C2}"/>
+    <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{367A85F5-96A9-40F4-925D-FDB06A2E3DDD}"/>
+    <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{7587EC6C-3EC1-4B0E-9CD2-9BA6EE18C958}"/>
+    <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{DBCC2C73-304C-4B93-8F29-C4F94B35CB1A}"/>
+    <hyperlink ref="I17" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{39FC4DB8-CB4D-48DD-ACA9-856296CD94DF}"/>
+    <hyperlink ref="I19" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{16316F4D-CE83-44A6-88A3-692A34400BFE}"/>
+    <hyperlink ref="I21" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{94FEED80-A7C9-47CF-B90F-98EA10E6FAE4}"/>
+    <hyperlink ref="I23" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{03B0DF73-0B97-475D-85F0-5C00EF91A545}"/>
+    <hyperlink ref="I24" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{B8810D5A-DC44-4DF4-A706-3855C0C45D96}"/>
+    <hyperlink ref="I26" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{3FE4B42C-F6A1-41EA-AC5E-89FB7E1D93FE}"/>
+    <hyperlink ref="I28" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{9C39FBDD-6917-41EF-9279-D36FFD85209E}"/>
+    <hyperlink ref="I29" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{29FBD2DC-19E8-4578-BFB0-1727BE9B485C}"/>
+    <hyperlink ref="I30" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{25AFED85-48D4-4D94-9CCD-02BB107963A7}"/>
+    <hyperlink ref="I31" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{653E5BFB-2C45-43C9-AD1D-B88AB88E9257}"/>
+    <hyperlink ref="I32" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5B17C2AD-56D7-412D-9670-FBEBD0BE0838}"/>
+    <hyperlink ref="I33" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{B5EDD756-7192-4902-BD7E-0922F5405BC4}"/>
+    <hyperlink ref="I35" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{4E7F0D4A-92D8-4A12-AE80-BD7D87CA95E1}"/>
+    <hyperlink ref="I36" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{0F818706-C153-4CBC-98B5-FC3FD12323E9}"/>
+    <hyperlink ref="I37" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{49E32576-5222-411C-9306-575C68BA48BA}"/>
+    <hyperlink ref="I38" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{D165A2DC-684A-41FF-BBA3-3D81B98CD413}"/>
+    <hyperlink ref="I42" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{67A44FEE-082D-4CB2-8E34-23D1DAD2B30B}"/>
+    <hyperlink ref="I43" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{09E7D7FC-DB0A-4BA1-AD89-7AAB980C3CB3}"/>
+    <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{D39F09F2-B2B5-4140-BC61-43F89B8D4C18}"/>
+    <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{456F843D-17A5-4985-BA3D-1F4BD3C6AABF}"/>
+    <hyperlink ref="I44" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{94C3CF6E-18EE-49FE-9D09-15DCFA40A1F1}"/>
+    <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{5898AEFA-DD35-4895-A8DE-88B1CF610C69}"/>
+    <hyperlink ref="I39" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D1D00F1F-3215-4A56-83EF-29A879D07E71}"/>
+    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{B973B264-05EE-4863-BFC9-474245901E65}"/>
+    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{A305219B-0027-478A-AFFE-2564BF13467E}"/>
+    <hyperlink ref="I40" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{511DE963-0BC7-4BDD-874D-BDB2F9A0F465}"/>
+    <hyperlink ref="I45" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDE193E1-1120-45C9-A636-97EC7A443022}"/>
+    <hyperlink ref="I46" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{E84AEDB7-FF67-4FD4-8232-B0DD829AEB2D}"/>
+    <hyperlink ref="I27" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{27C701D5-7B42-4357-AEDF-560CE040D9A7}"/>
+    <hyperlink ref="I22" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{37BF929F-CD7F-41BD-8673-EFD75351CCBF}"/>
+    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{4D026B69-EFE0-4411-AF1D-470665AE5544}"/>
+    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{4DAD8F7D-5BA1-49B6-A8CF-4B918380DD80}"/>
+    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{22BE950C-F455-4E27-99FA-6FC11355CA6C}"/>
+    <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{A9E1DC14-7AA1-4665-96BB-C377A5AC9EEB}"/>
+    <hyperlink ref="I34" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{ABD6399A-48A8-43DC-81D6-4783BF2F2E4E}"/>
+    <hyperlink ref="I16" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{8372074F-4EDD-49F0-B244-4991744D9248}"/>
+    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{F6B5C3BE-C6AB-4512-941C-184CE8BEEAF1}"/>
+    <hyperlink ref="I18" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{8543BA3C-E23B-47B4-96D1-A45EBF845020}"/>
+    <hyperlink ref="I20" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{5D01EC0A-D536-4864-962F-A6799D80AAC7}"/>
+    <hyperlink ref="I25" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{79A6BB29-939A-434D-9944-A7D8901809EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.1328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.53125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.46484375" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.53125" style="1"/>
+    <col min="10" max="10" width="12.44140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1177,7 +2825,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1209,7 +2857,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +2889,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1273,7 +2921,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1305,7 +2953,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1337,7 +2985,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="114" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +3017,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1401,7 +3049,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +3081,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1465,7 +3113,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +3127,7 @@
         <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>148</v>
@@ -1497,7 +3145,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1529,7 +3177,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1543,7 +3191,7 @@
         <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>164</v>
@@ -1561,7 +3209,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1593,7 +3241,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1625,7 +3273,7 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -1657,7 +3305,7 @@
         <v>45124</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -1689,7 +3337,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
@@ -1721,7 +3369,7 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -1753,7 +3401,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
@@ -1785,7 +3433,7 @@
         <v>45187</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1817,7 +3465,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -1849,7 +3497,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
@@ -1881,7 +3529,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
@@ -1913,7 +3561,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
@@ -1945,7 +3593,7 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -1977,7 +3625,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -2009,7 +3657,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -2041,7 +3689,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
@@ -2073,7 +3721,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="114" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
@@ -2105,7 +3753,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2137,7 +3785,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
@@ -2169,7 +3817,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -2201,7 +3849,7 @@
         <v>45084</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -2233,7 +3881,7 @@
         <v>45084</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
@@ -2265,7 +3913,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
@@ -2297,7 +3945,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="114" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -2329,7 +3977,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
@@ -2361,7 +4009,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
@@ -2393,7 +4041,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
@@ -2425,7 +4073,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>72</v>
       </c>
@@ -2457,7 +4105,7 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>115</v>
       </c>
@@ -2489,7 +4137,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>115</v>
       </c>
@@ -2521,7 +4169,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
@@ -2553,7 +4201,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>115</v>
       </c>
@@ -2585,7 +4233,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>115</v>
       </c>
@@ -2617,7 +4265,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>124</v>
       </c>
@@ -2649,7 +4297,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>215</v>
       </c>
@@ -2681,7 +4329,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="57" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>216</v>
       </c>
@@ -2768,7 +4416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
   <dimension ref="A1:I35"/>
   <sheetViews>
@@ -2776,18 +4424,18 @@
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="29.796875" customWidth="1"/>
-    <col min="3" max="3" width="31.19921875" customWidth="1"/>
-    <col min="6" max="6" width="51.46484375" customWidth="1"/>
-    <col min="7" max="7" width="16.796875" customWidth="1"/>
-    <col min="8" max="8" width="34.46484375" customWidth="1"/>
-    <col min="9" max="9" width="35.46484375" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" customWidth="1"/>
+    <col min="9" max="9" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2816,7 +4464,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2845,7 +4493,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -2874,7 +4522,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -2903,7 +4551,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2932,7 +4580,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2961,7 +4609,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -2990,7 +4638,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -3017,7 +4665,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -3046,7 +4694,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -3075,7 +4723,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -3104,7 +4752,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -3133,7 +4781,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
@@ -3162,7 +4810,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -3191,7 +4839,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>72</v>
       </c>
@@ -3220,7 +4868,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>72</v>
       </c>
@@ -3249,7 +4897,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>72</v>
       </c>
@@ -3278,7 +4926,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
@@ -3307,7 +4955,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>72</v>
       </c>
@@ -3336,7 +4984,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -3365,7 +5013,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -3394,7 +5042,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
@@ -3423,7 +5071,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>72</v>
       </c>
@@ -3452,7 +5100,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>72</v>
       </c>
@@ -3481,7 +5129,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -3510,7 +5158,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>72</v>
       </c>
@@ -3539,7 +5187,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -3568,7 +5216,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
@@ -3597,7 +5245,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>115</v>
       </c>
@@ -3626,7 +5274,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>115</v>
       </c>
@@ -3655,7 +5303,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>115</v>
       </c>
@@ -3684,7 +5332,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>115</v>
       </c>
@@ -3713,7 +5361,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>124</v>
       </c>
@@ -3740,7 +5388,7 @@
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>125</v>
       </c>
@@ -3767,7 +5415,7 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>126</v>
       </c>
@@ -3832,15 +5480,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4106,6 +5745,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4120,14 +5768,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4143,6 +5783,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Trying to fix binary
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABD7E08-96C2-420F-BD28-B49560C984AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650D014A-10B9-42A8-A65C-FD1919AB9F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-30" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments 12CY23" sheetId="3" r:id="rId1"/>
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 12CY23'!$A$1:$J$50</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1138,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3877,16 +3877,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4156,22 +4152,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4197,9 +4193,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Here Comes the Rain
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E365BE-AF96-4826-A01A-CE8F7304C38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91342630-5369-4341-AF27-2A9A7975AF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-30" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$51</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="246">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -763,6 +763,21 @@
   </si>
   <si>
     <t>[Preview]: Resources should be Zone Resilient - 130fb88f-0fc9-4678-bfe1-31022d71c7d5 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>In order to improve resilience and reliability, you need to be aware of where resources are deployed. To aid this awareness, ensure that the location of the resource group matches the location of the resources it contains.</t>
+  </si>
+  <si>
+    <t>Resource Group and Resource locations should match</t>
+  </si>
+  <si>
+    <t>Audit, Deny</t>
+  </si>
+  <si>
+    <t>Audit-ResourceRGLocation.json</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -1136,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1669,207 +1684,207 @@
         <v>45266</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>149</v>
+        <v>242</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>149</v>
+        <v>242</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="J17" s="5">
+        <v>45274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J18" s="5">
         <v>45124</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="J19" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>57</v>
+        <v>229</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="J20" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>223</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>223</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>225</v>
+        <v>55</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>234</v>
+        <v>56</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="J21" s="5">
-        <v>45187</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>63</v>
+        <v>230</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J22" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1878,16 +1893,16 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>207</v>
+        <v>62</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="J23" s="5">
         <v>45018</v>
@@ -1898,10 +1913,10 @@
         <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
@@ -1910,94 +1925,94 @@
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J24" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J25" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>226</v>
+        <v>69</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>235</v>
+        <v>70</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="J26" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
@@ -2006,48 +2021,48 @@
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>74</v>
+        <v>226</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>77</v>
+        <v>231</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J27" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>207</v>
+        <v>76</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="J28" s="5">
         <v>45018</v>
@@ -2058,10 +2073,10 @@
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
@@ -2070,62 +2085,62 @@
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J29" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="J30" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -2134,30 +2149,30 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -2166,16 +2181,16 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
@@ -2186,10 +2201,10 @@
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2198,30 +2213,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2230,30 +2245,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>213</v>
+        <v>94</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J34" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>211</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2262,30 +2277,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>212</v>
+        <v>98</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="J35" s="5">
         <v>45084</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2294,30 +2309,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>51</v>
+        <v>99</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J36" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2326,30 +2341,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="J37" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2358,30 +2373,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2390,48 +2405,48 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>200</v>
+        <v>113</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
@@ -2442,28 +2457,28 @@
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>203</v>
+        <v>152</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J41" s="5">
         <v>45018</v>
@@ -2474,42 +2489,42 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="J42" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2518,30 +2533,30 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>119</v>
+        <v>232</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="J43" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2550,62 +2565,62 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J44" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>144</v>
+        <v>122</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J45" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>204</v>
+        <v>142</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>40</v>
@@ -2614,30 +2629,30 @@
         <v>24</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>205</v>
+        <v>146</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>40</v>
@@ -2646,94 +2661,94 @@
         <v>24</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>206</v>
+        <v>154</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>45</v>
+        <v>156</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>45</v>
+        <v>157</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>215</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>201</v>
+        <v>45</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -2742,23 +2757,55 @@
         <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J50" s="5">
         <v>45018</v>
       </c>
     </row>
+    <row r="51" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J50" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:J51" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
     <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
@@ -2766,46 +2813,46 @@
     <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
     <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
     <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I18" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I20" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I22" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I24" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I25" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I27" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I29" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I30" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I31" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I32" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I33" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I34" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I36" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I37" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I38" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I39" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I43" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I44" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I19" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I21" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I23" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I25" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I26" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I28" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I30" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I31" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I32" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I33" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I34" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I35" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I37" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I38" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I39" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I40" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I44" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I45" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
     <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
     <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I45" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I46" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
     <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I40" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I49" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I50" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I41" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I46" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I47" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I28" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I23" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I41" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I50" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I51" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I42" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I47" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I48" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I29" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I24" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
     <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
     <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
-    <hyperlink ref="I35" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I17" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I36" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I18" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
     <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
-    <hyperlink ref="I19" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
-    <hyperlink ref="I21" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
-    <hyperlink ref="I26" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
+    <hyperlink ref="I20" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
+    <hyperlink ref="I22" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
+    <hyperlink ref="I27" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
     <hyperlink ref="I16" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3877,12 +3924,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4152,22 +4203,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4193,13 +4244,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Removing custom policy and using the built in.
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91342630-5369-4341-AF27-2A9A7975AF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A83A2-A20E-49AB-81FF-6F2C87D4E367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-30" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="245">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -771,13 +771,10 @@
     <t>Resource Group and Resource locations should match</t>
   </si>
   <si>
-    <t>Audit, Deny</t>
-  </si>
-  <si>
     <t>Audit-ResourceRGLocation.json</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>Audit resource location matches resource group location - 0a914e76-4921-4c19-b460-a2d36003525a (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,19 +1695,19 @@
         <v>40</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>241</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="J17" s="5">
         <v>45274</v>
@@ -2854,9 +2851,10 @@
     <hyperlink ref="I22" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
     <hyperlink ref="I27" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
     <hyperlink ref="I16" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
+    <hyperlink ref="I17" r:id="rId48" display="https://www.azadvertizer.net/azpolicyadvertizer/0a914e76-4921-4c19-b460-a2d36003525a.html" xr:uid="{25C8B460-23BD-4C40-8D4F-9A57005D6348}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId48"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -3924,16 +3922,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4203,22 +4197,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4244,9 +4238,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
New Policy/Assignment: Resource Group and Resource locations should match (#1507)
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E365BE-AF96-4826-A01A-CE8F7304C38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A83A2-A20E-49AB-81FF-6F2C87D4E367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-30" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$51</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="245">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -763,6 +763,18 @@
   </si>
   <si>
     <t>[Preview]: Resources should be Zone Resilient - 130fb88f-0fc9-4678-bfe1-31022d71c7d5 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>In order to improve resilience and reliability, you need to be aware of where resources are deployed. To aid this awareness, ensure that the location of the resource group matches the location of the resources it contains.</t>
+  </si>
+  <si>
+    <t>Resource Group and Resource locations should match</t>
+  </si>
+  <si>
+    <t>Audit-ResourceRGLocation.json</t>
+  </si>
+  <si>
+    <t>Audit resource location matches resource group location - 0a914e76-4921-4c19-b460-a2d36003525a (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1148,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1669,207 +1681,207 @@
         <v>45266</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="J17" s="5">
+        <v>45274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J18" s="5">
         <v>45124</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J18" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="J19" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>57</v>
+        <v>229</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="J20" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>223</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>223</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>225</v>
+        <v>55</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>234</v>
+        <v>56</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="J21" s="5">
-        <v>45187</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>63</v>
+        <v>230</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J22" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1878,16 +1890,16 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>207</v>
+        <v>62</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="J23" s="5">
         <v>45018</v>
@@ -1898,10 +1910,10 @@
         <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
@@ -1910,94 +1922,94 @@
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J24" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J25" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>226</v>
+        <v>69</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>235</v>
+        <v>70</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="J26" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>11</v>
@@ -2006,48 +2018,48 @@
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>74</v>
+        <v>226</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>77</v>
+        <v>231</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J27" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>207</v>
+        <v>76</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="J28" s="5">
         <v>45018</v>
@@ -2058,10 +2070,10 @@
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
@@ -2070,62 +2082,62 @@
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J29" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="J30" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -2134,30 +2146,30 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -2166,16 +2178,16 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
@@ -2186,10 +2198,10 @@
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2198,30 +2210,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2230,30 +2242,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>213</v>
+        <v>94</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J34" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>211</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2262,30 +2274,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>212</v>
+        <v>98</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="J35" s="5">
         <v>45084</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2294,30 +2306,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>51</v>
+        <v>99</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J36" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2326,30 +2338,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="J37" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2358,30 +2370,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2390,48 +2402,48 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>200</v>
+        <v>113</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
@@ -2442,28 +2454,28 @@
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>203</v>
+        <v>152</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J41" s="5">
         <v>45018</v>
@@ -2474,42 +2486,42 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="J42" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2518,30 +2530,30 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>119</v>
+        <v>232</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="J43" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2550,62 +2562,62 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J44" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>144</v>
+        <v>122</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J45" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>204</v>
+        <v>142</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>40</v>
@@ -2614,30 +2626,30 @@
         <v>24</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>205</v>
+        <v>146</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>40</v>
@@ -2646,94 +2658,94 @@
         <v>24</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>206</v>
+        <v>154</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>45</v>
+        <v>156</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>45</v>
+        <v>157</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>215</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>201</v>
+        <v>45</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -2742,23 +2754,55 @@
         <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J50" s="5">
         <v>45018</v>
       </c>
     </row>
+    <row r="51" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J50" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:J51" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
     <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
@@ -2766,50 +2810,51 @@
     <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
     <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
     <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I18" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I20" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I22" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I24" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I25" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I27" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I29" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I30" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I31" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I32" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I33" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I34" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I36" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I37" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I38" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I39" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I43" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I44" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I19" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I21" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I23" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I25" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I26" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I28" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I30" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I31" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I32" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I33" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I34" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I35" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I37" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I38" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I39" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I40" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I44" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I45" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
     <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
     <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I45" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I46" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
     <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I40" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I49" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I50" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I41" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I46" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I47" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I28" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I23" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I41" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I50" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I51" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I42" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I47" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I48" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I29" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I24" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
     <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
     <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
-    <hyperlink ref="I35" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I17" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I36" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I18" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
     <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
-    <hyperlink ref="I19" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
-    <hyperlink ref="I21" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
-    <hyperlink ref="I26" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
+    <hyperlink ref="I20" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
+    <hyperlink ref="I22" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
+    <hyperlink ref="I27" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
     <hyperlink ref="I16" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
+    <hyperlink ref="I17" r:id="rId48" display="https://www.azadvertizer.net/azpolicyadvertizer/0a914e76-4921-4c19-b460-a2d36003525a.html" xr:uid="{25C8B460-23BD-4C40-8D4F-9A57005D6348}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId48"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Policy Refresh Q2FY24 (#1552)
Co-authored-by: JamJarchitect <53943045+JamJarchitect@users.noreply.github.com>
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
Co-authored-by: Linda Karin Elsie Petersson <38290892+lvlindv@users.noreply.github.com>
Co-authored-by: brsteph <96074545+brsteph@users.noreply.github.com>
Co-authored-by: Arjen Huitema <arjenhuitema@microsoft.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E380B3-39F1-447E-B796-D38095CF90CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A83A2-A20E-49AB-81FF-6F2C87D4E367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-30" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments 12CY23" sheetId="5" r:id="rId1"/>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId2"/>
-    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId3"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
+    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$49</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 12CY23'!$A$1:$J$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$51</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="245">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -753,6 +751,30 @@
   </si>
   <si>
     <t>Deploy Azure Monitor Baseline Alerts for Landing Zone - Alerting-LandingZone (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Resources should be Zone Resilient</t>
+  </si>
+  <si>
+    <t>Some resource types can be deployed Zone Redundant (e.g. SQL Databases); some can be deploy Zone Aligned (e.g. Virtual Machines); and some can be deployed either Zone Aligned or Zone Redundant (e.g. Virtual Machine Scale Sets). Being zone aligned does not guarantee resilience, but it is the foundation on which a resilient solution can be built (e.g. three Virtual Machine Scale Sets zone aligned to three different zones in the same region with a load balancer). See https://aka.ms/AZResilience for more info.</t>
+  </si>
+  <si>
+    <t>AUDIT-ZoneResilientPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>[Preview]: Resources should be Zone Resilient - 130fb88f-0fc9-4678-bfe1-31022d71c7d5 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>In order to improve resilience and reliability, you need to be aware of where resources are deployed. To aid this awareness, ensure that the location of the resource group matches the location of the resources it contains.</t>
+  </si>
+  <si>
+    <t>Resource Group and Resource locations should match</t>
+  </si>
+  <si>
+    <t>Audit-ResourceRGLocation.json</t>
+  </si>
+  <si>
+    <t>Audit resource location matches resource group location - 0a914e76-4921-4c19-b460-a2d36003525a (azadvertizer.net)</t>
   </si>
 </sst>
 </file>
@@ -1125,11 +1147,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7B1182-4665-4109-8EF9-9158E84D9F8E}">
-  <dimension ref="A1:J49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1481,7 +1503,7 @@
         <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>148</v>
@@ -1545,7 +1567,7 @@
         <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>164</v>
@@ -1627,47 +1649,47 @@
         <v>45180</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>150</v>
+        <v>238</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>200</v>
+        <v>239</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="J16" s="5">
-        <v>45124</v>
+        <v>45266</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>242</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>242</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>40</v>
@@ -1676,30 +1698,30 @@
         <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>48</v>
+        <v>241</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>51</v>
+        <v>243</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>244</v>
       </c>
       <c r="J17" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>221</v>
+        <v>149</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -1708,30 +1730,30 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>222</v>
+        <v>150</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>233</v>
+        <v>152</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J18" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -1740,16 +1762,16 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J19" s="5">
         <v>45018</v>
@@ -1757,13 +1779,13 @@
     </row>
     <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
@@ -1772,94 +1794,94 @@
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J20" s="5">
-        <v>45187</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J21" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>207</v>
+        <v>230</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J22" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1868,254 +1890,254 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J23" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>71</v>
+        <v>172</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J24" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>224</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>224</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>226</v>
+        <v>65</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>235</v>
+        <v>66</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="J25" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J26" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>173</v>
+        <v>226</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>207</v>
+        <v>231</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J27" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="J28" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>81</v>
+        <v>172</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J29" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="J30" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
@@ -2124,30 +2146,30 @@
         <v>24</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -2156,30 +2178,30 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2188,30 +2210,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>213</v>
+        <v>89</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J33" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>211</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>211</v>
+        <v>91</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2220,30 +2242,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>212</v>
+        <v>92</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>214</v>
+        <v>94</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="J34" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2252,30 +2274,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>50</v>
+        <v>213</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="J35" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2284,30 +2306,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>104</v>
+        <v>212</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J36" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2316,30 +2338,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="J37" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2348,62 +2370,62 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>200</v>
+        <v>109</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>158</v>
+        <v>111</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2412,16 +2434,16 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>203</v>
+        <v>113</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
@@ -2432,10 +2454,10 @@
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>227</v>
+        <v>149</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>227</v>
+        <v>149</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -2444,62 +2466,62 @@
         <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>228</v>
+        <v>150</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>236</v>
+        <v>152</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J41" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>119</v>
+        <v>160</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="J42" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2508,19 +2530,19 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>121</v>
+        <v>228</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>123</v>
+        <v>232</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="J43" s="5">
-        <v>45018</v>
+        <v>45180</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2528,60 +2550,60 @@
         <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J44" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>205</v>
+        <v>122</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J45" s="5">
         <v>45018</v>
@@ -2592,10 +2614,10 @@
         <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>40</v>
@@ -2604,1765 +2626,183 @@
         <v>24</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>206</v>
+        <v>146</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>45</v>
+        <v>154</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>201</v>
+        <v>157</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>216</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>202</v>
+        <v>45</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
       </c>
     </row>
+    <row r="50" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J50" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J49" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{F68C5E7F-0D92-4692-B9FD-FA4BADBB8FAD}"/>
-    <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{4922A37A-092D-4A2C-81A4-B92C26D8C8E9}"/>
-    <hyperlink ref="I5" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{F8BA97F3-303F-4C38-8898-E256DD9130C2}"/>
-    <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{367A85F5-96A9-40F4-925D-FDB06A2E3DDD}"/>
-    <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{7587EC6C-3EC1-4B0E-9CD2-9BA6EE18C958}"/>
-    <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{DBCC2C73-304C-4B93-8F29-C4F94B35CB1A}"/>
-    <hyperlink ref="I17" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{39FC4DB8-CB4D-48DD-ACA9-856296CD94DF}"/>
-    <hyperlink ref="I19" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{16316F4D-CE83-44A6-88A3-692A34400BFE}"/>
-    <hyperlink ref="I21" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{94FEED80-A7C9-47CF-B90F-98EA10E6FAE4}"/>
-    <hyperlink ref="I23" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{03B0DF73-0B97-475D-85F0-5C00EF91A545}"/>
-    <hyperlink ref="I24" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{B8810D5A-DC44-4DF4-A706-3855C0C45D96}"/>
-    <hyperlink ref="I26" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{3FE4B42C-F6A1-41EA-AC5E-89FB7E1D93FE}"/>
-    <hyperlink ref="I28" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{9C39FBDD-6917-41EF-9279-D36FFD85209E}"/>
-    <hyperlink ref="I29" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{29FBD2DC-19E8-4578-BFB0-1727BE9B485C}"/>
-    <hyperlink ref="I30" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{25AFED85-48D4-4D94-9CCD-02BB107963A7}"/>
-    <hyperlink ref="I31" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{653E5BFB-2C45-43C9-AD1D-B88AB88E9257}"/>
-    <hyperlink ref="I32" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5B17C2AD-56D7-412D-9670-FBEBD0BE0838}"/>
-    <hyperlink ref="I33" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{B5EDD756-7192-4902-BD7E-0922F5405BC4}"/>
-    <hyperlink ref="I35" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{4E7F0D4A-92D8-4A12-AE80-BD7D87CA95E1}"/>
-    <hyperlink ref="I36" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{0F818706-C153-4CBC-98B5-FC3FD12323E9}"/>
-    <hyperlink ref="I37" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{49E32576-5222-411C-9306-575C68BA48BA}"/>
-    <hyperlink ref="I38" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{D165A2DC-684A-41FF-BBA3-3D81B98CD413}"/>
-    <hyperlink ref="I42" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{67A44FEE-082D-4CB2-8E34-23D1DAD2B30B}"/>
-    <hyperlink ref="I43" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{09E7D7FC-DB0A-4BA1-AD89-7AAB980C3CB3}"/>
-    <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{D39F09F2-B2B5-4140-BC61-43F89B8D4C18}"/>
-    <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{456F843D-17A5-4985-BA3D-1F4BD3C6AABF}"/>
-    <hyperlink ref="I44" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{94C3CF6E-18EE-49FE-9D09-15DCFA40A1F1}"/>
-    <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{5898AEFA-DD35-4895-A8DE-88B1CF610C69}"/>
-    <hyperlink ref="I39" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D1D00F1F-3215-4A56-83EF-29A879D07E71}"/>
-    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{B973B264-05EE-4863-BFC9-474245901E65}"/>
-    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{A305219B-0027-478A-AFFE-2564BF13467E}"/>
-    <hyperlink ref="I40" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{511DE963-0BC7-4BDD-874D-BDB2F9A0F465}"/>
-    <hyperlink ref="I45" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDE193E1-1120-45C9-A636-97EC7A443022}"/>
-    <hyperlink ref="I46" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{E84AEDB7-FF67-4FD4-8232-B0DD829AEB2D}"/>
-    <hyperlink ref="I27" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{27C701D5-7B42-4357-AEDF-560CE040D9A7}"/>
-    <hyperlink ref="I22" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{37BF929F-CD7F-41BD-8673-EFD75351CCBF}"/>
-    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{4D026B69-EFE0-4411-AF1D-470665AE5544}"/>
-    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{4DAD8F7D-5BA1-49B6-A8CF-4B918380DD80}"/>
-    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{22BE950C-F455-4E27-99FA-6FC11355CA6C}"/>
-    <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{A9E1DC14-7AA1-4665-96BB-C377A5AC9EEB}"/>
-    <hyperlink ref="I34" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{ABD6399A-48A8-43DC-81D6-4783BF2F2E4E}"/>
-    <hyperlink ref="I16" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{8372074F-4EDD-49F0-B244-4991744D9248}"/>
-    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{F6B5C3BE-C6AB-4512-941C-184CE8BEEAF1}"/>
-    <hyperlink ref="I18" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{8543BA3C-E23B-47B4-96D1-A45EBF845020}"/>
-    <hyperlink ref="I20" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{5D01EC0A-D536-4864-962F-A6799D80AAC7}"/>
-    <hyperlink ref="I25" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{79A6BB29-939A-434D-9944-A7D8901809EE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId47"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:J49"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.5546875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="J3" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="J8" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="J9" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="J11" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="J12" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="J13" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="J14" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="J15" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="J16" s="5">
-        <v>45124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="J18" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J19" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="J20" s="5">
-        <v>45187</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J21" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="J22" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J24" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="J25" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="J26" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="J27" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J28" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J29" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J30" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J31" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J32" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J33" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="J34" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J35" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J36" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J37" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J38" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="J39" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I40" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="J40" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="J41" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="J42" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J43" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="J44" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="J45" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="J46" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J47" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="J48" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="J49" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:J49" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:J51" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
     <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
@@ -4370,53 +2810,55 @@
     <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
     <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
     <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I17" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I19" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I21" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I23" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I24" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I26" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I28" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I29" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I30" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I31" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I32" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I33" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I35" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I36" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I37" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I38" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I42" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I43" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I19" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I21" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I23" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I25" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I26" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I28" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I30" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I31" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I32" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I33" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I34" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I35" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I37" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I38" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I39" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I40" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I44" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I45" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
     <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
     <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I44" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I46" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
     <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I39" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I40" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I45" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I46" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I27" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I22" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I41" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I50" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I51" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I42" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I47" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I48" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I29" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I24" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
     <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
     <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
     <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
     <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
-    <hyperlink ref="I34" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I16" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I36" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I18" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
     <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
-    <hyperlink ref="I18" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
-    <hyperlink ref="I20" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
-    <hyperlink ref="I25" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
+    <hyperlink ref="I20" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
+    <hyperlink ref="I22" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
+    <hyperlink ref="I27" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
+    <hyperlink ref="I16" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
+    <hyperlink ref="I17" r:id="rId48" display="https://www.azadvertizer.net/azpolicyadvertizer/0a914e76-4921-4c19-b460-a2d36003525a.html" xr:uid="{25C8B460-23BD-4C40-8D4F-9A57005D6348}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId47"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
   <dimension ref="A1:I35"/>
   <sheetViews>
@@ -5480,6 +3922,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5745,15 +4196,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5768,6 +4210,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5783,14 +4233,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update ALZ Policy Assignments v2.xlsx
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A83A2-A20E-49AB-81FF-6F2C87D4E367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FB21AF-F358-4D4C-9BED-2A346906E5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-30" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-46188" yWindow="-108" windowWidth="46296" windowHeight="26136" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="247">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -775,6 +775,12 @@
   </si>
   <si>
     <t>Audit resource location matches resource group location - 0a914e76-4921-4c19-b460-a2d36003525a (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforce policies in the Decommissioned Landing Zone</t>
+  </si>
+  <si>
+    <t>Enforce policies in the Sandbox Landing Zone</t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2745,7 +2751,7 @@
         <v>135</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -2777,7 +2783,7 @@
         <v>139</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>139</v>
+        <v>246</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -3922,12 +3928,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4197,22 +4207,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4238,13 +4248,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Minor Policy Doc update (#1575)
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551A83A2-A20E-49AB-81FF-6F2C87D4E367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FB21AF-F358-4D4C-9BED-2A346906E5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-30" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-46188" yWindow="-108" windowWidth="46296" windowHeight="26136" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="247">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -775,6 +775,12 @@
   </si>
   <si>
     <t>Audit resource location matches resource group location - 0a914e76-4921-4c19-b460-a2d36003525a (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enforce policies in the Decommissioned Landing Zone</t>
+  </si>
+  <si>
+    <t>Enforce policies in the Sandbox Landing Zone</t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2745,7 +2751,7 @@
         <v>135</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>11</v>
@@ -2777,7 +2783,7 @@
         <v>139</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>139</v>
+        <v>246</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -3922,12 +3928,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4197,22 +4207,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4238,13 +4248,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Binary changes to Excel
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0756AF16-46A4-4BD1-939E-13DC0C152604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695C8D20-2430-494C-8EB4-BBCC4C68C8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-38510" yWindow="20" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="258">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -772,6 +772,48 @@
   </si>
   <si>
     <t>Enforce-BackupPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-MDEndpointsAMAPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy-MDEndpointsAMA</t>
+  </si>
+  <si>
+    <t>Configure multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud</t>
+  </si>
+  <si>
+    <t>Configure the multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud (WDATP, WDATP_EXCLUDE_LINUX_PUBLIC_PREVIEW, WDATP_UNIFIED_SOLUTION etc.). See: https://learn.microsoft.com/azure/defender-for-cloud/integration-defender-for-endpoint for more information.</t>
+  </si>
+  <si>
+    <t>Configure multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud - 77b391e3-2d5d-40c3-83bf-65c846b3c6a3 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable allLogs category group resource logging for supported resources to Log Analytics</t>
+  </si>
+  <si>
+    <t>Enable allLogs category group resource logging for supported resources to Log Analytics - 0884adba-2312-4468-abeb-5422caed1038 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Resource logs should be enabled to track activities and events that take place on your resources and give you visibility and insights into any changes that occur. This initiative deploys diagnostic setting using the allLogs category group to route logs to Log Analytics Workspace for all supported resources</t>
+  </si>
+  <si>
+    <t>Trusted Launch improves security of a Virtual Machine which requires VM SKU, OS Disk &amp; OS Image to support it (Gen 2). To learn more about Trusted Launch, visit https://aka.ms/trustedlaunch.</t>
+  </si>
+  <si>
+    <t>AUDIT-TrustedLauchPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Audit-TrustedLaunch</t>
   </si>
 </sst>
 </file>
@@ -781,7 +823,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,6 +842,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Corbel"/>
       <family val="2"/>
@@ -836,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -861,6 +911,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1145,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,7 +1219,7 @@
     <col min="11" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1197,8 +1250,11 @@
       <c r="J1" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1230,7 +1286,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1262,79 +1318,85 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>247</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
+        <v>244</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="J4" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>254</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="J5" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -1343,30 +1405,30 @@
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J6" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1375,30 +1437,30 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J7" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1407,30 +1469,30 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>128</v>
+        <v>35</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>129</v>
+        <v>36</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="J8" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -1439,190 +1501,190 @@
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="J9" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>43</v>
+        <v>133</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="J10" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>147</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>148</v>
+        <v>41</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>206</v>
+        <v>42</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="J11" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J12" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J13" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J14" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -1631,94 +1693,94 @@
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>218</v>
+        <v>169</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>220</v>
+        <v>170</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="J15" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>240</v>
+        <v>219</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="J16" s="5">
-        <v>45266</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>150</v>
+        <v>238</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>200</v>
+        <v>239</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="J17" s="5">
-        <v>45124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -1727,60 +1789,63 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I18" s="4"/>
+        <v>256</v>
+      </c>
+      <c r="I18" s="6"/>
       <c r="J18" s="5">
-        <v>45363</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>51</v>
+        <v>152</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J19" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
@@ -1789,30 +1854,28 @@
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>233</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I20" s="4"/>
       <c r="J20" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>40</v>
@@ -1821,30 +1884,30 @@
         <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J21" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
@@ -1853,94 +1916,94 @@
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J22" s="5">
-        <v>45187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J23" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>207</v>
+        <v>230</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J24" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -1949,254 +2012,254 @@
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J25" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>71</v>
+        <v>172</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J26" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>224</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>224</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>226</v>
+        <v>65</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="J27" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J28" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>173</v>
+        <v>226</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>207</v>
+        <v>231</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J29" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="J30" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>81</v>
+        <v>172</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2205,30 +2268,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2237,30 +2300,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="J34" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2269,30 +2332,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>213</v>
+        <v>89</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J35" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>91</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>91</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2301,30 +2364,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>212</v>
+        <v>92</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>214</v>
+        <v>94</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="J36" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2333,30 +2396,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>50</v>
+        <v>213</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="J37" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2365,30 +2428,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>212</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J38" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2397,30 +2460,30 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2429,81 +2492,83 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>200</v>
+        <v>109</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="J41" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>111</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>241</v>
+        <v>111</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>242</v>
+        <v>112</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I42" s="4"/>
+        <v>113</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="J42" s="5">
-        <v>45363</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2511,31 +2576,31 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>203</v>
+        <v>152</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J43" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2543,10 +2608,10 @@
         <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2555,62 +2620,60 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>236</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I44" s="4"/>
       <c r="J44" s="5">
-        <v>45018</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>119</v>
+        <v>160</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="J45" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -2619,16 +2682,16 @@
         <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>121</v>
+        <v>228</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>123</v>
+        <v>232</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
@@ -2639,60 +2702,60 @@
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>205</v>
+        <v>122</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
@@ -2703,10 +2766,10 @@
         <v>115</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>40</v>
@@ -2715,167 +2778,232 @@
         <v>24</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>206</v>
+        <v>146</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>45</v>
+        <v>154</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="J50" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>201</v>
+        <v>157</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J51" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J52" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J53" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I52" s="6" t="s">
+      <c r="I54" s="6" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J51" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:K1" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
-    <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
-    <hyperlink ref="I5" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
-    <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
-    <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
-    <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I19" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I21" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I23" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I25" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I26" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I28" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I30" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I31" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I32" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I33" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I34" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I35" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I37" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I38" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I39" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I40" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I45" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I46" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I47" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
-    <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I41" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I51" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I52" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I43" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I48" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I49" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I29" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I24" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
-    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
-    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
-    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
-    <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
-    <hyperlink ref="I36" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I17" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
-    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
-    <hyperlink ref="I20" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
-    <hyperlink ref="I22" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
-    <hyperlink ref="I27" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
-    <hyperlink ref="I16" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
+    <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
+    <hyperlink ref="I7" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
+    <hyperlink ref="I8" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
+    <hyperlink ref="I11" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
+    <hyperlink ref="I21" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I23" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I25" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I27" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I28" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I30" r:id="rId11" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I35" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I36" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I37" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I40" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I41" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I42" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I47" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I48" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I9" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I10" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I49" r:id="rId26" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I3" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
+    <hyperlink ref="I43" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I53" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I54" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I45" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I50" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I51" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I31" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I26" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I15" r:id="rId36" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
+    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
+    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
+    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
+    <hyperlink ref="I38" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I19" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I16" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
+    <hyperlink ref="I22" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
+    <hyperlink ref="I24" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
+    <hyperlink ref="I29" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
+    <hyperlink ref="I17" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
+    <hyperlink ref="I4" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{EAA9BFF3-4905-49C3-ABC1-9A75BCE68CB9}"/>
+    <hyperlink ref="I5" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{E8F3A9AD-20B7-4E98-9BA2-CF6D98053BF8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId48"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -3956,6 +4084,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4221,15 +4358,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
@@ -4243,6 +4371,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4262,14 +4398,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Updating Microsoft Defender for Endpoints to use new initiative (#1639)
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0756AF16-46A4-4BD1-939E-13DC0C152604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695C8D20-2430-494C-8EB4-BBCC4C68C8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-38510" yWindow="20" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
     <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="258">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -772,6 +772,48 @@
   </si>
   <si>
     <t>Enforce-BackupPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-MDEndpointsAMAPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy-MDEndpointsAMA</t>
+  </si>
+  <si>
+    <t>Configure multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud</t>
+  </si>
+  <si>
+    <t>Configure the multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud (WDATP, WDATP_EXCLUDE_LINUX_PUBLIC_PREVIEW, WDATP_UNIFIED_SOLUTION etc.). See: https://learn.microsoft.com/azure/defender-for-cloud/integration-defender-for-endpoint for more information.</t>
+  </si>
+  <si>
+    <t>Configure multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud - 77b391e3-2d5d-40c3-83bf-65c846b3c6a3 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable allLogs category group resource logging for supported resources to Log Analytics</t>
+  </si>
+  <si>
+    <t>Enable allLogs category group resource logging for supported resources to Log Analytics - 0884adba-2312-4468-abeb-5422caed1038 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Resource logs should be enabled to track activities and events that take place on your resources and give you visibility and insights into any changes that occur. This initiative deploys diagnostic setting using the allLogs category group to route logs to Log Analytics Workspace for all supported resources</t>
+  </si>
+  <si>
+    <t>Trusted Launch improves security of a Virtual Machine which requires VM SKU, OS Disk &amp; OS Image to support it (Gen 2). To learn more about Trusted Launch, visit https://aka.ms/trustedlaunch.</t>
+  </si>
+  <si>
+    <t>AUDIT-TrustedLauchPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Audit-TrustedLaunch</t>
   </si>
 </sst>
 </file>
@@ -781,7 +823,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,6 +842,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Corbel"/>
       <family val="2"/>
@@ -836,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -861,6 +911,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1145,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1166,7 +1219,7 @@
     <col min="11" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1197,8 +1250,11 @@
       <c r="J1" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1230,7 +1286,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1262,79 +1318,85 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>247</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
+        <v>244</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="J4" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>254</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="J5" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -1343,30 +1405,30 @@
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J6" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1375,30 +1437,30 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J7" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1407,30 +1469,30 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>128</v>
+        <v>35</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>129</v>
+        <v>36</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="J8" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -1439,190 +1501,190 @@
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="J9" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>43</v>
+        <v>133</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="J10" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>147</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>148</v>
+        <v>41</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>206</v>
+        <v>42</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="J11" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J12" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J13" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J14" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>217</v>
+        <v>168</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
@@ -1631,94 +1693,94 @@
         <v>12</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>218</v>
+        <v>169</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>220</v>
+        <v>170</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="J15" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>240</v>
+        <v>219</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="J16" s="5">
-        <v>45266</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>149</v>
+        <v>237</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>150</v>
+        <v>238</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>200</v>
+        <v>239</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="J17" s="5">
-        <v>45124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -1727,60 +1789,63 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>242</v>
+        <v>255</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I18" s="4"/>
+        <v>256</v>
+      </c>
+      <c r="I18" s="6"/>
       <c r="J18" s="5">
-        <v>45363</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>51</v>
+        <v>152</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J19" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>11</v>
@@ -1789,30 +1854,28 @@
         <v>12</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>233</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I20" s="4"/>
       <c r="J20" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>40</v>
@@ -1821,30 +1884,30 @@
         <v>24</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J21" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
@@ -1853,94 +1916,94 @@
         <v>12</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J22" s="5">
-        <v>45187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J23" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>171</v>
+        <v>223</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>173</v>
+        <v>225</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>207</v>
+        <v>230</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J24" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -1949,254 +2012,254 @@
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J25" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>71</v>
+        <v>172</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J26" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>224</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>224</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>226</v>
+        <v>65</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="J27" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J28" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>173</v>
+        <v>226</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>207</v>
+        <v>231</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J29" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="J30" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>171</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>79</v>
+        <v>173</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>81</v>
+        <v>172</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2205,30 +2268,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2237,30 +2300,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="J34" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2269,30 +2332,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>213</v>
+        <v>89</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="J35" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>91</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>91</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2301,30 +2364,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>212</v>
+        <v>92</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>214</v>
+        <v>94</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="J36" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2333,30 +2396,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>50</v>
+        <v>213</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="J37" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>211</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2365,30 +2428,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>212</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J38" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2397,30 +2460,30 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>109</v>
+        <v>50</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2429,81 +2492,83 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>200</v>
+        <v>109</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="J41" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>111</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>241</v>
+        <v>111</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>242</v>
+        <v>112</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I42" s="4"/>
+        <v>113</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="J42" s="5">
-        <v>45363</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2511,31 +2576,31 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>203</v>
+        <v>152</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J43" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2543,10 +2608,10 @@
         <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2555,62 +2620,60 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>236</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I44" s="4"/>
       <c r="J44" s="5">
-        <v>45018</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>119</v>
+        <v>160</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="J45" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
@@ -2619,16 +2682,16 @@
         <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>121</v>
+        <v>228</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>123</v>
+        <v>232</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
@@ -2639,60 +2702,60 @@
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>205</v>
+        <v>122</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
@@ -2703,10 +2766,10 @@
         <v>115</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>40</v>
@@ -2715,167 +2778,232 @@
         <v>24</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>206</v>
+        <v>146</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>45</v>
+        <v>154</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="J50" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>215</v>
+        <v>115</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>201</v>
+        <v>157</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J51" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J52" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J53" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D54" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I52" s="6" t="s">
+      <c r="I54" s="6" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J51" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:K1" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
-    <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
-    <hyperlink ref="I5" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
-    <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
-    <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
-    <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I19" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I21" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I23" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I25" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I26" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I28" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I30" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I31" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I32" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I33" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I34" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I35" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I37" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I38" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I39" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I40" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I45" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I46" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I47" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
-    <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I41" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I51" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I52" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I43" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I48" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I49" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I29" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I24" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
-    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
-    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
-    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
-    <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
-    <hyperlink ref="I36" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I17" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
-    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
-    <hyperlink ref="I20" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
-    <hyperlink ref="I22" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
-    <hyperlink ref="I27" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
-    <hyperlink ref="I16" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
+    <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
+    <hyperlink ref="I7" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
+    <hyperlink ref="I8" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
+    <hyperlink ref="I11" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
+    <hyperlink ref="I21" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I23" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I25" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I27" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I28" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I30" r:id="rId11" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I35" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I36" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I37" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I40" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I41" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I42" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I47" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I48" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I9" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I10" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I49" r:id="rId26" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I3" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
+    <hyperlink ref="I43" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I53" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I54" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I45" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I50" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I51" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I31" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I26" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I15" r:id="rId36" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
+    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
+    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
+    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
+    <hyperlink ref="I38" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I19" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I16" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
+    <hyperlink ref="I22" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
+    <hyperlink ref="I24" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
+    <hyperlink ref="I29" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
+    <hyperlink ref="I17" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
+    <hyperlink ref="I4" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{EAA9BFF3-4905-49C3-ABC1-9A75BCE68CB9}"/>
+    <hyperlink ref="I5" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{E8F3A9AD-20B7-4E98-9BA2-CF6D98053BF8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId48"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -3956,6 +4084,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4221,15 +4358,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
@@ -4243,6 +4371,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4262,14 +4398,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
chore: Rename policy assignment from "Deploy-Resource-Diag" to "Deploy-Diag-Logs"
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695C8D20-2430-494C-8EB4-BBCC4C68C8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55EE716-271C-4975-871D-891B4BF9F7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="20" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="259">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -814,6 +814,9 @@
   </si>
   <si>
     <t>Audit-TrustedLaunch</t>
+  </si>
+  <si>
+    <t>Deploy-Diag-Logs</t>
   </si>
 </sst>
 </file>
@@ -1200,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,7 +1361,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>258</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>249</v>
@@ -4084,15 +4087,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4358,6 +4352,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
@@ -4371,14 +4374,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4398,6 +4393,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Diagnostic Settings v2 🎉 (#1641)
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695C8D20-2430-494C-8EB4-BBCC4C68C8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55EE716-271C-4975-871D-891B4BF9F7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="20" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="259">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -814,6 +814,9 @@
   </si>
   <si>
     <t>Audit-TrustedLaunch</t>
+  </si>
+  <si>
+    <t>Deploy-Diag-Logs</t>
   </si>
 </sst>
 </file>
@@ -1200,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1358,7 +1361,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>258</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>249</v>
@@ -4084,15 +4087,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4358,6 +4352,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
@@ -4371,14 +4374,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4398,6 +4393,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Update policy assignment table
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -5,19 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55EE716-271C-4975-871D-891B4BF9F7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC9EA86-D637-4C62-8A9D-9DB71A1B5220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
-    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
+    <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId2"/>
+    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="300">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -817,6 +819,129 @@
   </si>
   <si>
     <t>Deploy-Diag-Logs</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for Hybrid Virtual Machines</t>
+  </si>
+  <si>
+    <t>Enable ChangeTracking and Inventory for virtual machines</t>
+  </si>
+  <si>
+    <t>Enable ChangeTracking and Inventory for virtual machine scale sets</t>
+  </si>
+  <si>
+    <t>Enable ChangeTracking and Inventory for Arc-enabled virtual machines</t>
+  </si>
+  <si>
+    <t>Enable Defender for SQL on SQL VMs and Arc-enabled SQL Servers</t>
+  </si>
+  <si>
+    <t>Do not allow deletion of resource types</t>
+  </si>
+  <si>
+    <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for VMs with Azure Monitoring Agent(AMA)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for VMSS with Azure Monitoring Agent(AMA)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for Hybrid VMs with AMA</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for virtual machines</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for virtual machine scale sets</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for Arc-enabled virtual machines</t>
+  </si>
+  <si>
+    <t>Configure SQL VMs and Arc-enabled SQL Servers to install Microsoft Defender for SQL and AMA with a user-defined LA workspace</t>
+  </si>
+  <si>
+    <t>This policy initiative installs the Azure Monitoring Agent (AMA) on the virtual machines (VMs) and enables Azure Monitor for them. Azure Monitor collects and analyzes data from the VMs, such as performance metrics, logs, and dependencies.</t>
+  </si>
+  <si>
+    <t>This policy initiative installs the Azure Monitoring Agent (AMA) on the virtual machines scale sets (VMSS) and enables Azure Monitor for them. Azure Monitor collects and analyzes data from the VMs, such as performance metrics, logs, and dependencies.</t>
+  </si>
+  <si>
+    <t>This policy initiative installs the Azure Monitoring Agent (AMA) on Arc-enabled servers (Hybrid) and enables Azure Monitor for them. Azure Monitor collects and analyzes data from the VMs, such as performance metrics, logs, and dependencies.</t>
+  </si>
+  <si>
+    <t>With this policy initiative, you can enable automatic OS updates assessment every 24 hours. This is a custom initiative of built-in policies.</t>
+  </si>
+  <si>
+    <t>This policy initiative enables ChangeTracking and Inventory for virtual machines. It uses a Data Collection Rule to define what data to collect and where to send it, and a user-assigned identity to authenticate the Azure Monitor Agent.</t>
+  </si>
+  <si>
+    <t>This policy initiative enables ChangeTracking and Inventory for virtual machines scale sets. It uses a Data Collection Rule to define what data to collect and where to send it, and a user-assigned identity to authenticate the Azure Monitor Agent.</t>
+  </si>
+  <si>
+    <t>This policy initiative enables ChangeTracking and Inventory for Arc-enabled servers. It uses a Data Collection Rule to define what data to collect and where to send it, and a user-assigned identity to authenticate the Azure Monitor Agent.</t>
+  </si>
+  <si>
+    <t>This policy initiative enables Microsoft Defender for SQL and AMA on SQL VMs and Arc-enabled SQL Servers.</t>
+  </si>
+  <si>
+    <t>This policy enables you to specify the resource types that your organization can protect from accidentals deletion by blocking delete calls using deny action effect. Assigned to deny the deletion of the User Assignment Managed Identity that is used for AMA.</t>
+  </si>
+  <si>
+    <t>DenyAction</t>
+  </si>
+  <si>
+    <t>DINE-ChangeTrackingVMArcPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-ChangeTrackingVMPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-ChangeTrackingVMSSPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-VMHybridMonitoringPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-MDFCDefenderSQLAMAPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DENYACTION-ResourceDeletionPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>MODIFY-AUM-CheckUpdatesPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Configure SQL VMs and Arc-enabled SQL Servers to install Microsoft Defender for SQL and AMA with a user-defined LA workspace - de01d381-bae9-4670-8870-786f89f49e26 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for virtual machines - 92a36f05-ebc9-4bba-9128-b47ad2ea3354 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for virtual machine scale sets - c4a70814-96be-461c-889f-2b27429120dc (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for Arc-enabled virtual machines - 53448c70-089b-4f52-8f38-89196d7f2de1 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for VMs with Azure Monitoring Agent(AMA) - 924bfe3a-762f-40e7-86dd-5c8b95eb09e6 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for VMSS with Azure Monitoring Agent(AMA) - f5bf694c-cca7-4033-b883-3a23327d5485 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for Hybrid VMs with AMA - 2b00397d-c309-49c4-aa5a-f0b2c5bc6321 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines - Deploy-AUM-CheckUpdates (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Do not allow deletion of resource types - 78460a36-508a-49a4-b2b2-2f5ec564f4bb (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>2024-01-34</t>
   </si>
 </sst>
 </file>
@@ -1200,11 +1325,2360 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
+  <dimension ref="A1:K69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="J4" s="5">
+        <v>45427</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J5" s="5">
+        <v>45427</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J7" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J10" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J11" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J12" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J13" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="J14" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="J15" s="5">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="5">
+        <v>45427</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J17" s="5">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="J20" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="J22" s="5">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J24" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J25" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="J27" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J28" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J29" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J30" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J31" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J32" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J33" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J34" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J35" s="5">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="J36" s="5">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J37" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J38" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J39" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J40" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J41" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="5">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J43" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J44" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J45" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J46" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J47" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J48" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J49" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J50" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{CB9AA3F5-0FB5-4271-B843-BAC441E7FF28}"/>
+    <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{C1E76027-B2E2-46AE-8FBD-9F0D49770442}"/>
+    <hyperlink ref="I9" r:id="rId3" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{189AA603-D080-4747-8EE4-022DEBF70AC4}"/>
+    <hyperlink ref="I19" r:id="rId4" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{A326BBFF-13EF-4D72-866F-C82B6DB948CD}"/>
+    <hyperlink ref="I21" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{47846F9C-9BA5-4D50-BAC9-044A2B38522A}"/>
+    <hyperlink ref="I23" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{722CA2FF-9269-4E2F-8533-5ED7705D010E}"/>
+    <hyperlink ref="I25" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{137ED18D-F3D4-4225-915D-7618E3EB3F48}"/>
+    <hyperlink ref="I26" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{CFB3D49B-0E77-431E-8A4B-6A6C45FACD99}"/>
+    <hyperlink ref="I28" r:id="rId9" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{56989C35-212B-48D1-817B-986C70EFFD3A}"/>
+    <hyperlink ref="I30" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
+    <hyperlink ref="I31" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
+    <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
+    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
+    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{FB722C1D-B184-4DFC-8C0C-C02F60381DAC}"/>
+    <hyperlink ref="I35" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
+    <hyperlink ref="I37" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
+    <hyperlink ref="I38" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
+    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
+    <hyperlink ref="I40" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
+    <hyperlink ref="I45" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
+    <hyperlink ref="I46" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
+    <hyperlink ref="I7" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
+    <hyperlink ref="I8" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
+    <hyperlink ref="I47" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
+    <hyperlink ref="I3" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
+    <hyperlink ref="I41" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
+    <hyperlink ref="I51" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
+    <hyperlink ref="I52" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
+    <hyperlink ref="I43" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
+    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
+    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
+    <hyperlink ref="I29" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
+    <hyperlink ref="I24" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
+    <hyperlink ref="I13" r:id="rId34" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
+    <hyperlink ref="I12" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
+    <hyperlink ref="I11" r:id="rId36" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
+    <hyperlink ref="I10" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
+    <hyperlink ref="I36" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
+    <hyperlink ref="I17" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
+    <hyperlink ref="I14" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
+    <hyperlink ref="I20" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
+    <hyperlink ref="I22" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
+    <hyperlink ref="I27" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
+    <hyperlink ref="I15" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
+    <hyperlink ref="I4" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
+    <hyperlink ref="I5" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
+    <hyperlink ref="I59" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
+    <hyperlink ref="I56" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
+    <hyperlink ref="I57" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
+    <hyperlink ref="I58" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
+    <hyperlink ref="I53" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
+    <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
+    <hyperlink ref="I55" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
+    <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
+    <hyperlink ref="I60" r:id="rId55" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
+    <hyperlink ref="I68" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I65" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I66" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I67" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I62" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I63" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I64" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I69" r:id="rId63" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId64"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3010,12 +5484,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="A5" sqref="A5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4087,6 +6561,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4352,15 +6835,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
@@ -4374,6 +6848,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4393,14 +6875,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Policy Refresh H2 FY24 (#1651)
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
Co-authored-by: rozkurt <72864397+rozkurt@users.noreply.github.com>
Co-authored-by: Recep Ozkurt <recepo@microsoft.com>
Co-authored-by: JamJarchitect <53943045+JamJarchitect@users.noreply.github.com>
Co-authored-by: Ravivarman13 <81689429+Ravivarman13@users.noreply.github.com>
Co-authored-by: Arjen Huitema <arjenhuitema@microsoft.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FB21AF-F358-4D4C-9BED-2A346906E5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC9EA86-D637-4C62-8A9D-9DB71A1B5220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46188" yWindow="-108" windowWidth="46296" windowHeight="26136" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId1"/>
-    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId2"/>
+    <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId2"/>
+    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$J$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="300">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -765,22 +767,181 @@
     <t>[Preview]: Resources should be Zone Resilient - 130fb88f-0fc9-4678-bfe1-31022d71c7d5 (azadvertizer.net)</t>
   </si>
   <si>
-    <t>In order to improve resilience and reliability, you need to be aware of where resources are deployed. To aid this awareness, ensure that the location of the resource group matches the location of the resources it contains.</t>
-  </si>
-  <si>
-    <t>Resource Group and Resource locations should match</t>
-  </si>
-  <si>
-    <t>Audit-ResourceRGLocation.json</t>
-  </si>
-  <si>
-    <t>Audit resource location matches resource group location - 0a914e76-4921-4c19-b460-a2d36003525a (azadvertizer.net)</t>
-  </si>
-  <si>
-    <t>Enforce policies in the Decommissioned Landing Zone</t>
-  </si>
-  <si>
-    <t>Enforce policies in the Sandbox Landing Zone</t>
+    <t>Enforce enhanced recovery and backup policies</t>
+  </si>
+  <si>
+    <t>This initiative assignment enables recommended audit policies for Azure Backup and Site Recovery.</t>
+  </si>
+  <si>
+    <t>Enforce-BackupPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-MDEndpointsAMAPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Deploy-MDEndpointsAMA</t>
+  </si>
+  <si>
+    <t>Configure multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud</t>
+  </si>
+  <si>
+    <t>Configure the multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud (WDATP, WDATP_EXCLUDE_LINUX_PUBLIC_PREVIEW, WDATP_UNIFIED_SOLUTION etc.). See: https://learn.microsoft.com/azure/defender-for-cloud/integration-defender-for-endpoint for more information.</t>
+  </si>
+  <si>
+    <t>Configure multiple Microsoft Defender for Endpoint integration settings with Microsoft Defender for Cloud - 77b391e3-2d5d-40c3-83bf-65c846b3c6a3 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable allLogs category group resource logging for supported resources to Log Analytics</t>
+  </si>
+  <si>
+    <t>Enable allLogs category group resource logging for supported resources to Log Analytics - 0884adba-2312-4468-abeb-5422caed1038 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>UPDATE</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Resource logs should be enabled to track activities and events that take place on your resources and give you visibility and insights into any changes that occur. This initiative deploys diagnostic setting using the allLogs category group to route logs to Log Analytics Workspace for all supported resources</t>
+  </si>
+  <si>
+    <t>Trusted Launch improves security of a Virtual Machine which requires VM SKU, OS Disk &amp; OS Image to support it (Gen 2). To learn more about Trusted Launch, visit https://aka.ms/trustedlaunch.</t>
+  </si>
+  <si>
+    <t>AUDIT-TrustedLauchPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Audit-TrustedLaunch</t>
+  </si>
+  <si>
+    <t>Deploy-Diag-Logs</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for Hybrid Virtual Machines</t>
+  </si>
+  <si>
+    <t>Enable ChangeTracking and Inventory for virtual machines</t>
+  </si>
+  <si>
+    <t>Enable ChangeTracking and Inventory for virtual machine scale sets</t>
+  </si>
+  <si>
+    <t>Enable ChangeTracking and Inventory for Arc-enabled virtual machines</t>
+  </si>
+  <si>
+    <t>Enable Defender for SQL on SQL VMs and Arc-enabled SQL Servers</t>
+  </si>
+  <si>
+    <t>Do not allow deletion of resource types</t>
+  </si>
+  <si>
+    <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for VMs with Azure Monitoring Agent(AMA)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for VMSS with Azure Monitoring Agent(AMA)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for Hybrid VMs with AMA</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for virtual machines</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for virtual machine scale sets</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for Arc-enabled virtual machines</t>
+  </si>
+  <si>
+    <t>Configure SQL VMs and Arc-enabled SQL Servers to install Microsoft Defender for SQL and AMA with a user-defined LA workspace</t>
+  </si>
+  <si>
+    <t>This policy initiative installs the Azure Monitoring Agent (AMA) on the virtual machines (VMs) and enables Azure Monitor for them. Azure Monitor collects and analyzes data from the VMs, such as performance metrics, logs, and dependencies.</t>
+  </si>
+  <si>
+    <t>This policy initiative installs the Azure Monitoring Agent (AMA) on the virtual machines scale sets (VMSS) and enables Azure Monitor for them. Azure Monitor collects and analyzes data from the VMs, such as performance metrics, logs, and dependencies.</t>
+  </si>
+  <si>
+    <t>This policy initiative installs the Azure Monitoring Agent (AMA) on Arc-enabled servers (Hybrid) and enables Azure Monitor for them. Azure Monitor collects and analyzes data from the VMs, such as performance metrics, logs, and dependencies.</t>
+  </si>
+  <si>
+    <t>With this policy initiative, you can enable automatic OS updates assessment every 24 hours. This is a custom initiative of built-in policies.</t>
+  </si>
+  <si>
+    <t>This policy initiative enables ChangeTracking and Inventory for virtual machines. It uses a Data Collection Rule to define what data to collect and where to send it, and a user-assigned identity to authenticate the Azure Monitor Agent.</t>
+  </si>
+  <si>
+    <t>This policy initiative enables ChangeTracking and Inventory for virtual machines scale sets. It uses a Data Collection Rule to define what data to collect and where to send it, and a user-assigned identity to authenticate the Azure Monitor Agent.</t>
+  </si>
+  <si>
+    <t>This policy initiative enables ChangeTracking and Inventory for Arc-enabled servers. It uses a Data Collection Rule to define what data to collect and where to send it, and a user-assigned identity to authenticate the Azure Monitor Agent.</t>
+  </si>
+  <si>
+    <t>This policy initiative enables Microsoft Defender for SQL and AMA on SQL VMs and Arc-enabled SQL Servers.</t>
+  </si>
+  <si>
+    <t>This policy enables you to specify the resource types that your organization can protect from accidentals deletion by blocking delete calls using deny action effect. Assigned to deny the deletion of the User Assignment Managed Identity that is used for AMA.</t>
+  </si>
+  <si>
+    <t>DenyAction</t>
+  </si>
+  <si>
+    <t>DINE-ChangeTrackingVMArcPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-ChangeTrackingVMPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-ChangeTrackingVMSSPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-VMHybridMonitoringPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DINE-MDFCDefenderSQLAMAPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>DENYACTION-ResourceDeletionPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>MODIFY-AUM-CheckUpdatesPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Configure SQL VMs and Arc-enabled SQL Servers to install Microsoft Defender for SQL and AMA with a user-defined LA workspace - de01d381-bae9-4670-8870-786f89f49e26 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for virtual machines - 92a36f05-ebc9-4bba-9128-b47ad2ea3354 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for virtual machine scale sets - c4a70814-96be-461c-889f-2b27429120dc (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>[Preview]: Enable ChangeTracking and Inventory for Arc-enabled virtual machines - 53448c70-089b-4f52-8f38-89196d7f2de1 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for VMs with Azure Monitoring Agent(AMA) - 924bfe3a-762f-40e7-86dd-5c8b95eb09e6 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for VMSS with Azure Monitoring Agent(AMA) - f5bf694c-cca7-4033-b883-3a23327d5485 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Enable Azure Monitor for Hybrid VMs with AMA - 2b00397d-c309-49c4-aa5a-f0b2c5bc6321 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines - Deploy-AUM-CheckUpdates (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Do not allow deletion of resource types - 78460a36-508a-49a4-b2b2-2f5ec564f4bb (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>2024-01-34</t>
   </si>
 </sst>
 </file>
@@ -790,7 +951,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -809,6 +970,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Corbel"/>
       <family val="2"/>
@@ -845,7 +1014,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -870,6 +1039,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1153,11 +1325,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
-  <dimension ref="A1:J51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
+  <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,7 +1348,7 @@
     <col min="11" max="16384" width="8.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1206,8 +1379,11 @@
       <c r="J1" s="9" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1239,7 +1415,7 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1271,79 +1447,85 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>246</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>247</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
+        <v>244</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="J4" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>258</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
+        <v>254</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>250</v>
       </c>
       <c r="J5" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -1352,30 +1534,30 @@
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J6" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1384,30 +1566,30 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>128</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>37</v>
+        <v>130</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="J7" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -1416,190 +1598,190 @@
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="J8" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>131</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>134</v>
+        <v>42</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="J9" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>148</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>43</v>
+        <v>167</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>206</v>
       </c>
       <c r="J10" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="J11" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J12" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J13" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
@@ -1608,115 +1790,116 @@
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>169</v>
+        <v>218</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>208</v>
+        <v>219</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="J14" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>220</v>
+        <v>239</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>240</v>
       </c>
       <c r="J15" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>240</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="I16" s="6"/>
       <c r="J16" s="5">
-        <v>45266</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+        <v>45427</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>242</v>
+        <v>149</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>242</v>
+        <v>149</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>241</v>
+        <v>150</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>244</v>
+        <v>152</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J17" s="5">
-        <v>45274</v>
+        <v>45124</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1724,10 +1907,10 @@
         <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -1736,19 +1919,17 @@
         <v>12</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>150</v>
+        <v>242</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>200</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="5">
-        <v>45124</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2492,31 +2673,29 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>203</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I42" s="4"/>
       <c r="J42" s="5">
-        <v>45018</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2524,10 +2703,2360 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="J43" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>227</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J44" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J45" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J46" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J47" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J48" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J49" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J50" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{CB9AA3F5-0FB5-4271-B843-BAC441E7FF28}"/>
+    <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{C1E76027-B2E2-46AE-8FBD-9F0D49770442}"/>
+    <hyperlink ref="I9" r:id="rId3" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{189AA603-D080-4747-8EE4-022DEBF70AC4}"/>
+    <hyperlink ref="I19" r:id="rId4" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{A326BBFF-13EF-4D72-866F-C82B6DB948CD}"/>
+    <hyperlink ref="I21" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{47846F9C-9BA5-4D50-BAC9-044A2B38522A}"/>
+    <hyperlink ref="I23" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{722CA2FF-9269-4E2F-8533-5ED7705D010E}"/>
+    <hyperlink ref="I25" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{137ED18D-F3D4-4225-915D-7618E3EB3F48}"/>
+    <hyperlink ref="I26" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{CFB3D49B-0E77-431E-8A4B-6A6C45FACD99}"/>
+    <hyperlink ref="I28" r:id="rId9" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{56989C35-212B-48D1-817B-986C70EFFD3A}"/>
+    <hyperlink ref="I30" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
+    <hyperlink ref="I31" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
+    <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
+    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
+    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{FB722C1D-B184-4DFC-8C0C-C02F60381DAC}"/>
+    <hyperlink ref="I35" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
+    <hyperlink ref="I37" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
+    <hyperlink ref="I38" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
+    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
+    <hyperlink ref="I40" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
+    <hyperlink ref="I45" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
+    <hyperlink ref="I46" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
+    <hyperlink ref="I7" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
+    <hyperlink ref="I8" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
+    <hyperlink ref="I47" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
+    <hyperlink ref="I3" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
+    <hyperlink ref="I41" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
+    <hyperlink ref="I51" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
+    <hyperlink ref="I52" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
+    <hyperlink ref="I43" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
+    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
+    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
+    <hyperlink ref="I29" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
+    <hyperlink ref="I24" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
+    <hyperlink ref="I13" r:id="rId34" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
+    <hyperlink ref="I12" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
+    <hyperlink ref="I11" r:id="rId36" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
+    <hyperlink ref="I10" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
+    <hyperlink ref="I36" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
+    <hyperlink ref="I17" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
+    <hyperlink ref="I14" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
+    <hyperlink ref="I20" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
+    <hyperlink ref="I22" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
+    <hyperlink ref="I27" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
+    <hyperlink ref="I15" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
+    <hyperlink ref="I4" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
+    <hyperlink ref="I5" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
+    <hyperlink ref="I59" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
+    <hyperlink ref="I56" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
+    <hyperlink ref="I57" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
+    <hyperlink ref="I58" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
+    <hyperlink ref="I53" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
+    <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
+    <hyperlink ref="I55" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
+    <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
+    <hyperlink ref="I60" r:id="rId55" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
+    <hyperlink ref="I68" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I65" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I66" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I67" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I62" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I63" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I64" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I69" r:id="rId63" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId64"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
+  <dimension ref="A1:K54"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="40.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="8.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="J4" s="5">
+        <v>45427</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J5" s="5">
+        <v>45427</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="J12" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="J13" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="J14" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J15" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="J16" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="J17" s="5">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5">
+        <v>45427</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J19" s="5">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J21" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="J22" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="J24" s="5">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J26" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="J29" s="5">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J30" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="J31" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J32" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J33" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J34" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J36" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J37" s="5">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="J38" s="5">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J39" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J40" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J41" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J42" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="C43" s="1" t="s">
-        <v>227</v>
+        <v>149</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -2536,30 +5065,30 @@
         <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>228</v>
+        <v>150</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>236</v>
+        <v>152</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J43" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>116</v>
+        <v>241</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>116</v>
+        <v>241</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2568,308 +5097,399 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>117</v>
+        <v>242</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>119</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I44" s="4"/>
       <c r="J44" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>123</v>
+        <v>160</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="J45" s="5">
-        <v>45018</v>
+        <v>45180</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>142</v>
+        <v>227</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>145</v>
+        <v>228</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>144</v>
+        <v>232</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>205</v>
+        <v>118</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J48" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J49" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J50" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F48" s="1" t="s">
+      <c r="D51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I48" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="J48" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J49" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="J50" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H51" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J52" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="J53" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I51" s="6" t="s">
+      <c r="I54" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="J51" s="5">
-        <v>45018</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J51" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:K1" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{1E792A8F-904D-4E2C-A2A1-C9B9C56A3F2E}"/>
-    <hyperlink ref="I4" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Diagnostics-LogAnalytics.html" xr:uid="{38B70A03-97DE-4A85-A9D2-5678F4BD941A}"/>
-    <hyperlink ref="I5" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
-    <hyperlink ref="I6" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
-    <hyperlink ref="I7" r:id="rId5" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
-    <hyperlink ref="I10" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
-    <hyperlink ref="I19" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
-    <hyperlink ref="I21" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
-    <hyperlink ref="I23" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
-    <hyperlink ref="I25" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
-    <hyperlink ref="I26" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
-    <hyperlink ref="I28" r:id="rId12" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
-    <hyperlink ref="I30" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
-    <hyperlink ref="I31" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
-    <hyperlink ref="I32" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
-    <hyperlink ref="I33" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
-    <hyperlink ref="I34" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
-    <hyperlink ref="I35" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
-    <hyperlink ref="I37" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
-    <hyperlink ref="I38" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
-    <hyperlink ref="I39" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
-    <hyperlink ref="I40" r:id="rId22" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
-    <hyperlink ref="I44" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
-    <hyperlink ref="I45" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
-    <hyperlink ref="I8" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
-    <hyperlink ref="I9" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
-    <hyperlink ref="I46" r:id="rId27" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
-    <hyperlink ref="I3" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
-    <hyperlink ref="I41" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
-    <hyperlink ref="I50" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
-    <hyperlink ref="I51" r:id="rId31" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
-    <hyperlink ref="I42" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
-    <hyperlink ref="I47" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
-    <hyperlink ref="I48" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
-    <hyperlink ref="I29" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
-    <hyperlink ref="I24" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
-    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
-    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
-    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
-    <hyperlink ref="I11" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
-    <hyperlink ref="I36" r:id="rId41" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
-    <hyperlink ref="I18" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
-    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
-    <hyperlink ref="I20" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
-    <hyperlink ref="I22" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
-    <hyperlink ref="I27" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
-    <hyperlink ref="I16" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
-    <hyperlink ref="I17" r:id="rId48" display="https://www.azadvertizer.net/azpolicyadvertizer/0a914e76-4921-4c19-b460-a2d36003525a.html" xr:uid="{25C8B460-23BD-4C40-8D4F-9A57005D6348}"/>
+    <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{403AA18B-DBF1-4AA8-B4DF-9A5213193E9E}"/>
+    <hyperlink ref="I7" r:id="rId3" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/55f3eceb-5573-4f18-9695-226972c6d74a.html" xr:uid="{E9FCCFC8-0866-4A69-A4C1-74DBFF026C02}"/>
+    <hyperlink ref="I8" r:id="rId4" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/75714362-cae7-409e-9b99-a8e5075b7fad.html" xr:uid="{90A3E47F-6544-4825-A92E-355DC51F2102}"/>
+    <hyperlink ref="I11" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{7EB2E1DD-2BDA-43B9-89BE-B1DD688DDA21}"/>
+    <hyperlink ref="I21" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{0E15A082-2100-4C94-B2B3-A2DBD039D90D}"/>
+    <hyperlink ref="I23" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{0C71907C-DC2D-4207-8711-A409E58035F7}"/>
+    <hyperlink ref="I25" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{00639D9E-C3D1-468A-A415-47E1D1507892}"/>
+    <hyperlink ref="I27" r:id="rId9" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{14EE5C0C-D9E5-44C3-A2EA-07C36CBCC29B}"/>
+    <hyperlink ref="I28" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{11DAA40F-DE93-4D53-B13F-972E3CBC0E21}"/>
+    <hyperlink ref="I30" r:id="rId11" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{4145E0EB-6E59-4438-9EFD-3B42F5603D1F}"/>
+    <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{A6F3A07C-9063-47ED-96CF-634796D19DBC}"/>
+    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{632EE935-0DED-429D-9BE7-C5F869098584}"/>
+    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{59FC50E9-9828-4CDB-B58D-09264C3C1ED2}"/>
+    <hyperlink ref="I35" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{11D87F25-B30A-4ECA-8ECA-D4BB6CC6D768}"/>
+    <hyperlink ref="I36" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{5109A5AD-2BA3-45E2-ABB7-0E1E8334E401}"/>
+    <hyperlink ref="I37" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{CCAFEBFB-B8BE-4E8D-A02E-A4F075DD0DDE}"/>
+    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{507C3B44-8D78-4BC6-B1C5-62EA657782D3}"/>
+    <hyperlink ref="I40" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{E244C58A-4EB2-4E2D-8418-065C4E16B529}"/>
+    <hyperlink ref="I41" r:id="rId20" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{1E897C18-8632-479E-90FC-451B42A5B29D}"/>
+    <hyperlink ref="I42" r:id="rId21" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{C71016D8-B201-4848-AC85-9D48F841D238}"/>
+    <hyperlink ref="I47" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{01D8B03B-FA5C-4577-BF30-6B55CA7E1040}"/>
+    <hyperlink ref="I48" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{01B5198C-AE56-402C-92FC-204EF38787EC}"/>
+    <hyperlink ref="I9" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{F1583D5B-0B1A-421A-8669-5E193C2B0A62}"/>
+    <hyperlink ref="I10" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{677229A1-87E2-444B-AAC3-AECB7304F02A}"/>
+    <hyperlink ref="I49" r:id="rId26" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{BBC65376-FBA3-49B9-8FF2-E8247761B04D}"/>
+    <hyperlink ref="I3" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{3D0372AC-17C9-4045-953A-23943EE58F77}"/>
+    <hyperlink ref="I43" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{D9760150-5B04-440C-B371-F5363C61A943}"/>
+    <hyperlink ref="I53" r:id="rId29" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{DC17459F-015B-4756-879A-98A9C6A709C6}"/>
+    <hyperlink ref="I54" r:id="rId30" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{6FF63B5B-8187-4AEB-8E79-93AA1CA872C5}"/>
+    <hyperlink ref="I45" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{F1B46FC3-20C0-4F79-B05A-2D7701021673}"/>
+    <hyperlink ref="I50" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FDAAF030-411B-41AB-BAC6-EF247712AAF4}"/>
+    <hyperlink ref="I51" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{9CA60505-94EF-4989-A68F-F0288A1F2143}"/>
+    <hyperlink ref="I31" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{5CDAF92A-F8EB-40CC-B0C3-259FACA4084E}"/>
+    <hyperlink ref="I26" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{9EC622FD-2C1D-40CD-A2F9-2A54FF78628B}"/>
+    <hyperlink ref="I15" r:id="rId36" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{827AF8B9-4257-4CD6-8CB9-17130EA44984}"/>
+    <hyperlink ref="I14" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{55A1A726-1009-4C39-B452-41E57E45A801}"/>
+    <hyperlink ref="I13" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{0ADD50A7-1865-4C03-B5BB-5C036F8CDCBE}"/>
+    <hyperlink ref="I12" r:id="rId39" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{2A106504-4142-4533-A6BD-AC59879B77CA}"/>
+    <hyperlink ref="I38" r:id="rId40" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{524C3A9E-8F2E-4C3D-B2B5-539B8C7F6A0B}"/>
+    <hyperlink ref="I19" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{A8345879-CC35-40F1-9DA8-86AC54A555C3}"/>
+    <hyperlink ref="I16" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{9AC28FEE-4C92-4159-8E45-DBB8E131C2DB}"/>
+    <hyperlink ref="I22" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{DE079C54-1429-45DC-9CF8-3ED4FA5A9360}"/>
+    <hyperlink ref="I24" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{879FD1F1-324E-4AF4-B2CB-6D0290E2AD34}"/>
+    <hyperlink ref="I29" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{B74624BF-BB9A-4BC5-8090-3082D6D21F24}"/>
+    <hyperlink ref="I17" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{0AFACD71-B22A-4AE8-9A67-860B1920587A}"/>
+    <hyperlink ref="I4" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{EAA9BFF3-4905-49C3-ABC1-9A75BCE68CB9}"/>
+    <hyperlink ref="I5" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{E8F3A9AD-20B7-4E98-9BA2-CF6D98053BF8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="A5" sqref="A5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3941,6 +6561,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4206,15 +6835,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
   <ds:schemaRefs>
@@ -4228,6 +6848,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4247,14 +6875,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>

</xml_diff>

<commit_message>
Update Display Name in spreadsheet
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53699783-BECB-4FCE-9D05-43241396CD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4926854-FDAD-4DB7-999E-DDEAE8AC1160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId1"/>
@@ -836,9 +836,6 @@
     <t>Enable Defender for SQL on SQL VMs and Arc-enabled SQL Servers</t>
   </si>
   <si>
-    <t>Do not allow deletion of resource types</t>
-  </si>
-  <si>
     <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines</t>
   </si>
   <si>
@@ -942,6 +939,9 @@
   </si>
   <si>
     <t>DENYACTION-DeleteUAMIAMAPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Do not allow deletion of specified resource and resource type</t>
   </si>
 </sst>
 </file>
@@ -1328,9 +1328,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3023,7 +3023,7 @@
         <v>29</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -3032,7 +3032,7 @@
         <v>24</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>14</v>
@@ -3041,10 +3041,10 @@
         <v>32</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>252</v>
@@ -3058,7 +3058,7 @@
         <v>34</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
@@ -3067,7 +3067,7 @@
         <v>24</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
@@ -3076,10 +3076,10 @@
         <v>36</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>252</v>
@@ -3093,7 +3093,7 @@
         <v>259</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -3102,19 +3102,19 @@
         <v>24</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>252</v>
@@ -3128,7 +3128,7 @@
         <v>260</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3137,19 +3137,19 @@
         <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>252</v>
@@ -3163,7 +3163,7 @@
         <v>261</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3172,19 +3172,19 @@
         <v>24</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>252</v>
@@ -3198,7 +3198,7 @@
         <v>262</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3207,19 +3207,19 @@
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>252</v>
@@ -3233,7 +3233,7 @@
         <v>263</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -3242,16 +3242,16 @@
         <v>24</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>252</v>
@@ -3262,10 +3262,10 @@
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>40</v>
@@ -3274,13 +3274,13 @@
         <v>12</v>
       </c>
       <c r="F60" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="I60" s="6"/>
       <c r="K60" s="1" t="s">
@@ -3292,10 +3292,10 @@
         <v>44</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -3304,19 +3304,19 @@
         <v>12</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I61" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J61" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>296</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>252</v>
@@ -3330,7 +3330,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
@@ -3339,7 +3339,7 @@
         <v>24</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>14</v>
@@ -3348,10 +3348,10 @@
         <v>32</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>252</v>
@@ -3365,7 +3365,7 @@
         <v>34</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -3374,7 +3374,7 @@
         <v>24</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>14</v>
@@ -3383,10 +3383,10 @@
         <v>36</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>252</v>
@@ -3400,7 +3400,7 @@
         <v>259</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
@@ -3409,19 +3409,19 @@
         <v>24</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>252</v>
@@ -3435,7 +3435,7 @@
         <v>260</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3444,19 +3444,19 @@
         <v>24</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>252</v>
@@ -3470,7 +3470,7 @@
         <v>261</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3479,19 +3479,19 @@
         <v>24</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>252</v>
@@ -3505,7 +3505,7 @@
         <v>262</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3514,19 +3514,19 @@
         <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>252</v>
@@ -3540,7 +3540,7 @@
         <v>263</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -3549,16 +3549,16 @@
         <v>24</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>252</v>
@@ -3569,10 +3569,10 @@
         <v>72</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -3581,19 +3581,19 @@
         <v>12</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I69" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J69" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>296</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>252</v>
@@ -6545,6 +6545,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6810,29 +6832,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6852,26 +6872,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
New custom policy DenyAction Delete UAMI used by AMA (#1662)
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
Co-authored-by: Sacha Narinx <Springstone@users.noreply.github.com>
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC9EA86-D637-4C62-8A9D-9DB71A1B5220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4926854-FDAD-4DB7-999E-DDEAE8AC1160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1453" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="300">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -836,9 +836,6 @@
     <t>Enable Defender for SQL on SQL VMs and Arc-enabled SQL Servers</t>
   </si>
   <si>
-    <t>Do not allow deletion of resource types</t>
-  </si>
-  <si>
     <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines</t>
   </si>
   <si>
@@ -887,9 +884,6 @@
     <t>This policy initiative enables Microsoft Defender for SQL and AMA on SQL VMs and Arc-enabled SQL Servers.</t>
   </si>
   <si>
-    <t>This policy enables you to specify the resource types that your organization can protect from accidentals deletion by blocking delete calls using deny action effect. Assigned to deny the deletion of the User Assignment Managed Identity that is used for AMA.</t>
-  </si>
-  <si>
     <t>DenyAction</t>
   </si>
   <si>
@@ -908,9 +902,6 @@
     <t>DINE-MDFCDefenderSQLAMAPolicyAssignment.json</t>
   </si>
   <si>
-    <t>DENYACTION-ResourceDeletionPolicyAssignment.json</t>
-  </si>
-  <si>
     <t>MODIFY-AUM-CheckUpdatesPolicyAssignment.json</t>
   </si>
   <si>
@@ -938,10 +929,19 @@
     <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines - Deploy-AUM-CheckUpdates (azadvertizer.net)</t>
   </si>
   <si>
-    <t>Do not allow deletion of resource types - 78460a36-508a-49a4-b2b2-2f5ec564f4bb (azadvertizer.net)</t>
-  </si>
-  <si>
     <t>2024-01-34</t>
+  </si>
+  <si>
+    <t>Do not allow deletion of the User Assigned Managed Identity used by AMA</t>
+  </si>
+  <si>
+    <t>This policy provides a safeguard against accidental removal of the User Assigned Managed Identity used by AMA by blocking delete calls using deny action effect.</t>
+  </si>
+  <si>
+    <t>DENYACTION-DeleteUAMIAMAPolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>Do not allow deletion of specified resource and resource type</t>
   </si>
 </sst>
 </file>
@@ -1328,9 +1328,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3023,7 +3023,7 @@
         <v>29</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -3032,7 +3032,7 @@
         <v>24</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>14</v>
@@ -3041,10 +3041,10 @@
         <v>32</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>252</v>
@@ -3058,7 +3058,7 @@
         <v>34</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
@@ -3067,7 +3067,7 @@
         <v>24</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
@@ -3076,10 +3076,10 @@
         <v>36</v>
       </c>
       <c r="I54" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>252</v>
@@ -3093,7 +3093,7 @@
         <v>259</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -3102,19 +3102,19 @@
         <v>24</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>252</v>
@@ -3128,7 +3128,7 @@
         <v>260</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3137,19 +3137,19 @@
         <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>252</v>
@@ -3163,7 +3163,7 @@
         <v>261</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3172,19 +3172,19 @@
         <v>24</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>252</v>
@@ -3198,7 +3198,7 @@
         <v>262</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3207,19 +3207,19 @@
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>252</v>
@@ -3233,7 +3233,7 @@
         <v>263</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -3242,49 +3242,47 @@
         <v>24</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H59" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I59" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="I59" s="6" t="s">
-        <v>290</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>264</v>
+        <v>296</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="I60" s="6" t="s">
         <v>298</v>
       </c>
+      <c r="I60" s="6"/>
       <c r="K60" s="1" t="s">
         <v>252</v>
       </c>
@@ -3294,10 +3292,10 @@
         <v>44</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
@@ -3306,19 +3304,19 @@
         <v>12</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>252</v>
@@ -3332,7 +3330,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
@@ -3341,7 +3339,7 @@
         <v>24</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>14</v>
@@ -3350,10 +3348,10 @@
         <v>32</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>252</v>
@@ -3367,7 +3365,7 @@
         <v>34</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -3376,7 +3374,7 @@
         <v>24</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>14</v>
@@ -3385,10 +3383,10 @@
         <v>36</v>
       </c>
       <c r="I63" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J63" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>252</v>
@@ -3402,7 +3400,7 @@
         <v>259</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
@@ -3411,19 +3409,19 @@
         <v>24</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>252</v>
@@ -3437,7 +3435,7 @@
         <v>260</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3446,19 +3444,19 @@
         <v>24</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>252</v>
@@ -3472,7 +3470,7 @@
         <v>261</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3481,19 +3479,19 @@
         <v>24</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>252</v>
@@ -3507,7 +3505,7 @@
         <v>262</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3516,19 +3514,19 @@
         <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>252</v>
@@ -3542,7 +3540,7 @@
         <v>263</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -3551,16 +3549,16 @@
         <v>24</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H68" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I68" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>290</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>252</v>
@@ -3571,10 +3569,10 @@
         <v>72</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -3583,19 +3581,19 @@
         <v>12</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>252</v>
@@ -3658,18 +3656,17 @@
     <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
     <hyperlink ref="I55" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
     <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
-    <hyperlink ref="I60" r:id="rId55" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
-    <hyperlink ref="I68" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
-    <hyperlink ref="I65" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
-    <hyperlink ref="I66" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
-    <hyperlink ref="I67" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
-    <hyperlink ref="I62" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
-    <hyperlink ref="I63" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
-    <hyperlink ref="I64" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
-    <hyperlink ref="I69" r:id="rId63" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I68" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I65" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I66" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I67" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I62" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I63" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I64" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I69" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId64"/>
+  <pageSetup orientation="portrait" r:id="rId63"/>
 </worksheet>
 </file>
 
@@ -6877,6 +6874,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update policy count in ALZ-Policies.md
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4926854-FDAD-4DB7-999E-DDEAE8AC1160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CA70F0-7F56-407C-9E6E-5728E0D091B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="29016" windowHeight="18696" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="300">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -1326,11 +1326,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2385,10 +2385,10 @@
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2397,30 +2397,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2429,30 +2429,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>94</v>
+        <v>213</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="J34" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>211</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2461,30 +2461,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>98</v>
+        <v>212</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J35" s="5">
         <v>45084</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2493,30 +2493,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>212</v>
+        <v>102</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>214</v>
+        <v>50</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="J36" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2525,30 +2525,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="J37" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2557,30 +2557,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2589,48 +2589,48 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>114</v>
+        <v>152</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
@@ -2641,10 +2641,10 @@
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -2653,19 +2653,17 @@
         <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>150</v>
+        <v>242</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>200</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I41" s="4"/>
       <c r="J41" s="5">
-        <v>45018</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2673,29 +2671,31 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>158</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>241</v>
+        <v>158</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>242</v>
+        <v>159</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I42" s="4"/>
+        <v>160</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>203</v>
+      </c>
       <c r="J42" s="5">
-        <v>45363</v>
+        <v>45180</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2703,42 +2703,42 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>227</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>159</v>
+        <v>228</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>160</v>
+        <v>232</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>203</v>
+        <v>236</v>
       </c>
       <c r="J43" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>227</v>
+        <v>116</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>116</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2747,30 +2747,30 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>228</v>
+        <v>117</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>236</v>
+        <v>118</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J44" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
@@ -2779,62 +2779,62 @@
         <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="J45" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>123</v>
+        <v>146</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>143</v>
+        <v>204</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>40</v>
@@ -2843,30 +2843,30 @@
         <v>24</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>144</v>
+        <v>154</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>204</v>
+        <v>155</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>204</v>
+        <v>155</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>40</v>
@@ -2875,94 +2875,94 @@
         <v>24</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>205</v>
+        <v>157</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>206</v>
+        <v>45</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>124</v>
+        <v>215</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>45</v>
+        <v>138</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="J50" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -2971,48 +2971,51 @@
         <v>12</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="J51" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>216</v>
+        <v>44</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>139</v>
+        <v>29</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>139</v>
+        <v>265</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>140</v>
+        <v>272</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>202</v>
+        <v>291</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -3020,10 +3023,10 @@
         <v>44</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -3032,16 +3035,16 @@
         <v>24</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>295</v>
@@ -3055,10 +3058,10 @@
         <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>34</v>
+        <v>259</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
@@ -3067,16 +3070,16 @@
         <v>24</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>36</v>
+        <v>284</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="J54" s="5" t="s">
         <v>295</v>
@@ -3090,10 +3093,10 @@
         <v>44</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -3102,16 +3105,16 @@
         <v>24</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>295</v>
@@ -3125,10 +3128,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3137,16 +3140,16 @@
         <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J56" s="5" t="s">
         <v>295</v>
@@ -3160,10 +3163,10 @@
         <v>44</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3172,16 +3175,16 @@
         <v>24</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J57" s="5" t="s">
         <v>295</v>
@@ -3190,15 +3193,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3207,52 +3210,47 @@
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>263</v>
+        <v>296</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>279</v>
+        <v>297</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>14</v>
+        <v>280</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I59" s="6" t="s">
-        <v>287</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="I59" s="6"/>
       <c r="K59" s="1" t="s">
         <v>252</v>
       </c>
@@ -3262,58 +3260,63 @@
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>280</v>
+        <v>49</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="I60" s="6"/>
+        <v>286</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>295</v>
+      </c>
       <c r="K60" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>264</v>
+        <v>29</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>295</v>
@@ -3327,10 +3330,10 @@
         <v>72</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
@@ -3339,16 +3342,16 @@
         <v>24</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J62" s="5" t="s">
         <v>295</v>
@@ -3362,10 +3365,10 @@
         <v>72</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>34</v>
+        <v>259</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -3374,16 +3377,16 @@
         <v>24</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>36</v>
+        <v>284</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="J63" s="5" t="s">
         <v>295</v>
@@ -3397,10 +3400,10 @@
         <v>72</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
@@ -3409,16 +3412,16 @@
         <v>24</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="J64" s="5" t="s">
         <v>295</v>
@@ -3432,10 +3435,10 @@
         <v>72</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3444,16 +3447,16 @@
         <v>24</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J65" s="5" t="s">
         <v>295</v>
@@ -3467,10 +3470,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3479,16 +3482,16 @@
         <v>24</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>295</v>
@@ -3497,15 +3500,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3514,88 +3517,53 @@
         <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>287</v>
+        <v>294</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>295</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="I69" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K69" s="1" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3614,59 +3582,58 @@
     <hyperlink ref="I30" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
     <hyperlink ref="I31" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
     <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
-    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
-    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{FB722C1D-B184-4DFC-8C0C-C02F60381DAC}"/>
-    <hyperlink ref="I35" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
-    <hyperlink ref="I37" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
-    <hyperlink ref="I38" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
-    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
-    <hyperlink ref="I40" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
-    <hyperlink ref="I45" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
-    <hyperlink ref="I46" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
-    <hyperlink ref="I7" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
-    <hyperlink ref="I8" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
-    <hyperlink ref="I47" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
-    <hyperlink ref="I3" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
-    <hyperlink ref="I41" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
-    <hyperlink ref="I51" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
-    <hyperlink ref="I52" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
-    <hyperlink ref="I43" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
-    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
-    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
-    <hyperlink ref="I29" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
-    <hyperlink ref="I24" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
-    <hyperlink ref="I13" r:id="rId34" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
-    <hyperlink ref="I12" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
-    <hyperlink ref="I11" r:id="rId36" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
-    <hyperlink ref="I10" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
-    <hyperlink ref="I36" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
-    <hyperlink ref="I17" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
-    <hyperlink ref="I14" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
-    <hyperlink ref="I20" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
-    <hyperlink ref="I22" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
-    <hyperlink ref="I27" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
-    <hyperlink ref="I15" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
-    <hyperlink ref="I4" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
-    <hyperlink ref="I5" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
-    <hyperlink ref="I59" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
-    <hyperlink ref="I56" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
-    <hyperlink ref="I57" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
-    <hyperlink ref="I58" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
-    <hyperlink ref="I53" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
-    <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
-    <hyperlink ref="I55" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
-    <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
-    <hyperlink ref="I68" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
-    <hyperlink ref="I65" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
-    <hyperlink ref="I66" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
-    <hyperlink ref="I67" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
-    <hyperlink ref="I62" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
-    <hyperlink ref="I63" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
-    <hyperlink ref="I64" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
-    <hyperlink ref="I69" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{FB722C1D-B184-4DFC-8C0C-C02F60381DAC}"/>
+    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
+    <hyperlink ref="I36" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
+    <hyperlink ref="I37" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
+    <hyperlink ref="I38" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
+    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
+    <hyperlink ref="I44" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
+    <hyperlink ref="I45" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
+    <hyperlink ref="I7" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
+    <hyperlink ref="I8" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
+    <hyperlink ref="I46" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
+    <hyperlink ref="I3" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
+    <hyperlink ref="I40" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
+    <hyperlink ref="I50" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
+    <hyperlink ref="I51" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
+    <hyperlink ref="I42" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
+    <hyperlink ref="I47" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
+    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
+    <hyperlink ref="I29" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
+    <hyperlink ref="I24" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
+    <hyperlink ref="I13" r:id="rId33" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
+    <hyperlink ref="I12" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
+    <hyperlink ref="I11" r:id="rId35" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
+    <hyperlink ref="I10" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
+    <hyperlink ref="I35" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
+    <hyperlink ref="I17" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
+    <hyperlink ref="I14" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
+    <hyperlink ref="I20" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
+    <hyperlink ref="I22" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
+    <hyperlink ref="I27" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
+    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
+    <hyperlink ref="I4" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
+    <hyperlink ref="I5" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
+    <hyperlink ref="I58" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
+    <hyperlink ref="I55" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
+    <hyperlink ref="I56" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
+    <hyperlink ref="I57" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
+    <hyperlink ref="I52" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
+    <hyperlink ref="I53" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
+    <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
+    <hyperlink ref="I60" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
+    <hyperlink ref="I67" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I64" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I65" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I66" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I61" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I62" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I63" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I68" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId63"/>
+  <pageSetup orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
 
@@ -6545,28 +6512,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6832,27 +6777,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6872,6 +6819,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Remove duplicate assignment and portal option for Azure Policy Add-on… (#1710)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4926854-FDAD-4DB7-999E-DDEAE8AC1160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CA70F0-7F56-407C-9E6E-5728E0D091B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="29016" windowHeight="18696" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="300">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -1326,11 +1326,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2385,10 +2385,10 @@
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2397,30 +2397,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2429,30 +2429,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>94</v>
+        <v>213</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="J34" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>211</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>211</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2461,30 +2461,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>98</v>
+        <v>212</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J35" s="5">
         <v>45084</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>47</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2493,30 +2493,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>212</v>
+        <v>102</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>214</v>
+        <v>50</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="J36" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2525,30 +2525,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="J37" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2557,30 +2557,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2589,48 +2589,48 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>114</v>
+        <v>152</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
@@ -2641,10 +2641,10 @@
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>241</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -2653,19 +2653,17 @@
         <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>150</v>
+        <v>242</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>151</v>
+        <v>84</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>200</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I41" s="4"/>
       <c r="J41" s="5">
-        <v>45018</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2673,29 +2671,31 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>158</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>241</v>
+        <v>158</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>242</v>
+        <v>159</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I42" s="4"/>
+        <v>160</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>203</v>
+      </c>
       <c r="J42" s="5">
-        <v>45363</v>
+        <v>45180</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2703,42 +2703,42 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>227</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>159</v>
+        <v>228</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>160</v>
+        <v>232</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>203</v>
+        <v>236</v>
       </c>
       <c r="J43" s="5">
-        <v>45180</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>227</v>
+        <v>116</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>116</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2747,30 +2747,30 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>228</v>
+        <v>117</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>236</v>
+        <v>118</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J44" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
@@ -2779,62 +2779,62 @@
         <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="J45" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>123</v>
+        <v>146</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>204</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>143</v>
+        <v>204</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>40</v>
@@ -2843,30 +2843,30 @@
         <v>24</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>144</v>
+        <v>154</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>204</v>
+        <v>155</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>204</v>
+        <v>155</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>40</v>
@@ -2875,94 +2875,94 @@
         <v>24</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>205</v>
+        <v>157</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>206</v>
+        <v>45</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>124</v>
+        <v>215</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>45</v>
+        <v>138</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="J50" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>11</v>
@@ -2971,48 +2971,51 @@
         <v>12</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="J51" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>216</v>
+        <v>44</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>139</v>
+        <v>29</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>139</v>
+        <v>265</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>140</v>
+        <v>272</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>202</v>
+        <v>291</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -3020,10 +3023,10 @@
         <v>44</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
@@ -3032,16 +3035,16 @@
         <v>24</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>295</v>
@@ -3055,10 +3058,10 @@
         <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>34</v>
+        <v>259</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
@@ -3067,16 +3070,16 @@
         <v>24</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>36</v>
+        <v>284</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="J54" s="5" t="s">
         <v>295</v>
@@ -3090,10 +3093,10 @@
         <v>44</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -3102,16 +3105,16 @@
         <v>24</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="J55" s="5" t="s">
         <v>295</v>
@@ -3125,10 +3128,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3137,16 +3140,16 @@
         <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J56" s="5" t="s">
         <v>295</v>
@@ -3160,10 +3163,10 @@
         <v>44</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3172,16 +3175,16 @@
         <v>24</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J57" s="5" t="s">
         <v>295</v>
@@ -3190,15 +3193,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3207,52 +3210,47 @@
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>263</v>
+        <v>296</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>271</v>
+        <v>299</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>279</v>
+        <v>297</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>14</v>
+        <v>280</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="I59" s="6" t="s">
-        <v>287</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="I59" s="6"/>
       <c r="K59" s="1" t="s">
         <v>252</v>
       </c>
@@ -3262,58 +3260,63 @@
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>280</v>
+        <v>49</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="I60" s="6"/>
+        <v>286</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>295</v>
+      </c>
       <c r="K60" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>264</v>
+        <v>29</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>295</v>
@@ -3327,10 +3330,10 @@
         <v>72</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
@@ -3339,16 +3342,16 @@
         <v>24</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J62" s="5" t="s">
         <v>295</v>
@@ -3362,10 +3365,10 @@
         <v>72</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>34</v>
+        <v>259</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -3374,16 +3377,16 @@
         <v>24</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>36</v>
+        <v>284</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="J63" s="5" t="s">
         <v>295</v>
@@ -3397,10 +3400,10 @@
         <v>72</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
@@ -3409,16 +3412,16 @@
         <v>24</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="J64" s="5" t="s">
         <v>295</v>
@@ -3432,10 +3435,10 @@
         <v>72</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3444,16 +3447,16 @@
         <v>24</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="J65" s="5" t="s">
         <v>295</v>
@@ -3467,10 +3470,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3479,16 +3482,16 @@
         <v>24</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>295</v>
@@ -3497,15 +3500,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3514,88 +3517,53 @@
         <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>287</v>
+        <v>294</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>295</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="I69" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K69" s="1" t="s">
         <v>252</v>
       </c>
     </row>
@@ -3614,59 +3582,58 @@
     <hyperlink ref="I30" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
     <hyperlink ref="I31" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
     <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
-    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
-    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{FB722C1D-B184-4DFC-8C0C-C02F60381DAC}"/>
-    <hyperlink ref="I35" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
-    <hyperlink ref="I37" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
-    <hyperlink ref="I38" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
-    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
-    <hyperlink ref="I40" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
-    <hyperlink ref="I45" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
-    <hyperlink ref="I46" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
-    <hyperlink ref="I7" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
-    <hyperlink ref="I8" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
-    <hyperlink ref="I47" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
-    <hyperlink ref="I3" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
-    <hyperlink ref="I41" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
-    <hyperlink ref="I51" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
-    <hyperlink ref="I52" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
-    <hyperlink ref="I43" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
-    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
-    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
-    <hyperlink ref="I29" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
-    <hyperlink ref="I24" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
-    <hyperlink ref="I13" r:id="rId34" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
-    <hyperlink ref="I12" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
-    <hyperlink ref="I11" r:id="rId36" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
-    <hyperlink ref="I10" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
-    <hyperlink ref="I36" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
-    <hyperlink ref="I17" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
-    <hyperlink ref="I14" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
-    <hyperlink ref="I20" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
-    <hyperlink ref="I22" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
-    <hyperlink ref="I27" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
-    <hyperlink ref="I15" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
-    <hyperlink ref="I4" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
-    <hyperlink ref="I5" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
-    <hyperlink ref="I59" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
-    <hyperlink ref="I56" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
-    <hyperlink ref="I57" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
-    <hyperlink ref="I58" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
-    <hyperlink ref="I53" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
-    <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
-    <hyperlink ref="I55" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
-    <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
-    <hyperlink ref="I68" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
-    <hyperlink ref="I65" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
-    <hyperlink ref="I66" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
-    <hyperlink ref="I67" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
-    <hyperlink ref="I62" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
-    <hyperlink ref="I63" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
-    <hyperlink ref="I64" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
-    <hyperlink ref="I69" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{FB722C1D-B184-4DFC-8C0C-C02F60381DAC}"/>
+    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
+    <hyperlink ref="I36" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
+    <hyperlink ref="I37" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
+    <hyperlink ref="I38" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
+    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
+    <hyperlink ref="I44" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
+    <hyperlink ref="I45" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
+    <hyperlink ref="I7" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
+    <hyperlink ref="I8" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
+    <hyperlink ref="I46" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
+    <hyperlink ref="I3" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
+    <hyperlink ref="I40" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
+    <hyperlink ref="I50" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
+    <hyperlink ref="I51" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
+    <hyperlink ref="I42" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
+    <hyperlink ref="I47" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
+    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
+    <hyperlink ref="I29" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
+    <hyperlink ref="I24" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
+    <hyperlink ref="I13" r:id="rId33" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
+    <hyperlink ref="I12" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
+    <hyperlink ref="I11" r:id="rId35" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
+    <hyperlink ref="I10" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
+    <hyperlink ref="I35" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
+    <hyperlink ref="I17" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
+    <hyperlink ref="I14" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
+    <hyperlink ref="I20" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
+    <hyperlink ref="I22" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
+    <hyperlink ref="I27" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
+    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
+    <hyperlink ref="I4" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
+    <hyperlink ref="I5" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
+    <hyperlink ref="I58" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
+    <hyperlink ref="I55" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
+    <hyperlink ref="I56" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
+    <hyperlink ref="I57" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
+    <hyperlink ref="I52" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
+    <hyperlink ref="I53" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
+    <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
+    <hyperlink ref="I60" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
+    <hyperlink ref="I67" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I64" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I65" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I66" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I61" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I62" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I63" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I68" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId63"/>
+  <pageSetup orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
 
@@ -6545,28 +6512,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6832,27 +6777,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6872,6 +6819,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Policy Excel updates (#1715)
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -5,21 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CA70F0-7F56-407C-9E6E-5728E0D091B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679EC49-138E-4518-8A26-2D088C4FAE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="29016" windowHeight="18696" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId1"/>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId2"/>
-    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId3"/>
+    <sheet name="Overview" sheetId="8" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId2"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$70</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="310">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -836,6 +837,9 @@
     <t>Enable Defender for SQL on SQL VMs and Arc-enabled SQL Servers</t>
   </si>
   <si>
+    <t>Do not allow deletion of resource types</t>
+  </si>
+  <si>
     <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines</t>
   </si>
   <si>
@@ -884,6 +888,9 @@
     <t>This policy initiative enables Microsoft Defender for SQL and AMA on SQL VMs and Arc-enabled SQL Servers.</t>
   </si>
   <si>
+    <t>This policy enables you to specify the resource types that your organization can protect from accidentals deletion by blocking delete calls using deny action effect. Assigned to deny the deletion of the User Assignment Managed Identity that is used for AMA.</t>
+  </si>
+  <si>
     <t>DenyAction</t>
   </si>
   <si>
@@ -902,6 +909,9 @@
     <t>DINE-MDFCDefenderSQLAMAPolicyAssignment.json</t>
   </si>
   <si>
+    <t>DENYACTION-ResourceDeletionPolicyAssignment.json</t>
+  </si>
+  <si>
     <t>MODIFY-AUM-CheckUpdatesPolicyAssignment.json</t>
   </si>
   <si>
@@ -929,19 +939,40 @@
     <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines - Deploy-AUM-CheckUpdates (azadvertizer.net)</t>
   </si>
   <si>
-    <t>2024-01-34</t>
-  </si>
-  <si>
-    <t>Do not allow deletion of the User Assigned Managed Identity used by AMA</t>
-  </si>
-  <si>
-    <t>This policy provides a safeguard against accidental removal of the User Assigned Managed Identity used by AMA by blocking delete calls using deny action effect.</t>
-  </si>
-  <si>
-    <t>DENYACTION-DeleteUAMIAMAPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>Do not allow deletion of specified resource and resource type</t>
+    <t>Do not allow deletion of resource types - 78460a36-508a-49a4-b2b2-2f5ec564f4bb (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deny virtual machines and virtual machine scale sets that do not use managed disk</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud Security Benchmark</t>
+  </si>
+  <si>
+    <t>Configure SQL servers to have auditing enabled to Log Analytics workspace - 25da7dfb-0666-4a15-a8f5-402127efd8bb (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Configure SQL servers to have auditing enabled to Log Analytics workspace</t>
+  </si>
+  <si>
+    <t>To ensure the operations performed against your SQL assets are captured, SQL servers should have auditing enabled. If auditing is not enabled, this policy will configure auditing events to flow to the specified Log Analytics workspace.</t>
+  </si>
+  <si>
+    <t>Enforce backup for all virtual machines by deploying a recovery services vault in the same location and resource group as the virtual machine. Doing this is useful when different application teams in your organization are allocated separate resource groups and need to manage their own backups and restores. You can optionally exclude virtual machines containing a specified tag to control the scope of assignment. See https://aka.ms/AzureVMAppCentricBackupExcludeTag.</t>
+  </si>
+  <si>
+    <t>Configure backup on virtual machines without a given tag to a new recovery services vault with a default policy - 98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Quick links to ALZ Policies and Initiatives:</t>
+  </si>
+  <si>
+    <t>ALZ Initiatives (AzAdvertizer)</t>
+  </si>
+  <si>
+    <t>ALZ Policies (AzAdvertizer)</t>
+  </si>
+  <si>
+    <t>ALZ Policies (GitHub)</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1045,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1044,6 +1075,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1060,6 +1092,138 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57C42FFB-0C15-3558-BD31-1C4590C92C51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="167640" y="182880"/>
+          <a:ext cx="7048500" cy="3223260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1600" b="1"/>
+            <a:t>Notes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AE" sz="1600" b="1"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t> document includes Azure Landing Zone (ALZ) default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="1" baseline="0"/>
+            <a:t>assignments</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t>, not the exhaustive list of custom policies that ALZ provides. Default assignments are those made without changing any options in the portal accelerator and keeping all the "Yes" options as is. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0"/>
+            <a:t>What is not included are the optional policies and initiatives</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t> that ALZ does not assign by default, for example, "Workload Specific Compliance" initiatives.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t>For the complete list of ALZ initiatives and policies please use https://www.azadvertizer.net and use the filters to select "ALZ" policies/initiatives, or use the quick links below.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0"/>
+            <a:t>While</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t> we make every effort to keep this document up-to-date, it is challenging keeping a binary updated outside our normal GitHub processes. For the most up-to-date version please review ALZ Policies on GitHub (link below)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AE" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1325,12 +1489,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
-  <dimension ref="A1:K68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FFA7FA-CF8D-416B-AD3C-43815126868D}">
+  <dimension ref="B20:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33:XFD33"/>
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B21" r:id="rId1" location="%7B%22col_8%22%3A%7B%22flt%22%3A%22ALZ%22%7D%7D" display="ALZ Initiatives" xr:uid="{DBFEFF67-2F59-430A-9C74-2F9C44BB7FF7}"/>
+    <hyperlink ref="B22" r:id="rId2" display="ALZ Policies" xr:uid="{3710756B-881D-4F79-B7FB-86E68C96AF9B}"/>
+    <hyperlink ref="B23" r:id="rId3" xr:uid="{08074762-F5B3-4CF0-9C48-937CB547FB81}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
+  <dimension ref="A1:K70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1730,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>300</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>
@@ -1714,7 +1922,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>163</v>
@@ -2385,10 +2593,10 @@
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2397,30 +2605,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>96</v>
+        <v>302</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>97</v>
+        <v>302</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2429,30 +2637,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>98</v>
+        <v>303</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>301</v>
       </c>
       <c r="J34" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>211</v>
+        <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2461,30 +2669,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>212</v>
+        <v>98</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="J35" s="5">
         <v>45084</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2493,30 +2701,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>51</v>
+        <v>99</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J36" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2525,30 +2733,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="J37" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2557,30 +2765,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2589,48 +2797,48 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>200</v>
+        <v>113</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
@@ -2641,10 +2849,10 @@
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>11</v>
@@ -2653,17 +2861,19 @@
         <v>12</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>242</v>
+        <v>150</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I41" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="J41" s="5">
-        <v>45363</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2671,31 +2881,29 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I42" s="6" t="s">
-        <v>203</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I42" s="4"/>
       <c r="J42" s="5">
-        <v>45180</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2703,42 +2911,42 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="J43" s="5">
-        <v>45018</v>
+        <v>45180</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>11</v>
@@ -2747,48 +2955,48 @@
         <v>12</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>119</v>
+        <v>232</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="J44" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>121</v>
+        <v>304</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>123</v>
+        <v>70</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>305</v>
       </c>
       <c r="J45" s="5">
         <v>45018</v>
@@ -2799,60 +3007,60 @@
         <v>115</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>205</v>
+        <v>122</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J47" s="5">
         <v>45018</v>
@@ -2863,10 +3071,10 @@
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>40</v>
@@ -2875,182 +3083,176 @@
         <v>24</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J48" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J49" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I50" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="J48" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="J50" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J49" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="J50" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>202</v>
+      <c r="J51" s="5">
+        <v>45018</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>265</v>
+        <v>135</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>272</v>
+        <v>136</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="J52" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>266</v>
+        <v>139</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>273</v>
+        <v>140</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>36</v>
+        <v>141</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -3058,10 +3260,10 @@
         <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>259</v>
+        <v>29</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
@@ -3070,19 +3272,19 @@
         <v>24</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>284</v>
+        <v>32</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="J54" s="5">
+        <v>45322</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>252</v>
@@ -3093,10 +3295,10 @@
         <v>44</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>260</v>
+        <v>34</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
@@ -3105,19 +3307,19 @@
         <v>24</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="J55" s="5" t="s">
         <v>295</v>
+      </c>
+      <c r="J55" s="5">
+        <v>45322</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>252</v>
@@ -3128,10 +3330,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3140,19 +3342,19 @@
         <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
+      </c>
+      <c r="J56" s="5">
+        <v>45322</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>252</v>
@@ -3163,10 +3365,10 @@
         <v>44</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3175,33 +3377,33 @@
         <v>24</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
+      </c>
+      <c r="J57" s="5">
+        <v>45322</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3210,7 +3412,7 @@
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
@@ -3219,72 +3421,80 @@
         <v>285</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>287</v>
+        <v>292</v>
+      </c>
+      <c r="J58" s="5">
+        <v>45322</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>296</v>
+        <v>262</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>280</v>
+        <v>14</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="I59" s="6"/>
+        <v>283</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="J59" s="5">
+        <v>45322</v>
+      </c>
       <c r="K59" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="J60" s="5" t="s">
-        <v>295</v>
+        <v>290</v>
+      </c>
+      <c r="J60" s="5">
+        <v>45322</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>252</v>
@@ -3292,69 +3502,69 @@
     </row>
     <row r="61" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>29</v>
+        <v>264</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>14</v>
+        <v>282</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>32</v>
+        <v>288</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>295</v>
+        <v>298</v>
+      </c>
+      <c r="J61" s="5">
+        <v>45322</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>34</v>
+        <v>265</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>36</v>
+        <v>289</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>295</v>
+        <v>297</v>
+      </c>
+      <c r="J62" s="5">
+        <v>45322</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>252</v>
@@ -3365,10 +3575,10 @@
         <v>72</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>259</v>
+        <v>29</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>11</v>
@@ -3377,19 +3587,19 @@
         <v>24</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>284</v>
+        <v>32</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="J63" s="5">
+        <v>45322</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>252</v>
@@ -3400,10 +3610,10 @@
         <v>72</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>260</v>
+        <v>34</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
@@ -3412,19 +3622,19 @@
         <v>24</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="J64" s="5" t="s">
         <v>295</v>
+      </c>
+      <c r="J64" s="5">
+        <v>45322</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>252</v>
@@ -3435,10 +3645,10 @@
         <v>72</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3447,19 +3657,19 @@
         <v>24</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
+      </c>
+      <c r="J65" s="5">
+        <v>45322</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>252</v>
@@ -3470,10 +3680,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3482,33 +3692,33 @@
         <v>24</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J66" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
+      </c>
+      <c r="J66" s="5">
+        <v>45322</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3517,7 +3727,7 @@
         <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
@@ -3526,49 +3736,122 @@
         <v>285</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>287</v>
+        <v>292</v>
+      </c>
+      <c r="J67" s="5">
+        <v>45322</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="J68" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
+      </c>
+      <c r="J68" s="5">
+        <v>45322</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>252</v>
       </c>
     </row>
+    <row r="69" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J69" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J70" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:K70" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{CB9AA3F5-0FB5-4271-B843-BAC441E7FF28}"/>
     <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{C1E76027-B2E2-46AE-8FBD-9F0D49770442}"/>
@@ -3582,31 +3865,31 @@
     <hyperlink ref="I30" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
     <hyperlink ref="I31" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
     <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
-    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{FB722C1D-B184-4DFC-8C0C-C02F60381DAC}"/>
-    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
-    <hyperlink ref="I36" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
-    <hyperlink ref="I37" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
-    <hyperlink ref="I38" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
-    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
-    <hyperlink ref="I44" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
-    <hyperlink ref="I45" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
+    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
+    <hyperlink ref="I35" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
+    <hyperlink ref="I37" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
+    <hyperlink ref="I38" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
+    <hyperlink ref="I39" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
+    <hyperlink ref="I40" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
+    <hyperlink ref="I46" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
+    <hyperlink ref="I47" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
     <hyperlink ref="I7" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
     <hyperlink ref="I8" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
-    <hyperlink ref="I46" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
+    <hyperlink ref="I48" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
     <hyperlink ref="I3" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
-    <hyperlink ref="I40" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
-    <hyperlink ref="I50" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
-    <hyperlink ref="I51" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
-    <hyperlink ref="I42" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
-    <hyperlink ref="I47" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
-    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
+    <hyperlink ref="I41" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
+    <hyperlink ref="I52" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
+    <hyperlink ref="I53" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
+    <hyperlink ref="I43" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
+    <hyperlink ref="I49" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
+    <hyperlink ref="I50" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
     <hyperlink ref="I29" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
     <hyperlink ref="I24" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
     <hyperlink ref="I13" r:id="rId33" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
     <hyperlink ref="I12" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
     <hyperlink ref="I11" r:id="rId35" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
     <hyperlink ref="I10" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
-    <hyperlink ref="I35" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
+    <hyperlink ref="I36" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
     <hyperlink ref="I17" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
     <hyperlink ref="I14" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
     <hyperlink ref="I20" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
@@ -3615,29 +3898,32 @@
     <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
     <hyperlink ref="I4" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
     <hyperlink ref="I5" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
-    <hyperlink ref="I58" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
-    <hyperlink ref="I55" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
-    <hyperlink ref="I56" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
-    <hyperlink ref="I57" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
-    <hyperlink ref="I52" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
-    <hyperlink ref="I53" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
-    <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
-    <hyperlink ref="I60" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
-    <hyperlink ref="I67" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
-    <hyperlink ref="I64" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
-    <hyperlink ref="I65" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
-    <hyperlink ref="I66" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
-    <hyperlink ref="I61" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
-    <hyperlink ref="I62" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
-    <hyperlink ref="I63" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
-    <hyperlink ref="I68" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I60" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
+    <hyperlink ref="I57" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
+    <hyperlink ref="I58" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
+    <hyperlink ref="I59" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
+    <hyperlink ref="I54" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
+    <hyperlink ref="I55" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
+    <hyperlink ref="I56" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
+    <hyperlink ref="I62" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
+    <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
+    <hyperlink ref="I69" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I66" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I67" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I68" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I63" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I64" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I65" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I70" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I34" r:id="rId63" display="https://www.azadvertizer.net/azpolicyadvertizer/25da7dfb-0666-4a15-a8f5-402127efd8bb.html" xr:uid="{38CBF8C3-8CFC-47E0-9942-240DA0287CA0}"/>
+    <hyperlink ref="I45" r:id="rId64" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html" xr:uid="{C93DAC5F-2A0F-4915-AA1B-7CC1E650BB8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId62"/>
+  <pageSetup orientation="portrait" r:id="rId65"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:K54"/>
   <sheetViews>
@@ -5448,7 +5734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
   <dimension ref="A1:I35"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat: Add Subnets should be private policy definition
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679EC49-138E-4518-8A26-2D088C4FAE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA527A-DEAD-45E0-BF19-819E3B7258FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-38510" yWindow="20" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$72</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="315">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -973,6 +973,21 @@
   </si>
   <si>
     <t>ALZ Policies (GitHub)</t>
+  </si>
+  <si>
+    <t>Subnets should be private</t>
+  </si>
+  <si>
+    <t>Ensure your subnets are secure by default by preventing default outbound access. For more information go to https://aka.ms/defaultoutboundaccessretirement</t>
+  </si>
+  <si>
+    <t>Audit, Deny</t>
+  </si>
+  <si>
+    <t>Subnets should be private - 7bca8353-aa3b-429b-904a-9229c4385837 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>ENFORCE-SubnetPrivatePolicyAssignment.json</t>
   </si>
 </sst>
 </file>
@@ -1492,9 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FFA7FA-CF8D-416B-AD3C-43815126868D}">
   <dimension ref="B20:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1534,11 +1547,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,13 +2155,13 @@
     </row>
     <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>310</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>310</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -2157,158 +2170,158 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>311</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>312</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>51</v>
+        <v>314</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="J19" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="J20" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>57</v>
+        <v>229</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="J21" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>223</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>223</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>225</v>
+        <v>55</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>234</v>
+        <v>56</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="J22" s="5">
-        <v>45187</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>63</v>
+        <v>230</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J23" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
@@ -2317,16 +2330,16 @@
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>207</v>
+        <v>62</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="J24" s="5">
         <v>45018</v>
@@ -2337,10 +2350,10 @@
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -2349,94 +2362,94 @@
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J25" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J26" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>226</v>
+        <v>69</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>235</v>
+        <v>70</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="J27" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
@@ -2445,48 +2458,48 @@
         <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>74</v>
+        <v>226</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>77</v>
+        <v>231</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J28" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>207</v>
+        <v>76</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="J29" s="5">
         <v>45018</v>
@@ -2497,10 +2510,10 @@
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -2509,62 +2522,62 @@
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J30" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -2573,30 +2586,30 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2605,30 +2618,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>302</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>302</v>
+        <v>87</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2637,30 +2650,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>303</v>
+        <v>88</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>301</v>
+        <v>89</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="J34" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>302</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>302</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2669,30 +2682,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>98</v>
+        <v>303</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>301</v>
       </c>
       <c r="J35" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>96</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2701,30 +2714,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>212</v>
+        <v>98</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="J36" s="5">
         <v>45084</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2733,30 +2746,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>51</v>
+        <v>99</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J37" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2765,30 +2778,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2797,30 +2810,30 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2829,48 +2842,48 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>200</v>
+        <v>113</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="J41" s="5">
         <v>45018</v>
@@ -2881,10 +2894,10 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -2893,17 +2906,19 @@
         <v>12</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>242</v>
+        <v>150</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I42" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="J42" s="5">
-        <v>45363</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2911,31 +2926,29 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>203</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I43" s="4"/>
       <c r="J43" s="5">
-        <v>45180</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2943,127 +2956,127 @@
         <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="J44" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>227</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>227</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>304</v>
+        <v>228</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J45" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="J45" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>120</v>
+        <v>310</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>120</v>
+        <v>310</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>121</v>
+        <v>311</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>14</v>
+        <v>312</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>123</v>
+        <v>314</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="J47" s="5">
-        <v>45018</v>
+        <v>45519</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -3071,60 +3084,60 @@
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>205</v>
+        <v>122</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
@@ -3135,10 +3148,10 @@
         <v>115</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>40</v>
@@ -3147,182 +3160,176 @@
         <v>24</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J50" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="I52" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="J50" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="J52" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J51" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="J52" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>202</v>
+      <c r="J53" s="5">
+        <v>45018</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>266</v>
+        <v>135</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>273</v>
+        <v>136</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>294</v>
+        <v>201</v>
       </c>
       <c r="J54" s="5">
-        <v>45322</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>267</v>
+        <v>139</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>274</v>
+        <v>140</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>36</v>
+        <v>141</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="J55" s="5">
-        <v>45322</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -3330,10 +3337,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>259</v>
+        <v>29</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3342,16 +3349,16 @@
         <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J56" s="5">
         <v>45322</v>
@@ -3365,10 +3372,10 @@
         <v>44</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>260</v>
+        <v>34</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3377,16 +3384,16 @@
         <v>24</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>284</v>
+        <v>36</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="J57" s="5">
         <v>45322</v>
@@ -3400,10 +3407,10 @@
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3412,16 +3419,16 @@
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="J58" s="5">
         <v>45322</v>
@@ -3435,10 +3442,10 @@
         <v>44</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -3447,16 +3454,16 @@
         <v>24</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J59" s="5">
         <v>45322</v>
@@ -3465,15 +3472,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -3482,16 +3489,16 @@
         <v>24</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="J60" s="5">
         <v>45322</v>
@@ -3505,28 +3512,28 @@
         <v>44</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>282</v>
+        <v>14</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="J61" s="5">
         <v>45322</v>
@@ -3535,33 +3542,33 @@
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="J62" s="5">
         <v>45322</v>
@@ -3572,31 +3579,31 @@
     </row>
     <row r="63" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>29</v>
+        <v>264</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>14</v>
+        <v>282</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>32</v>
+        <v>288</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="J63" s="5">
         <v>45322</v>
@@ -3605,33 +3612,33 @@
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>34</v>
+        <v>265</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>36</v>
+        <v>289</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="J64" s="5">
         <v>45322</v>
@@ -3645,10 +3652,10 @@
         <v>72</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>259</v>
+        <v>29</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3657,16 +3664,16 @@
         <v>24</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J65" s="5">
         <v>45322</v>
@@ -3680,10 +3687,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>260</v>
+        <v>34</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3692,16 +3699,16 @@
         <v>24</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>284</v>
+        <v>36</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="J66" s="5">
         <v>45322</v>
@@ -3715,10 +3722,10 @@
         <v>72</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3727,16 +3734,16 @@
         <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="J67" s="5">
         <v>45322</v>
@@ -3750,10 +3757,10 @@
         <v>72</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -3762,16 +3769,16 @@
         <v>24</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J68" s="5">
         <v>45322</v>
@@ -3780,15 +3787,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -3797,16 +3804,16 @@
         <v>24</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="J69" s="5">
         <v>45322</v>
@@ -3815,33 +3822,33 @@
         <v>252</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J70" s="5">
         <v>45322</v>
@@ -3850,76 +3857,148 @@
         <v>252</v>
       </c>
     </row>
+    <row r="71" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J71" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J72" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K70" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:K72" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{CB9AA3F5-0FB5-4271-B843-BAC441E7FF28}"/>
     <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{C1E76027-B2E2-46AE-8FBD-9F0D49770442}"/>
     <hyperlink ref="I9" r:id="rId3" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{189AA603-D080-4747-8EE4-022DEBF70AC4}"/>
-    <hyperlink ref="I19" r:id="rId4" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{A326BBFF-13EF-4D72-866F-C82B6DB948CD}"/>
-    <hyperlink ref="I21" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{47846F9C-9BA5-4D50-BAC9-044A2B38522A}"/>
-    <hyperlink ref="I23" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{722CA2FF-9269-4E2F-8533-5ED7705D010E}"/>
-    <hyperlink ref="I25" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{137ED18D-F3D4-4225-915D-7618E3EB3F48}"/>
-    <hyperlink ref="I26" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{CFB3D49B-0E77-431E-8A4B-6A6C45FACD99}"/>
-    <hyperlink ref="I28" r:id="rId9" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{56989C35-212B-48D1-817B-986C70EFFD3A}"/>
-    <hyperlink ref="I30" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
-    <hyperlink ref="I31" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
-    <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
-    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
-    <hyperlink ref="I35" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
-    <hyperlink ref="I37" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
-    <hyperlink ref="I38" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
-    <hyperlink ref="I39" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
-    <hyperlink ref="I40" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
-    <hyperlink ref="I46" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
-    <hyperlink ref="I47" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
+    <hyperlink ref="I20" r:id="rId4" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{A326BBFF-13EF-4D72-866F-C82B6DB948CD}"/>
+    <hyperlink ref="I22" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{47846F9C-9BA5-4D50-BAC9-044A2B38522A}"/>
+    <hyperlink ref="I24" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{722CA2FF-9269-4E2F-8533-5ED7705D010E}"/>
+    <hyperlink ref="I26" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{137ED18D-F3D4-4225-915D-7618E3EB3F48}"/>
+    <hyperlink ref="I27" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{CFB3D49B-0E77-431E-8A4B-6A6C45FACD99}"/>
+    <hyperlink ref="I29" r:id="rId9" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{56989C35-212B-48D1-817B-986C70EFFD3A}"/>
+    <hyperlink ref="I31" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
+    <hyperlink ref="I32" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
+    <hyperlink ref="I33" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
+    <hyperlink ref="I34" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
+    <hyperlink ref="I36" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
+    <hyperlink ref="I38" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
+    <hyperlink ref="I39" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
+    <hyperlink ref="I40" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
+    <hyperlink ref="I41" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
+    <hyperlink ref="I48" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
+    <hyperlink ref="I49" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
     <hyperlink ref="I7" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
     <hyperlink ref="I8" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
-    <hyperlink ref="I48" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
+    <hyperlink ref="I50" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
     <hyperlink ref="I3" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
-    <hyperlink ref="I41" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
-    <hyperlink ref="I52" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
-    <hyperlink ref="I53" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
-    <hyperlink ref="I43" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
-    <hyperlink ref="I49" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
-    <hyperlink ref="I50" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
-    <hyperlink ref="I29" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
-    <hyperlink ref="I24" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
+    <hyperlink ref="I42" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
+    <hyperlink ref="I54" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
+    <hyperlink ref="I55" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
+    <hyperlink ref="I44" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
+    <hyperlink ref="I51" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
+    <hyperlink ref="I52" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
+    <hyperlink ref="I30" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
+    <hyperlink ref="I25" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
     <hyperlink ref="I13" r:id="rId33" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
     <hyperlink ref="I12" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
     <hyperlink ref="I11" r:id="rId35" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
     <hyperlink ref="I10" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
-    <hyperlink ref="I36" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
+    <hyperlink ref="I37" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
     <hyperlink ref="I17" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
     <hyperlink ref="I14" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
-    <hyperlink ref="I20" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
-    <hyperlink ref="I22" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
-    <hyperlink ref="I27" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
+    <hyperlink ref="I21" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
+    <hyperlink ref="I23" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
+    <hyperlink ref="I28" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
     <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
     <hyperlink ref="I4" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
     <hyperlink ref="I5" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
-    <hyperlink ref="I60" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
-    <hyperlink ref="I57" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
-    <hyperlink ref="I58" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
-    <hyperlink ref="I59" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
-    <hyperlink ref="I54" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
-    <hyperlink ref="I55" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
-    <hyperlink ref="I56" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
-    <hyperlink ref="I62" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
-    <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
-    <hyperlink ref="I69" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
-    <hyperlink ref="I66" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
-    <hyperlink ref="I67" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
-    <hyperlink ref="I68" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
-    <hyperlink ref="I63" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
-    <hyperlink ref="I64" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
-    <hyperlink ref="I65" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
-    <hyperlink ref="I70" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
-    <hyperlink ref="I34" r:id="rId63" display="https://www.azadvertizer.net/azpolicyadvertizer/25da7dfb-0666-4a15-a8f5-402127efd8bb.html" xr:uid="{38CBF8C3-8CFC-47E0-9942-240DA0287CA0}"/>
-    <hyperlink ref="I45" r:id="rId64" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html" xr:uid="{C93DAC5F-2A0F-4915-AA1B-7CC1E650BB8D}"/>
+    <hyperlink ref="I62" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
+    <hyperlink ref="I59" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
+    <hyperlink ref="I60" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
+    <hyperlink ref="I61" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
+    <hyperlink ref="I56" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
+    <hyperlink ref="I57" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
+    <hyperlink ref="I58" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
+    <hyperlink ref="I64" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
+    <hyperlink ref="I63" r:id="rId54" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
+    <hyperlink ref="I71" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I68" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I69" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I70" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I65" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I66" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I67" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I72" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I35" r:id="rId63" display="https://www.azadvertizer.net/azpolicyadvertizer/25da7dfb-0666-4a15-a8f5-402127efd8bb.html" xr:uid="{38CBF8C3-8CFC-47E0-9942-240DA0287CA0}"/>
+    <hyperlink ref="I46" r:id="rId64" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html" xr:uid="{C93DAC5F-2A0F-4915-AA1B-7CC1E650BB8D}"/>
+    <hyperlink ref="I19" r:id="rId65" display="https://www.azadvertizer.net/azpolicyadvertizer/7bca8353-aa3b-429b-904a-9229c4385837.html" xr:uid="{7166D0B8-5AFF-4B09-A435-5D5A160DC40B}"/>
+    <hyperlink ref="I47" r:id="rId66" display="https://www.azadvertizer.net/azpolicyadvertizer/7bca8353-aa3b-429b-904a-9229c4385837.html" xr:uid="{35261964-DE11-4D2A-A203-99D18A71AC16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId65"/>
+  <pageSetup orientation="portrait" r:id="rId67"/>
 </worksheet>
 </file>
 
@@ -6798,6 +6877,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7063,15 +7151,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7086,6 +7165,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7101,14 +7188,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Private subnet policy and portal update (#1728)
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679EC49-138E-4518-8A26-2D088C4FAE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA527A-DEAD-45E0-BF19-819E3B7258FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-38510" yWindow="20" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$72</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="315">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -973,6 +973,21 @@
   </si>
   <si>
     <t>ALZ Policies (GitHub)</t>
+  </si>
+  <si>
+    <t>Subnets should be private</t>
+  </si>
+  <si>
+    <t>Ensure your subnets are secure by default by preventing default outbound access. For more information go to https://aka.ms/defaultoutboundaccessretirement</t>
+  </si>
+  <si>
+    <t>Audit, Deny</t>
+  </si>
+  <si>
+    <t>Subnets should be private - 7bca8353-aa3b-429b-904a-9229c4385837 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>ENFORCE-SubnetPrivatePolicyAssignment.json</t>
   </si>
 </sst>
 </file>
@@ -1492,9 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FFA7FA-CF8D-416B-AD3C-43815126868D}">
   <dimension ref="B20:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1534,11 +1547,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N54" sqref="N54"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2142,13 +2155,13 @@
     </row>
     <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>310</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>310</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -2157,158 +2170,158 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>311</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>312</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>51</v>
+        <v>314</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="J19" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="J20" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>57</v>
+        <v>229</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="J21" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>223</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>223</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>225</v>
+        <v>55</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>234</v>
+        <v>56</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="J22" s="5">
-        <v>45187</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>63</v>
+        <v>230</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J23" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
@@ -2317,16 +2330,16 @@
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>207</v>
+        <v>62</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="J24" s="5">
         <v>45018</v>
@@ -2337,10 +2350,10 @@
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -2349,94 +2362,94 @@
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J25" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J26" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>226</v>
+        <v>69</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>235</v>
+        <v>70</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="J27" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
@@ -2445,48 +2458,48 @@
         <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>74</v>
+        <v>226</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>77</v>
+        <v>231</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J28" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>207</v>
+        <v>76</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="J29" s="5">
         <v>45018</v>
@@ -2497,10 +2510,10 @@
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -2509,62 +2522,62 @@
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J30" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -2573,30 +2586,30 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2605,30 +2618,30 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>302</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>302</v>
+        <v>87</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2637,30 +2650,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>303</v>
+        <v>88</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>301</v>
+        <v>89</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="J34" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>302</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>302</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2669,30 +2682,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>98</v>
+        <v>303</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>301</v>
       </c>
       <c r="J35" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>96</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2701,30 +2714,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>212</v>
+        <v>98</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="J36" s="5">
         <v>45084</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2733,30 +2746,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>51</v>
+        <v>99</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J37" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2765,30 +2778,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2797,30 +2810,30 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2829,48 +2842,48 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>200</v>
+        <v>113</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="J41" s="5">
         <v>45018</v>
@@ -2881,10 +2894,10 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -2893,17 +2906,19 @@
         <v>12</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>242</v>
+        <v>150</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I42" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="J42" s="5">
-        <v>45363</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2911,31 +2926,29 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>203</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I43" s="4"/>
       <c r="J43" s="5">
-        <v>45180</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2943,127 +2956,127 @@
         <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="J44" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>68</v>
+        <v>227</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>227</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>304</v>
+        <v>228</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J45" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="I46" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="J45" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>120</v>
+        <v>310</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>120</v>
+        <v>310</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>121</v>
+        <v>311</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>14</v>
+        <v>312</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>123</v>
+        <v>314</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="J47" s="5">
-        <v>45018</v>
+        <v>45519</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -3071,60 +3084,60 @@
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>144</v>
+        <v>118</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>205</v>
+        <v>122</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="J49" s="5">
         <v>45018</v>
@@ -3135,10 +3148,10 @@
         <v>115</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>40</v>
@@ -3147,182 +3160,176 @@
         <v>24</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J50" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="I52" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="J50" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="J52" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="I53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J51" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="J52" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>202</v>
+      <c r="J53" s="5">
+        <v>45018</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>29</v>
+        <v>135</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>266</v>
+        <v>135</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>273</v>
+        <v>136</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>294</v>
+        <v>201</v>
       </c>
       <c r="J54" s="5">
-        <v>45322</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>34</v>
+        <v>139</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>267</v>
+        <v>139</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>274</v>
+        <v>140</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>36</v>
+        <v>141</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="J55" s="5">
-        <v>45322</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -3330,10 +3337,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>259</v>
+        <v>29</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3342,16 +3349,16 @@
         <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J56" s="5">
         <v>45322</v>
@@ -3365,10 +3372,10 @@
         <v>44</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>260</v>
+        <v>34</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3377,16 +3384,16 @@
         <v>24</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>284</v>
+        <v>36</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="J57" s="5">
         <v>45322</v>
@@ -3400,10 +3407,10 @@
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3412,16 +3419,16 @@
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="J58" s="5">
         <v>45322</v>
@@ -3435,10 +3442,10 @@
         <v>44</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -3447,16 +3454,16 @@
         <v>24</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J59" s="5">
         <v>45322</v>
@@ -3465,15 +3472,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>11</v>
@@ -3482,16 +3489,16 @@
         <v>24</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="J60" s="5">
         <v>45322</v>
@@ -3505,28 +3512,28 @@
         <v>44</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>282</v>
+        <v>14</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="J61" s="5">
         <v>45322</v>
@@ -3535,33 +3542,33 @@
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="J62" s="5">
         <v>45322</v>
@@ -3572,31 +3579,31 @@
     </row>
     <row r="63" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>29</v>
+        <v>264</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>14</v>
+        <v>282</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>32</v>
+        <v>288</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="J63" s="5">
         <v>45322</v>
@@ -3605,33 +3612,33 @@
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>34</v>
+        <v>265</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>36</v>
+        <v>289</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="J64" s="5">
         <v>45322</v>
@@ -3645,10 +3652,10 @@
         <v>72</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>259</v>
+        <v>29</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3657,16 +3664,16 @@
         <v>24</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J65" s="5">
         <v>45322</v>
@@ -3680,10 +3687,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>260</v>
+        <v>34</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3692,16 +3699,16 @@
         <v>24</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>284</v>
+        <v>36</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="J66" s="5">
         <v>45322</v>
@@ -3715,10 +3722,10 @@
         <v>72</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3727,16 +3734,16 @@
         <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="J67" s="5">
         <v>45322</v>
@@ -3750,10 +3757,10 @@
         <v>72</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -3762,16 +3769,16 @@
         <v>24</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J68" s="5">
         <v>45322</v>
@@ -3780,15 +3787,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
@@ -3797,16 +3804,16 @@
         <v>24</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="J69" s="5">
         <v>45322</v>
@@ -3815,33 +3822,33 @@
         <v>252</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J70" s="5">
         <v>45322</v>
@@ -3850,76 +3857,148 @@
         <v>252</v>
       </c>
     </row>
+    <row r="71" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J71" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J72" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K70" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:K72" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{CB9AA3F5-0FB5-4271-B843-BAC441E7FF28}"/>
     <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{C1E76027-B2E2-46AE-8FBD-9F0D49770442}"/>
     <hyperlink ref="I9" r:id="rId3" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{189AA603-D080-4747-8EE4-022DEBF70AC4}"/>
-    <hyperlink ref="I19" r:id="rId4" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{A326BBFF-13EF-4D72-866F-C82B6DB948CD}"/>
-    <hyperlink ref="I21" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{47846F9C-9BA5-4D50-BAC9-044A2B38522A}"/>
-    <hyperlink ref="I23" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{722CA2FF-9269-4E2F-8533-5ED7705D010E}"/>
-    <hyperlink ref="I25" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{137ED18D-F3D4-4225-915D-7618E3EB3F48}"/>
-    <hyperlink ref="I26" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{CFB3D49B-0E77-431E-8A4B-6A6C45FACD99}"/>
-    <hyperlink ref="I28" r:id="rId9" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{56989C35-212B-48D1-817B-986C70EFFD3A}"/>
-    <hyperlink ref="I30" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
-    <hyperlink ref="I31" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
-    <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
-    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
-    <hyperlink ref="I35" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
-    <hyperlink ref="I37" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
-    <hyperlink ref="I38" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
-    <hyperlink ref="I39" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
-    <hyperlink ref="I40" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
-    <hyperlink ref="I46" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
-    <hyperlink ref="I47" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
+    <hyperlink ref="I20" r:id="rId4" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{A326BBFF-13EF-4D72-866F-C82B6DB948CD}"/>
+    <hyperlink ref="I22" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{47846F9C-9BA5-4D50-BAC9-044A2B38522A}"/>
+    <hyperlink ref="I24" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{722CA2FF-9269-4E2F-8533-5ED7705D010E}"/>
+    <hyperlink ref="I26" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{137ED18D-F3D4-4225-915D-7618E3EB3F48}"/>
+    <hyperlink ref="I27" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{CFB3D49B-0E77-431E-8A4B-6A6C45FACD99}"/>
+    <hyperlink ref="I29" r:id="rId9" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{56989C35-212B-48D1-817B-986C70EFFD3A}"/>
+    <hyperlink ref="I31" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
+    <hyperlink ref="I32" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
+    <hyperlink ref="I33" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
+    <hyperlink ref="I34" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
+    <hyperlink ref="I36" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
+    <hyperlink ref="I38" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
+    <hyperlink ref="I39" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
+    <hyperlink ref="I40" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
+    <hyperlink ref="I41" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
+    <hyperlink ref="I48" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
+    <hyperlink ref="I49" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
     <hyperlink ref="I7" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
     <hyperlink ref="I8" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
-    <hyperlink ref="I48" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
+    <hyperlink ref="I50" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
     <hyperlink ref="I3" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
-    <hyperlink ref="I41" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
-    <hyperlink ref="I52" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
-    <hyperlink ref="I53" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
-    <hyperlink ref="I43" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
-    <hyperlink ref="I49" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
-    <hyperlink ref="I50" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
-    <hyperlink ref="I29" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
-    <hyperlink ref="I24" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
+    <hyperlink ref="I42" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
+    <hyperlink ref="I54" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
+    <hyperlink ref="I55" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
+    <hyperlink ref="I44" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
+    <hyperlink ref="I51" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
+    <hyperlink ref="I52" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
+    <hyperlink ref="I30" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
+    <hyperlink ref="I25" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
     <hyperlink ref="I13" r:id="rId33" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
     <hyperlink ref="I12" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
     <hyperlink ref="I11" r:id="rId35" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
     <hyperlink ref="I10" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
-    <hyperlink ref="I36" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
+    <hyperlink ref="I37" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
     <hyperlink ref="I17" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
     <hyperlink ref="I14" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
-    <hyperlink ref="I20" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
-    <hyperlink ref="I22" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
-    <hyperlink ref="I27" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
+    <hyperlink ref="I21" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
+    <hyperlink ref="I23" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
+    <hyperlink ref="I28" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
     <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
     <hyperlink ref="I4" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
     <hyperlink ref="I5" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
-    <hyperlink ref="I60" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
-    <hyperlink ref="I57" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
-    <hyperlink ref="I58" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
-    <hyperlink ref="I59" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
-    <hyperlink ref="I54" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
-    <hyperlink ref="I55" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
-    <hyperlink ref="I56" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
-    <hyperlink ref="I62" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
-    <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
-    <hyperlink ref="I69" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
-    <hyperlink ref="I66" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
-    <hyperlink ref="I67" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
-    <hyperlink ref="I68" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
-    <hyperlink ref="I63" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
-    <hyperlink ref="I64" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
-    <hyperlink ref="I65" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
-    <hyperlink ref="I70" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
-    <hyperlink ref="I34" r:id="rId63" display="https://www.azadvertizer.net/azpolicyadvertizer/25da7dfb-0666-4a15-a8f5-402127efd8bb.html" xr:uid="{38CBF8C3-8CFC-47E0-9942-240DA0287CA0}"/>
-    <hyperlink ref="I45" r:id="rId64" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html" xr:uid="{C93DAC5F-2A0F-4915-AA1B-7CC1E650BB8D}"/>
+    <hyperlink ref="I62" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
+    <hyperlink ref="I59" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
+    <hyperlink ref="I60" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
+    <hyperlink ref="I61" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
+    <hyperlink ref="I56" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
+    <hyperlink ref="I57" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
+    <hyperlink ref="I58" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
+    <hyperlink ref="I64" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
+    <hyperlink ref="I63" r:id="rId54" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
+    <hyperlink ref="I71" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I68" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I69" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I70" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I65" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I66" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I67" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I72" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I35" r:id="rId63" display="https://www.azadvertizer.net/azpolicyadvertizer/25da7dfb-0666-4a15-a8f5-402127efd8bb.html" xr:uid="{38CBF8C3-8CFC-47E0-9942-240DA0287CA0}"/>
+    <hyperlink ref="I46" r:id="rId64" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html" xr:uid="{C93DAC5F-2A0F-4915-AA1B-7CC1E650BB8D}"/>
+    <hyperlink ref="I19" r:id="rId65" display="https://www.azadvertizer.net/azpolicyadvertizer/7bca8353-aa3b-429b-904a-9229c4385837.html" xr:uid="{7166D0B8-5AFF-4B09-A435-5D5A160DC40B}"/>
+    <hyperlink ref="I47" r:id="rId66" display="https://www.azadvertizer.net/azpolicyadvertizer/7bca8353-aa3b-429b-904a-9229c4385837.html" xr:uid="{35261964-DE11-4D2A-A203-99D18A71AC16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId65"/>
+  <pageSetup orientation="portrait" r:id="rId67"/>
 </worksheet>
 </file>
 
@@ -6798,6 +6877,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7063,15 +7151,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -7086,6 +7165,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7101,14 +7188,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Policy Refresh Q1FY25 (#1789)
Co-authored-by: JonasCordsen <106592722+JonasCordsen@users.noreply.github.com>
Co-authored-by: Jonas Nørregaard Cordsen <jnc@cescom.dk>
Co-authored-by: github-actions <41898282+github-actions[bot]@users.noreply.github.com>
Co-authored-by: Jack Tracey <41163455+jtracey93@users.noreply.github.com>
Co-authored-by: BeckyHope19 <105707948+BeckyHope19@users.noreply.github.com>
Co-authored-by: Zach Trocinski <30884663+oZakari@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Enterprise-Scale\docs\wiki\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\Springstone\Enterprise-Scale\docs\wiki\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4926854-FDAD-4DB7-999E-DDEAE8AC1160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA527A-DEAD-45E0-BF19-819E3B7258FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
+    <workbookView xWindow="-38510" yWindow="20" windowWidth="38620" windowHeight="21820" xr2:uid="{839F6A4D-21A7-4C10-BD9E-872DCD53FD8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId1"/>
-    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" r:id="rId2"/>
-    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" r:id="rId3"/>
+    <sheet name="Overview" sheetId="8" r:id="rId1"/>
+    <sheet name="ALZ Policy Assignments H1CY24" sheetId="7" r:id="rId2"/>
+    <sheet name="ALZ Policy Assignments 03CY23" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="ALZ Policy Pre-03CY23" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ALZ Policy Assignments 03CY23'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALZ Policy Assignments H1CY24'!$A$1:$K$72</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="315">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -836,6 +837,9 @@
     <t>Enable Defender for SQL on SQL VMs and Arc-enabled SQL Servers</t>
   </si>
   <si>
+    <t>Do not allow deletion of resource types</t>
+  </si>
+  <si>
     <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines</t>
   </si>
   <si>
@@ -884,6 +888,9 @@
     <t>This policy initiative enables Microsoft Defender for SQL and AMA on SQL VMs and Arc-enabled SQL Servers.</t>
   </si>
   <si>
+    <t>This policy enables you to specify the resource types that your organization can protect from accidentals deletion by blocking delete calls using deny action effect. Assigned to deny the deletion of the User Assignment Managed Identity that is used for AMA.</t>
+  </si>
+  <si>
     <t>DenyAction</t>
   </si>
   <si>
@@ -902,6 +909,9 @@
     <t>DINE-MDFCDefenderSQLAMAPolicyAssignment.json</t>
   </si>
   <si>
+    <t>DENYACTION-ResourceDeletionPolicyAssignment.json</t>
+  </si>
+  <si>
     <t>MODIFY-AUM-CheckUpdatesPolicyAssignment.json</t>
   </si>
   <si>
@@ -929,19 +939,55 @@
     <t>Configure periodic checking for missing system updates on azure virtual machines and Arc-enabled virtual machines - Deploy-AUM-CheckUpdates (azadvertizer.net)</t>
   </si>
   <si>
-    <t>2024-01-34</t>
-  </si>
-  <si>
-    <t>Do not allow deletion of the User Assigned Managed Identity used by AMA</t>
-  </si>
-  <si>
-    <t>This policy provides a safeguard against accidental removal of the User Assigned Managed Identity used by AMA by blocking delete calls using deny action effect.</t>
-  </si>
-  <si>
-    <t>DENYACTION-DeleteUAMIAMAPolicyAssignment.json</t>
-  </si>
-  <si>
-    <t>Do not allow deletion of specified resource and resource type</t>
+    <t>Do not allow deletion of resource types - 78460a36-508a-49a4-b2b2-2f5ec564f4bb (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Deny virtual machines and virtual machine scale sets that do not use managed disk</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud Security Benchmark</t>
+  </si>
+  <si>
+    <t>Configure SQL servers to have auditing enabled to Log Analytics workspace - 25da7dfb-0666-4a15-a8f5-402127efd8bb (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Configure SQL servers to have auditing enabled to Log Analytics workspace</t>
+  </si>
+  <si>
+    <t>To ensure the operations performed against your SQL assets are captured, SQL servers should have auditing enabled. If auditing is not enabled, this policy will configure auditing events to flow to the specified Log Analytics workspace.</t>
+  </si>
+  <si>
+    <t>Enforce backup for all virtual machines by deploying a recovery services vault in the same location and resource group as the virtual machine. Doing this is useful when different application teams in your organization are allocated separate resource groups and need to manage their own backups and restores. You can optionally exclude virtual machines containing a specified tag to control the scope of assignment. See https://aka.ms/AzureVMAppCentricBackupExcludeTag.</t>
+  </si>
+  <si>
+    <t>Configure backup on virtual machines without a given tag to a new recovery services vault with a default policy - 98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>Quick links to ALZ Policies and Initiatives:</t>
+  </si>
+  <si>
+    <t>ALZ Initiatives (AzAdvertizer)</t>
+  </si>
+  <si>
+    <t>ALZ Policies (AzAdvertizer)</t>
+  </si>
+  <si>
+    <t>ALZ Policies (GitHub)</t>
+  </si>
+  <si>
+    <t>Subnets should be private</t>
+  </si>
+  <si>
+    <t>Ensure your subnets are secure by default by preventing default outbound access. For more information go to https://aka.ms/defaultoutboundaccessretirement</t>
+  </si>
+  <si>
+    <t>Audit, Deny</t>
+  </si>
+  <si>
+    <t>Subnets should be private - 7bca8353-aa3b-429b-904a-9229c4385837 (azadvertizer.net)</t>
+  </si>
+  <si>
+    <t>ENFORCE-SubnetPrivatePolicyAssignment.json</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1060,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1044,6 +1090,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1060,6 +1107,138 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57C42FFB-0C15-3558-BD31-1C4590C92C51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="167640" y="182880"/>
+          <a:ext cx="7048500" cy="3223260"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1600" b="1"/>
+            <a:t>Notes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AE" sz="1600" b="1"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0"/>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t> document includes Azure Landing Zone (ALZ) default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="1" baseline="0"/>
+            <a:t>assignments</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t>, not the exhaustive list of custom policies that ALZ provides. Default assignments are those made without changing any options in the portal accelerator and keeping all the "Yes" options as is. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0"/>
+            <a:t>What is not included are the optional policies and initiatives</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t> that ALZ does not assign by default, for example, "Workload Specific Compliance" initiatives.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t>For the complete list of ALZ initiatives and policies please use https://www.azadvertizer.net and use the filters to select "ALZ" policies/initiatives, or use the quick links below.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0"/>
+            <a:t>While</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AE" sz="1100" b="0" baseline="0"/>
+            <a:t> we make every effort to keep this document up-to-date, it is challenging keeping a binary updated outside our normal GitHub processes. For the most up-to-date version please review ALZ Policies on GitHub (link below)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AE" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1325,12 +1504,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1FFA7FA-CF8D-416B-AD3C-43815126868D}">
+  <dimension ref="B20:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B21" r:id="rId1" location="%7B%22col_8%22%3A%7B%22flt%22%3A%22ALZ%22%7D%7D" display="ALZ Initiatives" xr:uid="{DBFEFF67-2F59-430A-9C74-2F9C44BB7FF7}"/>
+    <hyperlink ref="B22" r:id="rId2" display="ALZ Policies" xr:uid="{3710756B-881D-4F79-B7FB-86E68C96AF9B}"/>
+    <hyperlink ref="B23" r:id="rId3" xr:uid="{08074762-F5B3-4CF0-9C48-937CB547FB81}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7095E7F-24DE-43CD-9C57-427295435B12}">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,7 +1743,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>300</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>
@@ -1714,7 +1935,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>299</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>163</v>
@@ -1934,13 +2155,13 @@
     </row>
     <row r="19" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>310</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>310</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -1949,158 +2170,158 @@
         <v>24</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>311</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>312</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>51</v>
+        <v>314</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="J19" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="J20" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>57</v>
+        <v>229</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="J21" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>223</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>223</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>225</v>
+        <v>55</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>234</v>
+        <v>56</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="J22" s="5">
-        <v>45187</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>223</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>225</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>63</v>
+        <v>230</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>234</v>
       </c>
       <c r="J23" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>171</v>
+        <v>59</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>40</v>
@@ -2109,16 +2330,16 @@
         <v>12</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>173</v>
+        <v>60</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>207</v>
+        <v>62</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="J24" s="5">
         <v>45018</v>
@@ -2129,10 +2350,10 @@
         <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>40</v>
@@ -2141,94 +2362,94 @@
         <v>12</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J25" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J26" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>224</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>226</v>
+        <v>69</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>235</v>
+        <v>70</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="J27" s="5">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>73</v>
+        <v>224</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
@@ -2237,48 +2458,48 @@
         <v>12</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>74</v>
+        <v>226</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>77</v>
+        <v>231</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="J28" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>207</v>
+        <v>76</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="J29" s="5">
         <v>45018</v>
@@ -2289,10 +2510,10 @@
         <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>40</v>
@@ -2301,62 +2522,62 @@
         <v>12</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>67</v>
+        <v>172</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>207</v>
       </c>
       <c r="J30" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="J31" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>40</v>
@@ -2365,30 +2586,30 @@
         <v>24</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J32" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>40</v>
@@ -2397,16 +2618,16 @@
         <v>24</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J33" s="5">
         <v>45018</v>
@@ -2417,10 +2638,10 @@
         <v>72</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>40</v>
@@ -2429,30 +2650,30 @@
         <v>24</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="J34" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>96</v>
+        <v>302</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>302</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>40</v>
@@ -2461,30 +2682,30 @@
         <v>24</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>98</v>
+        <v>303</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>301</v>
       </c>
       <c r="J35" s="5">
-        <v>45084</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>211</v>
+        <v>96</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>211</v>
+        <v>97</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>40</v>
@@ -2493,30 +2714,30 @@
         <v>24</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>212</v>
+        <v>98</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="J36" s="5">
         <v>45084</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>40</v>
@@ -2525,30 +2746,30 @@
         <v>24</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>102</v>
+        <v>212</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>51</v>
+        <v>99</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="J37" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+        <v>45084</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>40</v>
@@ -2557,30 +2778,30 @@
         <v>24</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="J38" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>40</v>
@@ -2589,30 +2810,30 @@
         <v>24</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J39" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>40</v>
@@ -2621,48 +2842,48 @@
         <v>24</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J40" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>151</v>
+        <v>61</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>200</v>
+        <v>113</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="J41" s="5">
         <v>45018</v>
@@ -2673,10 +2894,10 @@
         <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>241</v>
+        <v>149</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -2685,17 +2906,19 @@
         <v>12</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>242</v>
+        <v>150</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="I42" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="J42" s="5">
-        <v>45363</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2703,31 +2926,29 @@
         <v>72</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>241</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>84</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>203</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="I43" s="4"/>
       <c r="J43" s="5">
-        <v>45180</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2735,42 +2956,42 @@
         <v>72</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>227</v>
+        <v>158</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>228</v>
+        <v>159</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="J44" s="5">
-        <v>45018</v>
+        <v>45180</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
@@ -2779,62 +3000,62 @@
         <v>12</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>117</v>
+        <v>228</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>119</v>
+        <v>232</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>236</v>
       </c>
       <c r="J45" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>121</v>
+        <v>304</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>123</v>
+        <v>70</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>305</v>
       </c>
       <c r="J46" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>142</v>
+        <v>310</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>143</v>
+        <v>310</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>40</v>
@@ -2843,281 +3064,272 @@
         <v>24</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>145</v>
+        <v>311</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>61</v>
+        <v>312</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>146</v>
+        <v>314</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>144</v>
+        <v>313</v>
       </c>
       <c r="J47" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>205</v>
+        <v>118</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="J48" s="5">
         <v>45018</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J49" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J50" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="J51" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" s="1" t="s">
+      <c r="D52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="J49" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J50" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="J51" s="5">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="J52" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>272</v>
+        <v>45</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>252</v>
+        <v>45</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J53" s="5">
+        <v>45018</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>266</v>
+        <v>135</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>273</v>
+        <v>136</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>14</v>
+        <v>137</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="J54" s="5">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>44</v>
+        <v>216</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>259</v>
+        <v>139</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>267</v>
+        <v>139</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>274</v>
+        <v>140</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>284</v>
+        <v>141</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
@@ -3125,10 +3337,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>260</v>
+        <v>29</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>11</v>
@@ -3137,19 +3349,19 @@
         <v>24</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>282</v>
+        <v>32</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="J56" s="5">
+        <v>45322</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>252</v>
@@ -3160,10 +3372,10 @@
         <v>44</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>261</v>
+        <v>34</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>11</v>
@@ -3172,19 +3384,19 @@
         <v>24</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>283</v>
+        <v>36</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="J57" s="5" t="s">
         <v>295</v>
+      </c>
+      <c r="J57" s="5">
+        <v>45322</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>252</v>
@@ -3195,10 +3407,10 @@
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>11</v>
@@ -3207,33 +3419,33 @@
         <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
+      </c>
+      <c r="J58" s="5">
+        <v>45322</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>11</v>
@@ -3242,95 +3454,103 @@
         <v>24</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>287</v>
+        <v>291</v>
+      </c>
+      <c r="J59" s="5">
+        <v>45322</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>299</v>
+        <v>270</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>280</v>
+        <v>14</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="I60" s="6"/>
+        <v>285</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="J60" s="5">
+        <v>45322</v>
+      </c>
       <c r="K60" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
+      </c>
+      <c r="J61" s="5">
+        <v>45322</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>29</v>
+        <v>263</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>11</v>
@@ -3339,19 +3559,19 @@
         <v>24</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>32</v>
+        <v>287</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>295</v>
+        <v>290</v>
+      </c>
+      <c r="J62" s="5">
+        <v>45322</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>252</v>
@@ -3359,69 +3579,69 @@
     </row>
     <row r="63" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>34</v>
+        <v>264</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>14</v>
+        <v>282</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>36</v>
+        <v>288</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>295</v>
+        <v>298</v>
+      </c>
+      <c r="J63" s="5">
+        <v>45322</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>295</v>
+        <v>297</v>
+      </c>
+      <c r="J64" s="5">
+        <v>45322</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>252</v>
@@ -3432,10 +3652,10 @@
         <v>72</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>260</v>
+        <v>29</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>11</v>
@@ -3444,19 +3664,19 @@
         <v>24</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>282</v>
+        <v>32</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="J65" s="5">
+        <v>45322</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>252</v>
@@ -3467,10 +3687,10 @@
         <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>261</v>
+        <v>34</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
@@ -3479,19 +3699,19 @@
         <v>24</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>283</v>
+        <v>36</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="J66" s="5" t="s">
         <v>295</v>
+      </c>
+      <c r="J66" s="5">
+        <v>45322</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>252</v>
@@ -3502,10 +3722,10 @@
         <v>72</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
@@ -3514,33 +3734,33 @@
         <v>24</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>295</v>
+        <v>296</v>
+      </c>
+      <c r="J67" s="5">
+        <v>45322</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
@@ -3549,128 +3769,240 @@
         <v>24</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>287</v>
+        <v>291</v>
+      </c>
+      <c r="J68" s="5">
+        <v>45322</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="J69" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
+      </c>
+      <c r="J69" s="5">
+        <v>45322</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>252</v>
       </c>
     </row>
+    <row r="70" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="J70" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J71" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="J72" s="5">
+        <v>45322</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
+  <autoFilter ref="A1:K72" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-MDFC-Config.html" xr:uid="{CB9AA3F5-0FB5-4271-B843-BAC441E7FF28}"/>
     <hyperlink ref="I6" r:id="rId2" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/1f3afdf9-d0c9-4c3d-847f-89da613e70a8.html" xr:uid="{C1E76027-B2E2-46AE-8FBD-9F0D49770442}"/>
     <hyperlink ref="I9" r:id="rId3" display="https://www.azadvertizer.net/azpolicyadvertizer/2465583e-4e78-4c15-b6be-a36cbc7c8b0f.html" xr:uid="{189AA603-D080-4747-8EE4-022DEBF70AC4}"/>
-    <hyperlink ref="I19" r:id="rId4" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{A326BBFF-13EF-4D72-866F-C82B6DB948CD}"/>
-    <hyperlink ref="I21" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{47846F9C-9BA5-4D50-BAC9-044A2B38522A}"/>
-    <hyperlink ref="I23" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{722CA2FF-9269-4E2F-8533-5ED7705D010E}"/>
-    <hyperlink ref="I25" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{137ED18D-F3D4-4225-915D-7618E3EB3F48}"/>
-    <hyperlink ref="I26" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{CFB3D49B-0E77-431E-8A4B-6A6C45FACD99}"/>
-    <hyperlink ref="I28" r:id="rId9" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{56989C35-212B-48D1-817B-986C70EFFD3A}"/>
-    <hyperlink ref="I30" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
-    <hyperlink ref="I31" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
-    <hyperlink ref="I32" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
-    <hyperlink ref="I33" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
-    <hyperlink ref="I34" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/a6fb4358-5bf4-4ad7-ba82-2cd2f41ce5e9.html" xr:uid="{FB722C1D-B184-4DFC-8C0C-C02F60381DAC}"/>
-    <hyperlink ref="I35" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
-    <hyperlink ref="I37" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
-    <hyperlink ref="I38" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
-    <hyperlink ref="I39" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
-    <hyperlink ref="I40" r:id="rId19" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
-    <hyperlink ref="I45" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
-    <hyperlink ref="I46" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
-    <hyperlink ref="I7" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
-    <hyperlink ref="I8" r:id="rId23" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
-    <hyperlink ref="I47" r:id="rId24" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
-    <hyperlink ref="I3" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
-    <hyperlink ref="I41" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
-    <hyperlink ref="I51" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
-    <hyperlink ref="I52" r:id="rId28" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
-    <hyperlink ref="I43" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
-    <hyperlink ref="I48" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
-    <hyperlink ref="I49" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
-    <hyperlink ref="I29" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
-    <hyperlink ref="I24" r:id="rId33" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
-    <hyperlink ref="I13" r:id="rId34" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
-    <hyperlink ref="I12" r:id="rId35" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
-    <hyperlink ref="I11" r:id="rId36" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
-    <hyperlink ref="I10" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
-    <hyperlink ref="I36" r:id="rId38" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
-    <hyperlink ref="I17" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
-    <hyperlink ref="I14" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
-    <hyperlink ref="I20" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
-    <hyperlink ref="I22" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
-    <hyperlink ref="I27" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
-    <hyperlink ref="I15" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
-    <hyperlink ref="I4" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
-    <hyperlink ref="I5" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
-    <hyperlink ref="I59" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
-    <hyperlink ref="I56" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
-    <hyperlink ref="I57" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
-    <hyperlink ref="I58" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
-    <hyperlink ref="I53" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
-    <hyperlink ref="I54" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
-    <hyperlink ref="I55" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
-    <hyperlink ref="I61" r:id="rId54" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
-    <hyperlink ref="I68" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
-    <hyperlink ref="I65" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
-    <hyperlink ref="I66" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
-    <hyperlink ref="I67" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
-    <hyperlink ref="I62" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
-    <hyperlink ref="I63" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
-    <hyperlink ref="I64" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
-    <hyperlink ref="I69" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I20" r:id="rId4" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{A326BBFF-13EF-4D72-866F-C82B6DB948CD}"/>
+    <hyperlink ref="I22" r:id="rId5" display="https://www.azadvertizer.net/azpolicyadvertizer/8e3e61b3-0b32-22d5-4edf-55f87fdb5955.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_1.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F8e3e61b3-0b32-22d5-4edf-55f87fdb5955_2.0.0.json" xr:uid="{47846F9C-9BA5-4D50-BAC9-044A2B38522A}"/>
+    <hyperlink ref="I24" r:id="rId6" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-PublicIP.html" xr:uid="{722CA2FF-9269-4E2F-8533-5ED7705D010E}"/>
+    <hyperlink ref="I26" r:id="rId7" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{137ED18D-F3D4-4225-915D-7618E3EB3F48}"/>
+    <hyperlink ref="I27" r:id="rId8" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86_9.0.0.json" xr:uid="{CFB3D49B-0E77-431E-8A4B-6A6C45FACD99}"/>
+    <hyperlink ref="I29" r:id="rId9" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-EncryptTransit.html" xr:uid="{56989C35-212B-48D1-817B-986C70EFFD3A}"/>
+    <hyperlink ref="I31" r:id="rId10" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-Subnet-Without-Nsg.html" xr:uid="{C9EE3BD2-2E35-4D8B-8C38-A0799E409D52}"/>
+    <hyperlink ref="I32" r:id="rId11" display="https://www.azadvertizer.net/azpolicyadvertizer/88c0b9da-ce96-4b03-9635-f29a937e2900.html" xr:uid="{07613AA7-E998-469B-8030-690A02055581}"/>
+    <hyperlink ref="I33" r:id="rId12" display="https://www.azadvertizer.net/azpolicyadvertizer/404c3081-a854-4457-ae30-26a93ef643f9.html" xr:uid="{8F69101F-5446-4B04-AB2B-D6FFEBBBD022}"/>
+    <hyperlink ref="I34" r:id="rId13" display="https://www.azadvertizer.net/azpolicyadvertizer/a8eff44f-8c92-45c3-a3fb-9880802d67a7.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_3.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2Fa8eff44f-8c92-45c3-a3fb-9880802d67a7_4.0.0.json" xr:uid="{7DE9128C-7DEE-46A2-84BC-774CCFDCA677}"/>
+    <hyperlink ref="I36" r:id="rId14" display="https://www.azadvertizer.net/azpolicyadvertizer/36d49e87-48c4-4f2e-beed-ba4ed02b71f5.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F36d49e87-48c4-4f2e-beed-ba4ed02b71f5_2.1.0.json" xr:uid="{2FC5978A-D8DE-4ADA-B941-5C9CAFD53837}"/>
+    <hyperlink ref="I38" r:id="rId15" display="https://www.azadvertizer.net/azpolicyadvertizer/94de2ad3-e0c1-4caf-ad78-5d47bbc83d3d.html" xr:uid="{E598A2CF-5677-4582-98AB-63076BF8DAD5}"/>
+    <hyperlink ref="I39" r:id="rId16" display="https://www.azadvertizer.net/azpolicyadvertizer/95edb821-ddaf-4404-9732-666045e056b4.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F95edb821-ddaf-4404-9732-666045e056b4_9.0.1.json" xr:uid="{44921BEE-02CB-40C5-A4E5-7C281FD86702}"/>
+    <hyperlink ref="I40" r:id="rId17" display="https://www.azadvertizer.net/azpolicyadvertizer/1c6e92c9-99f0-4e55-9cf2-0c234dc48f99.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1c6e92c9-99f0-4e55-9cf2-0c234dc48f99_7.0.1.json" xr:uid="{A1950EA2-BE5B-4B0D-8796-1CF7C5E8F60A}"/>
+    <hyperlink ref="I41" r:id="rId18" display="https://www.azadvertizer.net/azpolicyadvertizer/1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d.html?desc=compareJson&amp;left=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.0.json&amp;right=https%3A%2F%2Fwww.azadvertizer.net%2Fazpolicyadvertizerjson%2F1a5b4dca-0b6f-4cf5-907c-56316bc1bf3d_8.0.1.json" xr:uid="{B1A6BC2A-FB30-4DFC-A721-568E13122AE3}"/>
+    <hyperlink ref="I48" r:id="rId19" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deny-PublicPaaSEndpoints.html" xr:uid="{0C566A94-EA44-41D7-A37B-713E25CB154F}"/>
+    <hyperlink ref="I49" r:id="rId20" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-Private-DNS-Zones.html" xr:uid="{A5F7752B-7686-4E6D-A5F2-724252AFE550}"/>
+    <hyperlink ref="I7" r:id="rId21" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e77fc0b3-f7e9-4c58-bc13-cb753ed8e46e.html" xr:uid="{54ABE05A-2EC5-4C5C-8CC4-7E350C44E9C4}"/>
+    <hyperlink ref="I8" r:id="rId22" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/9cb3cc7a-b39b-4b82-bc89-e5a5d9ff7b97.html" xr:uid="{EB4696A4-2A1C-41C8-838D-D27E9DE5AB0F}"/>
+    <hyperlink ref="I50" r:id="rId23" display="https://www.azadvertizer.net/azpolicyadvertizer/83a86a26-fd1f-447c-b59d-e51f44264114.html" xr:uid="{92035E54-88D9-4668-980E-B15CCE5F3817}"/>
+    <hyperlink ref="I3" r:id="rId24" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e20d08c5-6d64-656d-6465-ce9e37fd0ebc.html" xr:uid="{2C80812F-3113-44DE-B796-C3B50DC2A259}"/>
+    <hyperlink ref="I42" r:id="rId25" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{1CFF66E3-406F-4011-AFAC-29F1FCF310E7}"/>
+    <hyperlink ref="I54" r:id="rId26" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Decomm.html" xr:uid="{18EE99AD-6122-4F01-A9C5-F54977412E6C}"/>
+    <hyperlink ref="I55" r:id="rId27" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ALZ-Sandbox.html" xr:uid="{03B98993-ABAE-4D72-B7C8-5FC64ADB5A2B}"/>
+    <hyperlink ref="I44" r:id="rId28" display="https://www.azadvertizer.net/azpolicyadvertizer/564feb30-bf6a-4854-b4bb-0d2d2d1e6c66.html" xr:uid="{E0771F2C-0363-4092-9B59-58E0A3684D26}"/>
+    <hyperlink ref="I51" r:id="rId29" display="https://www.azadvertizer.net/azpolicyadvertizer/Audit-PrivateLinkDnsZones.html" xr:uid="{FEA40CC4-448E-497C-BC10-0A58A09430EC}"/>
+    <hyperlink ref="I52" r:id="rId30" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{C745A8C1-3BB4-4AF8-ADE4-58B32C987257}"/>
+    <hyperlink ref="I30" r:id="rId31" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{A1C13FC3-A12B-40E4-9456-65B440CFEE13}"/>
+    <hyperlink ref="I25" r:id="rId32" display="https://www.azadvertizer.net/azpolicyadvertizer/Deny-MgmtPorts-From-Internet.html" xr:uid="{B3550C8E-52BB-4331-9436-1C6456298106}"/>
+    <hyperlink ref="I13" r:id="rId33" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Audit-UnusedResourcesCostOptimization.html" xr:uid="{98BDF766-448A-4078-9035-2801152641E7}"/>
+    <hyperlink ref="I12" r:id="rId34" display="https://www.azadvertizer.net/azpolicyadvertizer/06a78e20-9358-41c9-923c-fb736d382a4d.html" xr:uid="{85B4A94A-A65C-4EAA-8CE0-0D69D9D4B842}"/>
+    <hyperlink ref="I11" r:id="rId35" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-ACSB.html" xr:uid="{9C1C3010-2F7B-475D-A2AA-2C53811AD8D7}"/>
+    <hyperlink ref="I10" r:id="rId36" display="https://www.azadvertizer.net/azpolicyadvertizer/6c112d4e-5bc7-47ae-a041-ea2d9dccd749.html" xr:uid="{5F09C537-5909-40FC-8ADC-04A370AD27A7}"/>
+    <hyperlink ref="I37" r:id="rId37" display="https://www.azadvertizer.net/azpolicyadvertizer/86a912f6-9a06-4e26-b447-11b16ba8659f.html" xr:uid="{6A7A11D4-7491-400A-A13A-E7F7A8117ADC}"/>
+    <hyperlink ref="I17" r:id="rId38" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Enforce-Guardrails-KeyVault.html" xr:uid="{E52B6144-6E82-4A12-922D-754ACB01787A}"/>
+    <hyperlink ref="I14" r:id="rId39" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-ServiceHealth.html" xr:uid="{1F81D0A0-50F3-4666-AF0C-F42BB716E77E}"/>
+    <hyperlink ref="I21" r:id="rId40" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Connectivity.html" xr:uid="{C3DBEEF4-E3EA-4282-AAF1-17CFF059EB05}"/>
+    <hyperlink ref="I23" r:id="rId41" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Management.html" xr:uid="{19726F3A-C833-44BA-9CE0-8127E45CD473}"/>
+    <hyperlink ref="I28" r:id="rId42" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Alerting-Identity.html" xr:uid="{8D418295-0EDB-4521-8CB0-9D829AB64566}"/>
+    <hyperlink ref="I15" r:id="rId43" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/130fb88f-0fc9-4678-bfe1-31022d71c7d5.html" xr:uid="{282C3E22-7194-4034-B5F0-FDC1C3A592ED}"/>
+    <hyperlink ref="I4" r:id="rId44" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/77b391e3-2d5d-40c3-83bf-65c846b3c6a3.html" xr:uid="{CBAD478A-CFF1-4416-95E6-D597E751496A}"/>
+    <hyperlink ref="I5" r:id="rId45" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/0884adba-2312-4468-abeb-5422caed1038.html" xr:uid="{04EBABAF-FCD4-400B-865A-4629ACEE8A1C}"/>
+    <hyperlink ref="I62" r:id="rId46" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{84BA340D-A737-44A6-8243-CE38353F3505}"/>
+    <hyperlink ref="I59" r:id="rId47" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{284F4345-B5DC-417E-BC0C-C5D938B0B85E}"/>
+    <hyperlink ref="I60" r:id="rId48" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{7D374186-6F87-4F4B-BD1C-FF664D57FB3A}"/>
+    <hyperlink ref="I61" r:id="rId49" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{E2D95A4D-E4CA-478B-A2B1-A65EC02B99DF}"/>
+    <hyperlink ref="I56" r:id="rId50" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{51AA4039-6A88-49D1-8B12-DD32820D823E}"/>
+    <hyperlink ref="I57" r:id="rId51" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{065DDCB1-90A9-4EDD-8C92-5541BCE834DA}"/>
+    <hyperlink ref="I58" r:id="rId52" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{9EF972AC-F7F7-4674-9CCF-880CF2D66E95}"/>
+    <hyperlink ref="I64" r:id="rId53" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{931DDE7E-EDCD-452C-AD9D-64CA39733706}"/>
+    <hyperlink ref="I63" r:id="rId54" display="https://www.azadvertizer.net/azpolicyadvertizer/78460a36-508a-49a4-b2b2-2f5ec564f4bb.html" xr:uid="{395D3BF7-0DF4-4A65-AE8E-513FFAD36A0E}"/>
+    <hyperlink ref="I71" r:id="rId55" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/de01d381-bae9-4670-8870-786f89f49e26.html" xr:uid="{2BB42A42-9FE5-43D2-A4F4-291D3A119CED}"/>
+    <hyperlink ref="I68" r:id="rId56" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/92a36f05-ebc9-4bba-9128-b47ad2ea3354.html" xr:uid="{B7C3EF70-B4B5-41BB-B6B1-DD3E0613BADE}"/>
+    <hyperlink ref="I69" r:id="rId57" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/c4a70814-96be-461c-889f-2b27429120dc.html" xr:uid="{54066978-D3F9-4293-A399-6362596FA68D}"/>
+    <hyperlink ref="I70" r:id="rId58" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/53448c70-089b-4f52-8f38-89196d7f2de1.html" xr:uid="{44E5DFB7-2AB2-46AE-B5D5-7575A50E96BC}"/>
+    <hyperlink ref="I65" r:id="rId59" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/924bfe3a-762f-40e7-86dd-5c8b95eb09e6.html" xr:uid="{FE736BD0-ADD4-4D39-A67A-6885EA23C47A}"/>
+    <hyperlink ref="I66" r:id="rId60" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/f5bf694c-cca7-4033-b883-3a23327d5485.html" xr:uid="{0B5C4EB0-CA15-47CB-AEB7-9C34B93FBDAB}"/>
+    <hyperlink ref="I67" r:id="rId61" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/2b00397d-c309-49c4-aa5a-f0b2c5bc6321.html" xr:uid="{4A787895-3E1A-41AF-95EE-FF2ADB256422}"/>
+    <hyperlink ref="I72" r:id="rId62" display="https://www.azadvertizer.net/azpolicyinitiativesadvertizer/Deploy-AUM-CheckUpdates.html" xr:uid="{F20ADB34-F943-4C70-B074-C9F22D7BC15F}"/>
+    <hyperlink ref="I35" r:id="rId63" display="https://www.azadvertizer.net/azpolicyadvertizer/25da7dfb-0666-4a15-a8f5-402127efd8bb.html" xr:uid="{38CBF8C3-8CFC-47E0-9942-240DA0287CA0}"/>
+    <hyperlink ref="I46" r:id="rId64" display="https://www.azadvertizer.net/azpolicyadvertizer/98d0b9f8-fd90-49c9-88e2-d3baf3b0dd86.html" xr:uid="{C93DAC5F-2A0F-4915-AA1B-7CC1E650BB8D}"/>
+    <hyperlink ref="I19" r:id="rId65" display="https://www.azadvertizer.net/azpolicyadvertizer/7bca8353-aa3b-429b-904a-9229c4385837.html" xr:uid="{7166D0B8-5AFF-4B09-A435-5D5A160DC40B}"/>
+    <hyperlink ref="I47" r:id="rId66" display="https://www.azadvertizer.net/azpolicyadvertizer/7bca8353-aa3b-429b-904a-9229c4385837.html" xr:uid="{35261964-DE11-4D2A-A203-99D18A71AC16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId63"/>
+  <pageSetup orientation="portrait" r:id="rId67"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E503B61-35A4-4319-B932-EEE3DC552EA0}">
   <dimension ref="A1:K54"/>
   <sheetViews>
@@ -5481,7 +5813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9175C439-594F-4092-8051-A5B619C7BB77}">
   <dimension ref="A1:I35"/>
   <sheetViews>
@@ -6545,19 +6877,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6566,7 +6885,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001792584B535B9240A14A2E941038FA52" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8533dd5ab7486735195efbc21399c1d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="76c5ae4f-ecb0-448c-82d7-66022c31a977" xmlns:ns3="7c265764-6886-46a3-9c12-c296af1a4836" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e854eda2a58689c577d69670c76e567" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6832,19 +7151,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
-    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="76c5ae4f-ecb0-448c-82d7-66022c31a977">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7c265764-6886-46a3-9c12-c296af1a4836" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0FD48CAA-4BEA-4735-B3B6-DF2EAAF6E328}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -6852,7 +7172,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2E52F81-9253-48CD-8CFA-4E96C528D6ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6872,6 +7192,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4AD1D39-EA63-41E8-8401-20860C84E6BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76c5ae4f-ecb0-448c-82d7-66022c31a977"/>
+    <ds:schemaRef ds:uri="7c265764-6886-46a3-9c12-c296af1a4836"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Updating ALZ Excel for the last time, as this is moving to the ALZ Library
</commit_message>
<xml_diff>
--- a/docs/wiki/media/ALZ Policy Assignments v2.xlsx
+++ b/docs/wiki/media/ALZ Policy Assignments v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10118"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/springstone/repos/Springstone/Enterprise-Scale/docs/wiki/media/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/springstone/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:101_{325CDA05-F0B3-D448-ADCC-C2D3FB484848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6601C325-E8A7-FC49-A181-206B447BDAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="429">
   <si>
     <t>Assignment Scope (MG)</t>
   </si>
@@ -1304,6 +1304,21 @@
   </si>
   <si>
     <t>FY25H2</t>
+  </si>
+  <si>
+    <t>Microsoft Cloud Security Benchmark v2</t>
+  </si>
+  <si>
+    <t>[Preview]: Microsoft cloud security benchmark v2</t>
+  </si>
+  <si>
+    <t>DINE-ASB2PolicyAssignment.json</t>
+  </si>
+  <si>
+    <t>The Microsoft cloud security benchmark initiative represents the policies and controls implementing security recommendations defined in Microsoft cloud security benchmark, see https://aka.ms/azsecbm. This also serves as the Microsoft Defender for Cloud default policy initiative. You can directly assign this initiative, or manage its policies and compliance results within Microsoft Defender for Cloud.</t>
+  </si>
+  <si>
+    <t>https://www.azadvertizer.net/azpolicyinitiativesadvertizer/e3ec7e09-768c-4b64-882c-fcada3772047.html</t>
   </si>
 </sst>
 </file>
@@ -1929,11 +1944,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2148,15 +2163,15 @@
         <v>45018</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>123</v>
+        <v>424</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>123</v>
+        <v>425</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>11</v>
@@ -2165,30 +2180,30 @@
         <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>124</v>
+        <v>427</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>125</v>
+        <v>426</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>126</v>
+        <v>428</v>
       </c>
       <c r="J7" s="6">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>11</v>
@@ -2197,112 +2212,112 @@
         <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J8" s="6">
         <v>45018</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>33</v>
+        <v>130</v>
       </c>
       <c r="J9" s="6">
         <v>45018</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>131</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>132</v>
+        <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>133</v>
+        <v>32</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>134</v>
+        <v>33</v>
       </c>
       <c r="J10" s="6">
         <v>45018</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J11" s="6">
         <v>45018</v>
@@ -2313,74 +2328,74 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>218</v>
+        <v>135</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J12" s="6">
         <v>45018</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J13" s="6">
         <v>45018</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>11</v>
@@ -2389,158 +2404,158 @@
         <v>12</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J14" s="6">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" ht="176" x14ac:dyDescent="0.2">
+        <v>45018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J15" s="6">
-        <v>45266</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="I16" s="4"/>
+        <v>153</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="J16" s="6">
-        <v>45427</v>
-      </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="128" x14ac:dyDescent="0.2">
+        <v>45266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="6">
+        <v>45427</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" ht="128" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J18" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="J18" s="6">
-        <v>45124</v>
-      </c>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>11</v>
@@ -2549,60 +2564,60 @@
         <v>12</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="I19" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="J19" s="6">
-        <v>45363</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+        <v>45124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>220</v>
+        <v>164</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>221</v>
+        <v>69</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>223</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="I20" s="4"/>
       <c r="J20" s="6">
-        <v>45519</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>30</v>
@@ -2611,62 +2626,62 @@
         <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>38</v>
+        <v>220</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>39</v>
+        <v>221</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>40</v>
+        <v>222</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>41</v>
+        <v>223</v>
       </c>
       <c r="J21" s="6">
-        <v>45018</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="1" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>167</v>
+        <v>38</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>